<commit_message>
update OMV MODS xlsx for Kagwa (not done)
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/Desktop/OMV-dev-to-do/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0F50E-9D6E-0742-B236-A1A0AA0E8862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5AC1A3-3568-B544-BC74-999D31386436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="164">
   <si>
     <t>liv_000017</t>
   </si>
@@ -100,9 +100,6 @@
     <t>[East Africa]</t>
   </si>
   <si>
-    <t>Extract from David Livingstone's Field Diary XVII</t>
-  </si>
-  <si>
     <t>28 April 1873</t>
   </si>
   <si>
@@ -190,12 +187,6 @@
     <t>[Central Africa]</t>
   </si>
   <si>
-    <t>Narrative of Said Bin Habeeb, An Arab Inhabitant of Zanzibar</t>
-  </si>
-  <si>
-    <t>Narrative of Said Bin Habeeb, An Arab Inhabitant of Zanzibar, 31 May 1860</t>
-  </si>
-  <si>
     <t>[Said Bin Habeeb]</t>
   </si>
   <si>
@@ -211,12 +202,6 @@
     <t>31 May 1860</t>
   </si>
   <si>
-    <t>The Story of My Life</t>
-  </si>
-  <si>
-    <t>The Story of My Life, August 1891</t>
-  </si>
-  <si>
     <t>St. Nicholas: An Illustrated Magazine for Young Folks</t>
   </si>
   <si>
@@ -226,12 +211,6 @@
     <t>August 1891</t>
   </si>
   <si>
-    <t>Notes on African Geography</t>
-  </si>
-  <si>
-    <t>Notes on African Geography, 1845</t>
-  </si>
-  <si>
     <t>MacQueen, James, 1778-1870</t>
   </si>
   <si>
@@ -283,12 +262,6 @@
     <t>Brixton</t>
   </si>
   <si>
-    <t>To the Editor of the Times</t>
-  </si>
-  <si>
-    <t>To the Editor of the Times, 9 April 1874</t>
-  </si>
-  <si>
     <t>Waller, Horace, 1833-1896</t>
   </si>
   <si>
@@ -307,9 +280,6 @@
     <t>Jacob Wainwright</t>
   </si>
   <si>
-    <t>Jacob Wainwright, 1 September 1874</t>
-  </si>
-  <si>
     <t>[Wainwright, Jacob, c.1851/2-1892]</t>
   </si>
   <si>
@@ -334,9 +304,6 @@
     <t>4 May 1873</t>
   </si>
   <si>
-    <t>[Livingstone, David, 1813-1873]</t>
-  </si>
-  <si>
     <t>Allen and Co.</t>
   </si>
   <si>
@@ -484,9 +451,6 @@
     <t>location.physicalLocation, type="settlement"</t>
   </si>
   <si>
-    <t>Extract from David Livingstone's Field Diary XVII, 28 April 1873</t>
-  </si>
-  <si>
     <t>location.physicalLocation, type="repository"</t>
   </si>
   <si>
@@ -509,6 +473,57 @@
   </si>
   <si>
     <t>CWM/LMS, Incoming correspondence, 25/4/B</t>
+  </si>
+  <si>
+    <t>Addition to David Livingstone's Field Diary XVII</t>
+  </si>
+  <si>
+    <t>Addition to David Livingstone's Field Diary XVII, 28 April 1873</t>
+  </si>
+  <si>
+    <t>liv_020016</t>
+  </si>
+  <si>
+    <t>"Narrative of Said Bin Habeeb, An Arab Inhabitant of Zanzibar"</t>
+  </si>
+  <si>
+    <t>"The Story of My Life"</t>
+  </si>
+  <si>
+    <t>"Narrative of Said Bin Habeeb, An Arab Inhabitant of Zanzibar," 31 May 1860</t>
+  </si>
+  <si>
+    <t>"The Story of My Life," August 1891</t>
+  </si>
+  <si>
+    <t>"Notes on African Geography," 1845</t>
+  </si>
+  <si>
+    <t>"Notes on African Geography"</t>
+  </si>
+  <si>
+    <t>"To the Editor of the Times"</t>
+  </si>
+  <si>
+    <t>"To the Editor of the Times," 9 April 1874</t>
+  </si>
+  <si>
+    <t>"Jacob Wainwright," 1 September 1874</t>
+  </si>
+  <si>
+    <t>"Jacob Wainwright"</t>
+  </si>
+  <si>
+    <t>"The Katikiro of Uganda and His Secretary"</t>
+  </si>
+  <si>
+    <t>"The Katikiro of Uganda and His Secretary," 1906</t>
+  </si>
+  <si>
+    <t>Stone, Benjamin, 1838-1914</t>
+  </si>
+  <si>
+    <t>Kagwa, Apolo, 1864-1927</t>
   </si>
 </sst>
 </file>
@@ -538,7 +553,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,6 +569,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -598,6 +619,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,11 +937,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P17" sqref="P17:T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -938,64 +962,64 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="51">
@@ -1003,19 +1027,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1030,10 +1051,10 @@
         <v>360</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="34">
@@ -1047,10 +1068,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1079,13 +1100,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -1100,7 +1121,7 @@
         <v>833</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>21</v>
@@ -1111,16 +1132,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1135,10 +1156,10 @@
         <v>836</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="34">
@@ -1146,34 +1167,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="34">
@@ -1181,34 +1202,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="68">
@@ -1216,133 +1237,133 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="85">
+    </row>
+    <row r="9" spans="1:20" ht="68">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="Q9" s="1">
         <v>15</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" ht="119">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="68">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="1">
         <v>18</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="85">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="51">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>155</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>154</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="Q11" s="1">
         <v>15</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="T11" s="1">
         <v>1845</v>
@@ -1353,34 +1374,34 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="51">
@@ -1388,34 +1409,34 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="34">
@@ -1423,57 +1444,60 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="119">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="68">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="Q15" s="1">
         <v>93</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="85">
@@ -1481,35 +1505,60 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="34">
+      <c r="A17" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1542,81 +1591,81 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="Q1" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="102">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1625,94 +1674,94 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="M2" s="1">
         <v>1874</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="51">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="M3" s="1">
         <v>1874</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="51">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="51">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1721,33 +1770,33 @@
         <v>17</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="34">
       <c r="A6" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1756,51 +1805,51 @@
         <v>17</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="119">
       <c r="A7" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods worksheet for wellington
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5AC1A3-3568-B544-BC74-999D31386436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9375B492-93B5-7B44-848E-70967F279696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="167">
   <si>
     <t>liv_000017</t>
   </si>
@@ -524,6 +524,15 @@
   </si>
   <si>
     <t>Kagwa, Apolo, 1864-1927</t>
+  </si>
+  <si>
+    <t>liv_021008</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Livingstone Pictures/Box 1, file 8</t>
+  </si>
+  <si>
+    <t>University of London. School of Oriental and African Studies, London</t>
   </si>
 </sst>
 </file>
@@ -939,9 +948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P17" sqref="P17:T17"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1567,11 +1576,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1852,6 +1861,41 @@
         <v>143</v>
       </c>
     </row>
+    <row r="8" spans="1:20" ht="68">
+      <c r="A8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T7">
     <sortCondition ref="A2:A7"/>

</xml_diff>

<commit_message>
update MODS worksheet for Sechele
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9375B492-93B5-7B44-848E-70967F279696}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F91189-4E20-AB40-9BAA-FA40D1AB2CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
   <si>
     <t>liv_000017</t>
   </si>
@@ -529,10 +529,28 @@
     <t>liv_021008</t>
   </si>
   <si>
-    <t>CWM/LMS/Home/Livingstone Pictures/Box 1, file 8</t>
-  </si>
-  <si>
     <t>University of London. School of Oriental and African Studies, London</t>
+  </si>
+  <si>
+    <t>liv_021009</t>
+  </si>
+  <si>
+    <t>Sechele</t>
+  </si>
+  <si>
+    <t>Sechele, [Second half of nineteenth century]</t>
+  </si>
+  <si>
+    <t>[Second half of nineteenth century]</t>
+  </si>
+  <si>
+    <t>[Southern Africa]</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Livingstone Pictures/Box 1/File 8</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Africa Pictures/10</t>
   </si>
 </sst>
 </file>
@@ -1576,11 +1594,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1884,16 +1902,51 @@
         <v>67</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="51">
+      <c r="A9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MODS worksheet for Ncwadi
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2731CB35-36C1-4F40-BA48-4112B5E44BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A853361-7726-A240-A902-9BE6CC557F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="188">
   <si>
     <t>liv_000017</t>
   </si>
@@ -274,9 +274,6 @@
     <t>The Times</t>
   </si>
   <si>
-    <t>10 April 1874</t>
-  </si>
-  <si>
     <t>Jacob Wainwright</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>Abdullah Susi [Mislabeled Jacob Wainwright], [c.1874]</t>
   </si>
   <si>
-    <t>Anon.</t>
-  </si>
-  <si>
     <t>David Livingstone Centre</t>
   </si>
   <si>
@@ -572,6 +566,36 @@
   </si>
   <si>
     <t>St. John's, Leytonstone</t>
+  </si>
+  <si>
+    <t>The Illustrated Missionary News</t>
+  </si>
+  <si>
+    <t>originInfo, type="issue"</t>
+  </si>
+  <si>
+    <t>81, 93</t>
+  </si>
+  <si>
+    <t>1 June 1894; 12 June 1893</t>
+  </si>
+  <si>
+    <t>10 April 1874; [1874]; [1874]</t>
+  </si>
+  <si>
+    <t>Anonymous</t>
+  </si>
+  <si>
+    <t>Ncwadi</t>
+  </si>
+  <si>
+    <t>liv_020015</t>
+  </si>
+  <si>
+    <t>“Gleanings and Glances” (Excerpt); “Letter from an African Chief”</t>
+  </si>
+  <si>
+    <t>“Gleanings and Glances” (Excerpt); “Letter from an African Chief,” 1 June 1894, 12 June 1893</t>
   </si>
 </sst>
 </file>
@@ -979,11 +1003,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1004,64 +1028,64 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="51">
@@ -1069,16 +1093,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1113,7 +1137,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1148,7 +1172,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -1183,7 +1207,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1218,7 +1242,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1253,7 +1277,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1291,7 +1315,7 @@
         <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>45</v>
@@ -1317,10 +1341,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>52</v>
@@ -1329,7 +1353,7 @@
         <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>53</v>
@@ -1349,10 +1373,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
@@ -1361,7 +1385,7 @@
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>56</v>
@@ -1381,10 +1405,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1396,7 +1420,7 @@
         <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>62</v>
@@ -1425,7 +1449,7 @@
         <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
@@ -1437,7 +1461,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>69</v>
@@ -1460,7 +1484,7 @@
         <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
@@ -1472,7 +1496,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>74</v>
@@ -1486,10 +1510,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>76</v>
@@ -1501,7 +1525,7 @@
         <v>78</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>79</v>
@@ -1510,7 +1534,7 @@
         <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>80</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="68">
@@ -1518,28 +1542,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="Q15" s="1">
         <v>93</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="85">
@@ -1547,16 +1571,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
@@ -1565,13 +1589,13 @@
         <v>67</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>23</v>
@@ -1579,25 +1603,25 @@
     </row>
     <row r="17" spans="1:20" ht="85">
       <c r="A17" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
@@ -1606,6 +1630,41 @@
       </c>
       <c r="T17" s="5">
         <v>1906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="85">
+      <c r="A18" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>28</v>
+      </c>
+      <c r="R18" s="1">
+        <v>6</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1617,9 +1676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1639,81 +1698,81 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="102">
       <c r="A2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1722,33 +1781,33 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M2" s="1">
         <v>1874</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="51">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1757,59 +1816,59 @@
         <v>67</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M3" s="1">
         <v>1874</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="51">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="51">
       <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1818,33 +1877,33 @@
         <v>17</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="34">
       <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1853,33 +1912,33 @@
         <v>17</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="119">
       <c r="A7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1888,33 +1947,33 @@
         <v>67</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="68">
       <c r="A8" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>16</v>
@@ -1923,33 +1982,33 @@
         <v>67</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="51">
       <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
@@ -1958,33 +2017,33 @@
         <v>67</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="102">
       <c r="A10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>99</v>
+        <v>183</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>16</v>
@@ -1993,16 +2052,16 @@
         <v>67</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MODS for new artifacts
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257CCC1-9278-F24E-9D42-516D57031862}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35305D7-ED72-9D4E-ADD1-D800215B3BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="270">
   <si>
     <t>liv_000017</t>
   </si>
@@ -424,18 +424,9 @@
     <t>location.physicalLocation</t>
   </si>
   <si>
-    <t>[publications]</t>
-  </si>
-  <si>
-    <t>originInfo [title]</t>
-  </si>
-  <si>
     <t>originInfo, type="volume"</t>
   </si>
   <si>
-    <t>originInfo, type="info"</t>
-  </si>
-  <si>
     <t>originInfo, type="pages"</t>
   </si>
   <si>
@@ -620,13 +611,244 @@
   </si>
   <si>
     <t>Limaoe (on the Kolobeng)</t>
+  </si>
+  <si>
+    <t>liv_021011</t>
+  </si>
+  <si>
+    <t>liv_021012</t>
+  </si>
+  <si>
+    <t>liv_021013</t>
+  </si>
+  <si>
+    <t>liv_021014</t>
+  </si>
+  <si>
+    <t>liv_021015</t>
+  </si>
+  <si>
+    <t>liv_021016</t>
+  </si>
+  <si>
+    <t>liv_021017</t>
+  </si>
+  <si>
+    <t>liv_021018</t>
+  </si>
+  <si>
+    <t>“Apolo Kagwa, Katikiro of Uganda, and His Son”; “Ham Mukasa, with Father, Wife, and Children”</t>
+  </si>
+  <si>
+    <t>Mukasa, Ham, c.1870-1956</t>
+  </si>
+  <si>
+    <t>The Wonderful Story of Uganda; The Story of Ham Mukasa</t>
+  </si>
+  <si>
+    <t>opposite 98, opposite 173</t>
+  </si>
+  <si>
+    <t>originInfo, type="place"</t>
+  </si>
+  <si>
+    <t>originInfo, type="publisher"</t>
+  </si>
+  <si>
+    <t>Church Missionary Society</t>
+  </si>
+  <si>
+    <t>Mullins, J.D.</t>
+  </si>
+  <si>
+    <t>Edward Wilmot Blyden</t>
+  </si>
+  <si>
+    <t>Blyden, Edward Wilmot, 1832-1912</t>
+  </si>
+  <si>
+    <t>The Aims and Methods of a Liberal Education for Africans</t>
+  </si>
+  <si>
+    <t>Cambridge, MA</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>John Wilson and Son</t>
+  </si>
+  <si>
+    <t>George Young</t>
+  </si>
+  <si>
+    <t>frontispiece</t>
+  </si>
+  <si>
+    <t>Sarojini Naidu</t>
+  </si>
+  <si>
+    <t>Naidu, Sarojini, 1879-1949</t>
+  </si>
+  <si>
+    <t>The Bird of Time</t>
+  </si>
+  <si>
+    <t>William Heineman</t>
+  </si>
+  <si>
+    <t>John Lane Company</t>
+  </si>
+  <si>
+    <t>Swami Vivekanada</t>
+  </si>
+  <si>
+    <t>Swami Vivekanada, [c.1893]</t>
+  </si>
+  <si>
+    <t>Vivekanada, Swami, 1863-1902</t>
+  </si>
+  <si>
+    <t>Inspired Talks</t>
+  </si>
+  <si>
+    <t>Madras</t>
+  </si>
+  <si>
+    <t>The Ramakrishna Mission</t>
+  </si>
+  <si>
+    <t>Cornelia Sorabji</t>
+  </si>
+  <si>
+    <t>Sorabji, Cornelia, 1866-1954</t>
+  </si>
+  <si>
+    <t>Love and Life Behind the Purdah</t>
+  </si>
+  <si>
+    <t>Freemantle &amp; Co.</t>
+  </si>
+  <si>
+    <t>Hutchinson &amp; Co.</t>
+  </si>
+  <si>
+    <t>Uganda’s Katikiro in England</t>
+  </si>
+  <si>
+    <t>Ham Mukasa and Apolo Kagwa</t>
+  </si>
+  <si>
+    <t>Bassano, Alexander, 1829-1913</t>
+  </si>
+  <si>
+    <t>McKay, Claude, 1889-1948</t>
+  </si>
+  <si>
+    <t>Songs from Jamaica</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>Aston W. Gardner</t>
+  </si>
+  <si>
+    <t>Jamaica Agency</t>
+  </si>
+  <si>
+    <t>frontispieces, title page</t>
+  </si>
+  <si>
+    <t>Inscribed Frontispiece and Title Page</t>
+  </si>
+  <si>
+    <t>Inscribed Page; Solomon T. Plaatje, Inscribed; Elizabeth Lilith M'belle ("Mrs. S.T. Plaatje")</t>
+  </si>
+  <si>
+    <t>Inscribed Page; Solomon T. Plaatje, Inscribed; Elizabeth Lilith M'belle ("Mrs. S.T. Plaatje"); 16 November 1921, [early twentieth century], [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Plaatje, Solomon T., 1876-1932</t>
+  </si>
+  <si>
+    <t>Wakefield, ?</t>
+  </si>
+  <si>
+    <t>Taylor, D.</t>
+  </si>
+  <si>
+    <t>Native Life in South Africa</t>
+  </si>
+  <si>
+    <t>Kimberley</t>
+  </si>
+  <si>
+    <t>Tsala Ea Batho</t>
+  </si>
+  <si>
+    <t>The Crisis</t>
+  </si>
+  <si>
+    <t>[1920?]</t>
+  </si>
+  <si>
+    <t>n.pag.</t>
+  </si>
+  <si>
+    <t>[periodicals/artifacts]</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New York </t>
+  </si>
+  <si>
+    <t>Melbourne</t>
+  </si>
+  <si>
+    <t>Cassell and Company, Limited</t>
+  </si>
+  <si>
+    <t>[books/artifacts]</t>
+  </si>
+  <si>
+    <t>“Apolo Kagwa, Katikiro of Uganda, and His Son”; “Ham Mukasa, with Father, Wife, and Children”; [Early twentieth century], [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Edward Wilmot Blyden, [Late nineteenth or early twentieth century]</t>
+  </si>
+  <si>
+    <t>Sarojini Naidu, [Early twentieth century]</t>
+  </si>
+  <si>
+    <t>Cornelia Sorabji, [Late nineteenth or early twentieth century]</t>
+  </si>
+  <si>
+    <t>Ham Mukasa and Apolo Kagwa, [Early twentieth century]</t>
+  </si>
+  <si>
+    <t>Inscribed Frontispiece and Title Page, [Early twentieth century]</t>
+  </si>
+  <si>
+    <t>Barnett, Henry Walter, 1862-1934</t>
+  </si>
+  <si>
+    <t>[books/periodicals]</t>
+  </si>
+  <si>
+    <t>originInfo, type="book"</t>
+  </si>
+  <si>
+    <t>originInfo, type="author"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -644,6 +866,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -696,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -711,6 +940,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1027,11 +1260,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1044,13 +1277,15 @@
     <col min="8" max="8" width="12.83203125" style="3" customWidth="1"/>
     <col min="9" max="11" width="21.83203125" style="1" customWidth="1"/>
     <col min="12" max="14" width="20.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="3" customWidth="1"/>
     <col min="16" max="19" width="15.83203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="20.83203125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="12.83203125" style="3" customWidth="1"/>
+    <col min="22" max="32" width="15.83203125" style="5" customWidth="1"/>
+    <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
+    <row r="1" spans="1:32" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -1076,13 +1311,13 @@
         <v>128</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>127</v>
@@ -1094,33 +1329,69 @@
         <v>126</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="51">
+      <c r="U1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="51">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
@@ -1147,7 +1418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="34">
+    <row r="3" spans="1:32" ht="34">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1182,7 +1453,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="51">
+    <row r="4" spans="1:32" ht="51">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1217,7 +1488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="51">
+    <row r="5" spans="1:32" ht="51">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="34">
+    <row r="6" spans="1:32" ht="34">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1287,7 +1558,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="34">
+    <row r="7" spans="1:32" ht="34">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1322,7 +1593,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="68">
+    <row r="8" spans="1:32" ht="68">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1360,15 +1631,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="68">
+    <row r="9" spans="1:32" ht="68">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>52</v>
@@ -1392,15 +1663,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="68">
+    <row r="10" spans="1:32" ht="68">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
@@ -1424,15 +1695,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="51">
+    <row r="11" spans="1:32" ht="51">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1459,7 +1730,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="68">
+    <row r="12" spans="1:32" ht="68">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1485,7 +1756,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>69</v>
@@ -1494,7 +1765,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="68">
+    <row r="13" spans="1:32" ht="68">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1520,7 +1791,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>74</v>
@@ -1529,15 +1800,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="34">
+    <row r="14" spans="1:32" ht="34">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>76</v>
@@ -1558,18 +1829,18 @@
         <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="68">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="68">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>81</v>
@@ -1590,7 +1861,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="85">
+    <row r="16" spans="1:32" ht="85">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1616,7 +1887,7 @@
         <v>87</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>88</v>
@@ -1625,58 +1896,78 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="85">
+    <row r="17" spans="1:32" ht="85">
       <c r="A17" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="P17" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="5">
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="V17" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB17" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="AC17" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="AE17" s="5">
+        <v>1906</v>
+      </c>
+      <c r="AF17" s="5">
         <v>74</v>
       </c>
-      <c r="T17" s="5">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="85">
+    </row>
+    <row r="18" spans="1:32" ht="85">
       <c r="A18" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>122</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q18" s="1">
         <v>28</v>
@@ -1685,27 +1976,27 @@
         <v>6</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="51">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="51">
       <c r="A19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>121</v>
@@ -1720,13 +2011,13 @@
         <v>68</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="N19" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1736,11 +2027,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1750,15 +2041,19 @@
     <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
     <col min="4" max="6" width="20.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" style="3" customWidth="1"/>
-    <col min="9" max="11" width="20.83203125" style="1" customWidth="1"/>
-    <col min="12" max="14" width="15.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" style="3" customWidth="1"/>
-    <col min="16" max="20" width="15.83203125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="15" style="6" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="3" customWidth="1"/>
+    <col min="10" max="12" width="20.83203125" style="1" customWidth="1"/>
+    <col min="13" max="15" width="15.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="16.5" style="5" customWidth="1"/>
+    <col min="19" max="25" width="15.83203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.83203125" style="3" customWidth="1"/>
+    <col min="27" max="31" width="15.83203125" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="34">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -1781,46 +2076,76 @@
         <v>124</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="102">
+    </row>
+    <row r="2" spans="1:30" ht="102">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -1836,26 +2161,26 @@
       <c r="G2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1874</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="51">
+    <row r="3" spans="1:30" ht="51">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -1871,23 +2196,23 @@
       <c r="G3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="L3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="1">
         <v>1874</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="51">
+      <c r="O3" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="51">
       <c r="A4" s="1" t="s">
         <v>109</v>
       </c>
@@ -1903,20 +2228,20 @@
       <c r="G4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="51">
+      <c r="O4" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="51">
       <c r="A5" s="1" t="s">
         <v>95</v>
       </c>
@@ -1927,31 +2252,31 @@
         <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="34">
+      <c r="O5" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="34">
       <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
@@ -1962,31 +2287,31 @@
         <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="119">
+      <c r="O6" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="119">
       <c r="A7" s="1" t="s">
         <v>92</v>
       </c>
@@ -2002,28 +2327,28 @@
       <c r="G7" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="68">
+      <c r="O7" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="68">
       <c r="A8" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>100</v>
@@ -2032,102 +2357,439 @@
         <v>101</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="51">
+      <c r="A9" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" ht="51">
-      <c r="A9" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>165</v>
       </c>
       <c r="N9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="102">
+      <c r="A10" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="102">
-      <c r="A10" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>175</v>
+    </row>
+    <row r="11" spans="1:30" ht="136">
+      <c r="A11" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1904</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="68">
+      <c r="A12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1920</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="34">
+      <c r="A13" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="X13" s="1">
+        <v>1912</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="51">
+      <c r="A14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="X14" s="1">
+        <v>1901</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="51">
+      <c r="A15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="X15" s="1">
+        <v>1901</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="51">
+      <c r="A16" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="X16" s="1">
+        <v>1904</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="51">
+      <c r="A17" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="X17" s="1">
+        <v>1912</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="136">
+      <c r="A18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T7">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE7">
     <sortCondition ref="A2:A7"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update MODS worksheet for naidu title
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35305D7-ED72-9D4E-ADD1-D800215B3BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4A1833-2925-D14C-A4E4-B358B5F3CCA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -685,9 +685,6 @@
     <t>frontispiece</t>
   </si>
   <si>
-    <t>Sarojini Naidu</t>
-  </si>
-  <si>
     <t>Naidu, Sarojini, 1879-1949</t>
   </si>
   <si>
@@ -820,9 +817,6 @@
     <t>Edward Wilmot Blyden, [Late nineteenth or early twentieth century]</t>
   </si>
   <si>
-    <t>Sarojini Naidu, [Early twentieth century]</t>
-  </si>
-  <si>
     <t>Cornelia Sorabji, [Late nineteenth or early twentieth century]</t>
   </si>
   <si>
@@ -842,6 +836,12 @@
   </si>
   <si>
     <t>originInfo, type="author"</t>
+  </si>
+  <si>
+    <t>Sarojini Naidu (with Facsimile Signature)</t>
+  </si>
+  <si>
+    <t>Sarojini Naidu (with Facsimile Signature), [Early twentieth century]</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AF19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
     </sheetView>
@@ -1329,7 +1329,7 @@
         <v>126</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>135</v>
@@ -1347,16 +1347,16 @@
         <v>125</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>205</v>
@@ -1929,16 +1929,16 @@
         <v>67</v>
       </c>
       <c r="Z17" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA17" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AB17" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="AB17" s="5" t="s">
+      <c r="AC17" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="AC17" s="5" t="s">
-        <v>258</v>
       </c>
       <c r="AE17" s="5">
         <v>1906</v>
@@ -2029,9 +2029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2100,16 +2100,16 @@
         <v>126</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>205</v>
@@ -2130,7 +2130,7 @@
         <v>131</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>135</v>
@@ -2459,7 +2459,7 @@
         <v>201</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>178</v>
@@ -2500,7 +2500,7 @@
         <v>209</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>178</v>
@@ -2536,15 +2536,15 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="34">
+    <row r="13" spans="1:30" ht="68">
       <c r="A13" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>178</v>
@@ -2556,10 +2556,10 @@
         <v>122</v>
       </c>
       <c r="Q13" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="S13" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>67</v>
@@ -2568,10 +2568,10 @@
         <v>213</v>
       </c>
       <c r="V13" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="W13" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="X13" s="1">
         <v>1912</v>
@@ -2585,10 +2585,10 @@
         <v>196</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>178</v>
@@ -2600,16 +2600,16 @@
         <v>122</v>
       </c>
       <c r="Q14" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="S14" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="T14" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="X14" s="1">
         <v>1901</v>
@@ -2623,13 +2623,13 @@
         <v>197</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>123</v>
@@ -2638,16 +2638,16 @@
         <v>122</v>
       </c>
       <c r="Q15" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="X15" s="1">
         <v>1901</v>
@@ -2661,13 +2661,13 @@
         <v>198</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>123</v>
@@ -2679,13 +2679,13 @@
         <v>202</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X16" s="1">
         <v>1904</v>
@@ -2699,13 +2699,13 @@
         <v>199</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>123</v>
@@ -2714,28 +2714,28 @@
         <v>122</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V17" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="W17" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="X17" s="1">
         <v>1912</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="136">
@@ -2743,19 +2743,19 @@
         <v>200</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>123</v>
@@ -2764,28 +2764,28 @@
         <v>122</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="S18" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>213</v>
       </c>
       <c r="V18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods metadata for sorabji
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBAF344-B613-E444-A24E-D38493E54A82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E744064-3915-2B48-89DB-878AED002A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -709,9 +709,6 @@
     <t>The Ramakrishna Mission</t>
   </si>
   <si>
-    <t>Cornelia Sorabji</t>
-  </si>
-  <si>
     <t>Sorabji, Cornelia, 1866-1954</t>
   </si>
   <si>
@@ -835,13 +832,16 @@
     <t>Sarojini Naidu (with Facsimile Signature), [early twentieth century]</t>
   </si>
   <si>
-    <t>Cornelia Sorabji, [late nineteenth or early twentieth century]</t>
-  </si>
-  <si>
     <t>Ham Mukasa and Apolo Kagwa, [early twentieth century]</t>
   </si>
   <si>
     <t>Inscribed Frontispiece and Title Page, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Cornelia Sorabji (with Superimposed Facsimile Signature)</t>
+  </si>
+  <si>
+    <t>Cornelia Sorabji (with Superimposed Facsimile Signature), [late nineteenth or early twentieth century]</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1329,7 @@
         <v>126</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>135</v>
@@ -1347,16 +1347,16 @@
         <v>125</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>203</v>
@@ -1929,16 +1929,16 @@
         <v>67</v>
       </c>
       <c r="Z17" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA17" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AB17" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="AB17" s="5" t="s">
+      <c r="AC17" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="AC17" s="5" t="s">
-        <v>255</v>
       </c>
       <c r="AE17" s="5">
         <v>1906</v>
@@ -2031,7 +2031,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2100,16 +2100,16 @@
         <v>126</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>203</v>
@@ -2130,7 +2130,7 @@
         <v>131</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>135</v>
@@ -2389,7 +2389,7 @@
         <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>176</v>
@@ -2424,7 +2424,7 @@
         <v>166</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>176</v>
@@ -2459,7 +2459,7 @@
         <v>199</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>176</v>
@@ -2500,7 +2500,7 @@
         <v>207</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>176</v>
@@ -2541,10 +2541,10 @@
         <v>193</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>176</v>
@@ -2618,18 +2618,18 @@
         <v>214</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="51">
+    <row r="15" spans="1:30" ht="85">
       <c r="A15" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>225</v>
+        <v>268</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>123</v>
@@ -2638,16 +2638,16 @@
         <v>122</v>
       </c>
       <c r="Q15" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="S15" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="X15" s="1">
         <v>1901</v>
@@ -2661,13 +2661,13 @@
         <v>196</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>123</v>
@@ -2679,13 +2679,13 @@
         <v>200</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="X16" s="1">
         <v>1904</v>
@@ -2699,13 +2699,13 @@
         <v>197</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>123</v>
@@ -2714,28 +2714,28 @@
         <v>122</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="S17" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="T17" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V17" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="W17" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="X17" s="1">
         <v>1912</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="136">
@@ -2743,19 +2743,19 @@
         <v>198</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>123</v>
@@ -2764,28 +2764,28 @@
         <v>122</v>
       </c>
       <c r="Q18" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="S18" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>211</v>
       </c>
       <c r="V18" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2794,5 +2794,6 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update mods for plaatje/mckay
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E744064-3915-2B48-89DB-878AED002A4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375638F9-3C11-5640-823E-E48771710EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -748,15 +748,6 @@
     <t>frontispieces, title page</t>
   </si>
   <si>
-    <t>Inscribed Frontispiece and Title Page</t>
-  </si>
-  <si>
-    <t>Inscribed Page; Solomon T. Plaatje, Inscribed; Elizabeth Lilith M'belle ("Mrs. S.T. Plaatje")</t>
-  </si>
-  <si>
-    <t>Inscribed Page; Solomon T. Plaatje, Inscribed; Elizabeth Lilith M'belle ("Mrs. S.T. Plaatje"); 16 November 1921, [early twentieth century], [early twentieth century]</t>
-  </si>
-  <si>
     <t>Plaatje, Solomon T., 1876-1932</t>
   </si>
   <si>
@@ -772,9 +763,6 @@
     <t>Kimberley</t>
   </si>
   <si>
-    <t>Tsala Ea Batho</t>
-  </si>
-  <si>
     <t>The Crisis</t>
   </si>
   <si>
@@ -835,13 +823,25 @@
     <t>Ham Mukasa and Apolo Kagwa, [early twentieth century]</t>
   </si>
   <si>
-    <t>Inscribed Frontispiece and Title Page, [early twentieth century]</t>
-  </si>
-  <si>
     <t>Cornelia Sorabji (with Superimposed Facsimile Signature)</t>
   </si>
   <si>
     <t>Cornelia Sorabji (with Superimposed Facsimile Signature), [late nineteenth or early twentieth century]</t>
+  </si>
+  <si>
+    <t>Page Inscribed to Kelly Miller; Solomon T. Plaatje, Signed; Elizabeth Lilith M’belle (“Mrs. S.T. Plaatje”)</t>
+  </si>
+  <si>
+    <t>Page Inscribed to Kelly Miller; Solomon T. Plaatje, Signed; Elizabeth Lilith M’belle (“Mrs. S.T. Plaatje”); 16 November 1921, [early twentieth century], [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Frontispiece Inscribed to Arthur Schomburg and Title Page</t>
+  </si>
+  <si>
+    <t>Frontispiece Inscribed to Arthur Schomburg and Title Page, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Tsala ea Batho</t>
   </si>
 </sst>
 </file>
@@ -1329,7 +1329,7 @@
         <v>126</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>135</v>
@@ -1347,16 +1347,16 @@
         <v>125</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="W1" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>203</v>
@@ -1929,16 +1929,16 @@
         <v>67</v>
       </c>
       <c r="Z17" s="5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="AB17" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="AC17" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="AE17" s="5">
         <v>1906</v>
@@ -2029,9 +2029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2100,16 +2100,16 @@
         <v>126</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>203</v>
@@ -2130,7 +2130,7 @@
         <v>131</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AA1" s="2" t="s">
         <v>135</v>
@@ -2389,7 +2389,7 @@
         <v>160</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>176</v>
@@ -2424,7 +2424,7 @@
         <v>166</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>176</v>
@@ -2459,7 +2459,7 @@
         <v>199</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>176</v>
@@ -2500,7 +2500,7 @@
         <v>207</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>176</v>
@@ -2541,10 +2541,10 @@
         <v>193</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>176</v>
@@ -2623,13 +2623,13 @@
         <v>195</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>123</v>
@@ -2664,7 +2664,7 @@
         <v>230</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>231</v>
@@ -2694,15 +2694,15 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="51">
+    <row r="17" spans="1:25" ht="68">
       <c r="A17" s="1" t="s">
         <v>197</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>232</v>
@@ -2738,24 +2738,24 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="136">
+    <row r="18" spans="1:25" ht="153">
       <c r="A18" s="1" t="s">
         <v>198</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>123</v>
@@ -2764,28 +2764,28 @@
         <v>122</v>
       </c>
       <c r="Q18" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="S18" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="T18" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>211</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MODS for selim aga
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375638F9-3C11-5640-823E-E48771710EB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE95C59-FCD0-0E48-83E1-32C6A4F6B6D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="276">
   <si>
     <t>liv_000017</t>
   </si>
@@ -842,6 +842,24 @@
   </si>
   <si>
     <t>Tsala ea Batho</t>
+  </si>
+  <si>
+    <t>liv_020017</t>
+  </si>
+  <si>
+    <t>The Niger Expedtion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Niger Expedition, 25 September 1858, 24 June 1858 </t>
+  </si>
+  <si>
+    <t>Aga, Selim, c.1828-1875</t>
+  </si>
+  <si>
+    <t>The Preston Chronicle and Lancashire Advertiser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 September 1858, 24 June 1858 </t>
   </si>
 </sst>
 </file>
@@ -1260,11 +1278,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF19"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2020,6 +2038,35 @@
         <v>190</v>
       </c>
     </row>
+    <row r="20" spans="1:32" ht="68">
+      <c r="A20" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S20" s="1">
+        <v>3</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2029,8 +2076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update mods for susi title
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE862C1C-7F00-EB44-AEA2-BA4F88194295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635ADFB-54B4-E845-AB47-F7182EE5EC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -322,12 +322,6 @@
     <t>liv_021005</t>
   </si>
   <si>
-    <t>Abdullah Susi [Mislabeled Jacob Wainwright]</t>
-  </si>
-  <si>
-    <t>Abdullah Susi [Mislabeled Jacob Wainwright], [c.1874]</t>
-  </si>
-  <si>
     <t>David Livingstone Centre</t>
   </si>
   <si>
@@ -860,6 +854,12 @@
   </si>
   <si>
     <t>Aga, Selim, c.1826-1875</t>
+  </si>
+  <si>
+    <t>Abdullah Susi (Mislabeled Jacob Wainwright), [c.1874]</t>
+  </si>
+  <si>
+    <t>Abdullah Susi (Mislabeled Jacob Wainwright)</t>
   </si>
 </sst>
 </file>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1305,100 +1305,100 @@
   <sheetData>
     <row r="1" spans="1:32" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="R1" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="51">
@@ -1406,16 +1406,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -1450,7 +1450,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -1485,7 +1485,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -1520,7 +1520,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -1555,7 +1555,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -1590,7 +1590,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1628,7 +1628,7 @@
         <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>45</v>
@@ -1654,10 +1654,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>52</v>
@@ -1666,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>53</v>
@@ -1686,10 +1686,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
@@ -1698,7 +1698,7 @@
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>56</v>
@@ -1718,10 +1718,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>59</v>
@@ -1733,7 +1733,7 @@
         <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>62</v>
@@ -1762,7 +1762,7 @@
         <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
@@ -1774,7 +1774,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>69</v>
@@ -1797,7 +1797,7 @@
         <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
@@ -1809,7 +1809,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>74</v>
@@ -1823,10 +1823,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>76</v>
@@ -1838,7 +1838,7 @@
         <v>78</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>79</v>
@@ -1847,7 +1847,7 @@
         <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="68">
@@ -1855,16 +1855,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>82</v>
@@ -1893,7 +1893,7 @@
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
@@ -1905,7 +1905,7 @@
         <v>87</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>88</v>
@@ -1916,47 +1916,47 @@
     </row>
     <row r="17" spans="1:32" ht="85">
       <c r="A17" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
       <c r="V17" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="X17" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y17" s="5" t="s">
         <v>67</v>
       </c>
       <c r="Z17" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA17" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB17" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AC17" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="AB17" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="AC17" s="5" t="s">
-        <v>250</v>
       </c>
       <c r="AE17" s="5">
         <v>1906</v>
@@ -1967,25 +1967,25 @@
     </row>
     <row r="18" spans="1:32" ht="85">
       <c r="A18" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="Q18" s="1">
         <v>28</v>
@@ -1994,30 +1994,30 @@
         <v>6</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="51">
       <c r="A19" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>16</v>
@@ -2029,42 +2029,42 @@
         <v>68</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="68">
       <c r="A20" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="S20" s="1">
         <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2076,9 +2076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2102,111 +2102,111 @@
   <sheetData>
     <row r="1" spans="1:30" s="2" customFormat="1" ht="34">
       <c r="A1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="102">
       <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>16</v>
@@ -2215,33 +2215,33 @@
         <v>17</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="N2" s="1">
         <v>1874</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="51">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>16</v>
@@ -2250,42 +2250,42 @@
         <v>67</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="N3" s="1">
         <v>1874</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="51">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="51">
@@ -2293,16 +2293,16 @@
         <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>275</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>274</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>16</v>
@@ -2311,33 +2311,33 @@
         <v>17</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>94</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="34">
       <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>16</v>
@@ -2346,16 +2346,16 @@
         <v>17</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="119">
@@ -2372,7 +2372,7 @@
         <v>89</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>16</v>
@@ -2390,24 +2390,24 @@
         <v>94</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="68">
       <c r="A8" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>16</v>
@@ -2416,33 +2416,33 @@
         <v>67</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="51">
       <c r="A9" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>16</v>
@@ -2451,33 +2451,33 @@
         <v>67</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="102">
       <c r="A10" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>16</v>
@@ -2486,353 +2486,353 @@
         <v>67</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M10" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="136">
       <c r="A11" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="X11" s="1">
         <v>1904</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="68">
       <c r="A12" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q12" s="5" t="s">
+      <c r="T12" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="X12" s="1">
         <v>1920</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="68">
       <c r="A13" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q13" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>67</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="X13" s="1">
         <v>1912</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="51">
       <c r="A14" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q14" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q14" s="5" t="s">
+      <c r="T14" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="V14" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="X14" s="1">
         <v>1901</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="85">
       <c r="A15" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q15" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="X15" s="1">
         <v>1901</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="51">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="Q16" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="X16" s="1">
         <v>1904</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="68">
       <c r="A17" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="T17" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>67</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="X17" s="1">
         <v>1912</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="153">
       <c r="A18" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="S18" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q18" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="S18" s="1" t="s">
+      <c r="U18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="U18" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="W18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for soga
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635ADFB-54B4-E845-AB47-F7182EE5EC87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286191D1-C60A-BB4B-BC5A-CB3654134C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="282">
   <si>
     <t>liv_000017</t>
   </si>
@@ -860,6 +860,24 @@
   </si>
   <si>
     <t>Abdullah Susi (Mislabeled Jacob Wainwright)</t>
+  </si>
+  <si>
+    <t>liv_020022</t>
+  </si>
+  <si>
+    <t>Jubilee of the Venerable Patriarch Brownlee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jubilee of the Venerable Patriarch Brownlee, 14 February 1867, 17 January 1867 </t>
+  </si>
+  <si>
+    <t>Soga, Tiyo, c.1831-1871</t>
+  </si>
+  <si>
+    <t>Kaffrarian Watchman</t>
+  </si>
+  <si>
+    <t>14 February 1867</t>
   </si>
 </sst>
 </file>
@@ -1278,11 +1296,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF20"/>
+  <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2067,7 +2085,40 @@
         <v>272</v>
       </c>
     </row>
+    <row r="21" spans="1:32" ht="68">
+      <c r="A21" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>82</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2076,8 +2127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update mods for khama
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286191D1-C60A-BB4B-BC5A-CB3654134C4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23EACD3-F63C-8444-B6FF-A1DC85286936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="289">
   <si>
     <t>liv_000017</t>
   </si>
@@ -878,6 +878,27 @@
   </si>
   <si>
     <t>14 February 1867</t>
+  </si>
+  <si>
+    <t>liv_020024</t>
+  </si>
+  <si>
+    <t>Letter to A.M. Chirgwin</t>
+  </si>
+  <si>
+    <t>Letter to A.M. Chirgwin, 5 December 1934</t>
+  </si>
+  <si>
+    <t>Khama, Semane Setlhoko, 1881-1937</t>
+  </si>
+  <si>
+    <t>CWM/LMS/South Africa/Incoming Correspondence/Box 97/Semane</t>
+  </si>
+  <si>
+    <t>5 December 1934</t>
+  </si>
+  <si>
+    <t>Serowe, Palapye Road, Bechuanaland Protectorate</t>
   </si>
 </sst>
 </file>
@@ -961,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -980,6 +1001,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1296,11 +1320,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2115,6 +2139,41 @@
       </c>
       <c r="T21" s="1" t="s">
         <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" ht="68">
+      <c r="A22" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for nosutu item
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23EACD3-F63C-8444-B6FF-A1DC85286936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011AD811-EBD3-0A40-86BB-D4D7E96618DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="295">
   <si>
     <t>liv_000017</t>
   </si>
@@ -841,18 +841,9 @@
     <t>liv_020017</t>
   </si>
   <si>
-    <t>The Niger Expedtion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Niger Expedition, 25 September 1858, 24 June 1858 </t>
-  </si>
-  <si>
     <t>The Preston Chronicle and Lancashire Advertiser</t>
   </si>
   <si>
-    <t xml:space="preserve">25 September 1858, 24 June 1858 </t>
-  </si>
-  <si>
     <t>Aga, Selim, c.1826-1875</t>
   </si>
   <si>
@@ -865,12 +856,6 @@
     <t>liv_020022</t>
   </si>
   <si>
-    <t>Jubilee of the Venerable Patriarch Brownlee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jubilee of the Venerable Patriarch Brownlee, 14 February 1867, 17 January 1867 </t>
-  </si>
-  <si>
     <t>Soga, Tiyo, c.1831-1871</t>
   </si>
   <si>
@@ -899,6 +884,39 @@
   </si>
   <si>
     <t>Serowe, Palapye Road, Bechuanaland Protectorate</t>
+  </si>
+  <si>
+    <t>liv_020018</t>
+  </si>
+  <si>
+    <t>“Jubilee of the Venerable Patriarch Brownlee”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“Jubilee of the Venerable Patriarch Brownlee,” 14 February 1867, 17 January 1867 </t>
+  </si>
+  <si>
+    <t>“The Niger Expedtion”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“The Niger Expedition,” 25 September 1858, 24 June 1858 </t>
+  </si>
+  <si>
+    <t>“Letter of Gratitude from a Kafir Woman”</t>
+  </si>
+  <si>
+    <t>“Letter of Gratitude from a Kafir Woman,” 1 May 1874</t>
+  </si>
+  <si>
+    <t>Jotelo, Nosutu Soga</t>
+  </si>
+  <si>
+    <t>54, 56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 September 1858; 24 June 1858 </t>
+  </si>
+  <si>
+    <t>1 May 1874; October 1873</t>
   </si>
 </sst>
 </file>
@@ -1320,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF22"/>
+  <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1911,7 +1929,7 @@
       <c r="P15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="R15" s="1">
         <v>93</v>
       </c>
       <c r="S15" s="1" t="s">
@@ -2085,51 +2103,51 @@
         <v>268</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>120</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="S20" s="1">
         <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="68">
       <c r="A21" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>120</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="Q21" s="1">
         <v>1</v>
@@ -2138,21 +2156,21 @@
         <v>82</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="68">
       <c r="A22" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>119</v>
@@ -2167,13 +2185,45 @@
         <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R22" s="1">
+        <v>89</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="51">
+      <c r="A23" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2403,10 +2453,10 @@
         <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>174</v>

</xml_diff>

<commit_message>
update mods for new sarasvati items
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011AD811-EBD3-0A40-86BB-D4D7E96618DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266472F-D624-994D-A889-F692F1F74168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="309">
   <si>
     <t>liv_000017</t>
   </si>
@@ -917,6 +917,48 @@
   </si>
   <si>
     <t>1 May 1874; October 1873</t>
+  </si>
+  <si>
+    <t>liv_021019</t>
+  </si>
+  <si>
+    <t>liv_021020</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati (with Facsimile Signature)</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati (with Facsimile Signature), [late nineteenth century]</t>
+  </si>
+  <si>
+    <t>Gutekunst, Frederick, 1831-1917</t>
+  </si>
+  <si>
+    <t>Sarasvati, Pandita Ramabai, 1858-1922</t>
+  </si>
+  <si>
+    <t>The High-Caste Hindu Woman</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Press of The Jas B. Rodgers Printing Co.</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati, 1898</t>
+  </si>
+  <si>
+    <t>Manoramabai</t>
+  </si>
+  <si>
+    <t>The Widow's Friend</t>
+  </si>
+  <si>
+    <t>George Robertson &amp;amp; Co.</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
@@ -2234,11 +2276,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD18"/>
+  <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AH20" sqref="AH20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2995,6 +3037,85 @@
         <v>243</v>
       </c>
     </row>
+    <row r="19" spans="1:25" ht="85">
+      <c r="A19" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1887</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="51">
+      <c r="A20" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="X20" s="1">
+        <v>1903</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE7">
     <sortCondition ref="A2:A7"/>

</xml_diff>

<commit_message>
update mods for new Semane images
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7266472F-D624-994D-A889-F692F1F74168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B93BE2-2784-1248-9BF6-47B0152061BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="360">
   <si>
     <t>liv_000017</t>
   </si>
@@ -959,13 +959,166 @@
   </si>
   <si>
     <t>George Robertson &amp;amp; Co.</t>
+  </si>
+  <si>
+    <t>[alt text]</t>
+  </si>
+  <si>
+    <t>liv_000003</t>
+  </si>
+  <si>
+    <t>Two pages from a David Livingstone diary describing an exchange with Bon Ale/Bin Aleī and with the latter’s name in Arabic.</t>
+  </si>
+  <si>
+    <t>liv_000023</t>
+  </si>
+  <si>
+    <t>Page from a David Livingstone notebook with a detailed Swahili vocabulary list and Arabic numbers from 1 to 10 and 10 to 90.</t>
+  </si>
+  <si>
+    <t>Jacob Wainwright seated on board the ship “Malwa” and leaning against David Livingstone’s coffin and other boxes.</t>
+  </si>
+  <si>
+    <t>Jacob Wainwright standing with head bowed in front of David Livingstone’s coffin which is partly covered by a British flag.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Jacob Wainwright, in three-quarters profile facing to his right.</t>
+  </si>
+  <si>
+    <t>Portrait from the knees up of Abdullah Susi, seated, in half profile facing to his right and holding a walking stick.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Matthew Wellington, facing forward.</t>
+  </si>
+  <si>
+    <t>James Chuma (kneeling) and Abdullah Susi (seated) beside notebooks, maps, and other personal effects of David Livingstone.</t>
+  </si>
+  <si>
+    <t>Portrait from waist up of Matthew Wellington, seated and turned slightly to his right.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Matthew Wellington, in three-quarters profile facing to his left.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Sechele, in a golden frame.</t>
+  </si>
+  <si>
+    <t>African hut among a set of trees; caption says Susi and Chuma made this hut to model the one where David Livingstone died</t>
+  </si>
+  <si>
+    <t>Apolo Kagwa and his son, both seated at a table; Kagwa holds a pen above a notebook</t>
+  </si>
+  <si>
+    <t>Ham Mukasa’s father, Ham Mukasa with a child on his lap, and Ham Mukasa’s wife with a child on her lap, all seated</t>
+  </si>
+  <si>
+    <t>Headshot of Edward Wilmot Blyden.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Sarojini Naidu, in half profile facing to her right; facsimile signature below image.</t>
+  </si>
+  <si>
+    <t>Full-body portrait of Swami Vivekanada, standing, his body turned to the right but facing forward, holding a walking stick</t>
+  </si>
+  <si>
+    <t>Portrait from the knees up of Cornelia Sorabji, in seven-eighths profile with body turned to her left, but facing right.</t>
+  </si>
+  <si>
+    <t>Full-body portrait of Ham Mukasa, facing forward, and Apolo Kagwa, in three-quarters profile facing to his right, standing.</t>
+  </si>
+  <si>
+    <t>Page inscribed by Solomon T. Plaatje to Professor Kelly Miller, dated November 16, 1921, with reference to Howard University.</t>
+  </si>
+  <si>
+    <t>Portrait from the knees up of Solomon T. Plaatje, seated, in three-quarters profile facing to his right, writing at a table.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Elizabeth Lilith M'belle (Mrs. S.T. Plaatje); caption notes her contribution to Plaatje’ book.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Pandita Ramabai Sarasvati.</t>
+  </si>
+  <si>
+    <t>liv_021021</t>
+  </si>
+  <si>
+    <t>liv_021022</t>
+  </si>
+  <si>
+    <t>liv_021023</t>
+  </si>
+  <si>
+    <t>liv_021024</t>
+  </si>
+  <si>
+    <t>liv_021025</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Africa/Photographs/Box 7/File 45/20</t>
+  </si>
+  <si>
+    <t>[Bechualand]</t>
+  </si>
+  <si>
+    <t>[Early twentieth century]</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Africa/Photographs/Box 7/File 45/24</t>
+  </si>
+  <si>
+    <t>Jones, Neville</t>
+  </si>
+  <si>
+    <t>Semane Khama, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Semane Khama</t>
+  </si>
+  <si>
+    <t>Semane Khama, and Semane Khama and Schoolchildren (Collage Created by the London Missionary Society Editorial Office)</t>
+  </si>
+  <si>
+    <t>Semane Khama, and Semane Khama and Schoolchildren (Collage Created by the London Missionary Society Editorial Office); [early twentieth century], [early twentieth century]</t>
+  </si>
+  <si>
+    <t>“Tshekedi [Khama] with the Small Chief for Whom He Acts as Regent [Seretse Khama] &amp; Tshekedi’s mother [Semane Khama]”</t>
+  </si>
+  <si>
+    <t>“Tshekedi [Khama] with the Small Chief for Whom He Acts as Regent [Seretse Khama] &amp; Tshekedi’s mother [Semane Khama],” [early twentieth century]</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Africa/Photographs/Box 7/File 51/25</t>
+  </si>
+  <si>
+    <t>Serowe</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Africa/Photographs/Box 7/File 51/29</t>
+  </si>
+  <si>
+    <t>Semane Khama and Children, Khama III's Jubilee</t>
+  </si>
+  <si>
+    <t>Semane Khama and Children, Khama III's Jubilee, 1911</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Missionary Portraits/Box 12/File 34/5a</t>
+  </si>
+  <si>
+    <t>Gilbert, [?]</t>
+  </si>
+  <si>
+    <t>Tshekedi and Semane Khama</t>
+  </si>
+  <si>
+    <t>Tshekedi and Semane Khama, [early twentieth century]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -988,11 +1141,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1042,7 +1207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1053,17 +1218,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1383,7 +1563,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -1401,7 +1581,7 @@
     <col min="16" max="19" width="15.83203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="20.83203125" style="1" customWidth="1"/>
     <col min="21" max="21" width="12.83203125" style="3" customWidth="1"/>
-    <col min="22" max="32" width="15.83203125" style="5" customWidth="1"/>
+    <col min="22" max="32" width="15.83203125" style="4" customWidth="1"/>
     <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -2035,35 +2215,35 @@
       <c r="G17" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
       <c r="V17" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="X17" s="5" t="s">
+      <c r="X17" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="Y17" s="5" t="s">
+      <c r="Y17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Z17" s="5" t="s">
+      <c r="Z17" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AA17" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="AB17" s="5" t="s">
+      <c r="AB17" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="AC17" s="5" t="s">
+      <c r="AC17" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="AE17" s="5">
+      <c r="AE17" s="4">
         <v>1906</v>
       </c>
-      <c r="AF17" s="5">
+      <c r="AF17" s="4">
         <v>74</v>
       </c>
     </row>
@@ -2229,7 +2409,7 @@
       <c r="L22" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="5" t="s">
         <v>282</v>
       </c>
       <c r="N22" s="1" t="s">
@@ -2276,844 +2456,1106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD20"/>
+  <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH20" sqref="AH20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
-    <col min="4" max="6" width="20.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="6" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="3" customWidth="1"/>
-    <col min="10" max="12" width="20.83203125" style="1" customWidth="1"/>
-    <col min="13" max="15" width="15.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.83203125" style="3" customWidth="1"/>
-    <col min="17" max="18" width="16.5" style="5" customWidth="1"/>
-    <col min="19" max="25" width="15.83203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" style="3" customWidth="1"/>
-    <col min="27" max="31" width="15.83203125" style="1" customWidth="1"/>
-    <col min="32" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="15" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="7" customWidth="1"/>
+    <col min="4" max="6" width="20.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" style="9" customWidth="1"/>
+    <col min="10" max="12" width="20.83203125" style="7" customWidth="1"/>
+    <col min="13" max="15" width="15.83203125" style="7" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" style="9" customWidth="1"/>
+    <col min="17" max="18" width="16.5" style="10" customWidth="1"/>
+    <col min="19" max="25" width="15.83203125" style="7" customWidth="1"/>
+    <col min="26" max="26" width="15.83203125" style="9" customWidth="1"/>
+    <col min="27" max="30" width="15.83203125" style="7" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" style="9" customWidth="1"/>
+    <col min="32" max="34" width="45.83203125" style="7" customWidth="1"/>
+    <col min="35" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="34">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:33" s="6" customFormat="1" ht="34">
+      <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="102">
-      <c r="A2" s="1" t="s">
+      <c r="AF1" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="102">
+      <c r="A2" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="7">
         <v>1874</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" ht="51">
-      <c r="A3" s="1" t="s">
+      <c r="AF2" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="51">
+      <c r="A3" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="7">
         <v>1874</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" ht="51">
-      <c r="A4" s="1" t="s">
+      <c r="AF3" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="51">
+      <c r="A4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" ht="51">
-      <c r="A5" s="1" t="s">
+      <c r="AF4" s="11" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="51">
+      <c r="A5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" ht="34">
-      <c r="A6" s="1" t="s">
+      <c r="AF5" s="11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="34">
+      <c r="A6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" ht="119">
-      <c r="A7" s="1" t="s">
+      <c r="AF6" s="11" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="119">
+      <c r="A7" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" ht="68">
-      <c r="A8" s="1" t="s">
+      <c r="AF7" s="11" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="68">
+      <c r="A8" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" ht="51">
-      <c r="A9" s="1" t="s">
+      <c r="AF8" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="AG8" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="51">
+      <c r="A9" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" ht="102">
-      <c r="A10" s="1" t="s">
+      <c r="AF9" s="11" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="102">
+      <c r="A10" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" ht="136">
-      <c r="A11" s="1" t="s">
+      <c r="AF10" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="136">
+      <c r="A11" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="Q11" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="R11" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="7">
         <v>1904</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Y11" s="7" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" ht="68">
-      <c r="A12" s="1" t="s">
+      <c r="AF11" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="AG11" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="68">
+      <c r="A12" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="7">
         <v>1920</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c r="Y12" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" ht="68">
-      <c r="A13" s="1" t="s">
+      <c r="AF12" s="11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="68">
+      <c r="A13" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="S13" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="T13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="U13" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="W13" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13" s="7">
         <v>1912</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Y13" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" ht="51">
-      <c r="A14" s="1" t="s">
+      <c r="AF13" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="51">
+      <c r="A14" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="Q14" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="S14" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="X14" s="1">
+      <c r="X14" s="7">
         <v>1901</v>
       </c>
-      <c r="Y14" s="1" t="s">
+      <c r="Y14" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" ht="85">
-      <c r="A15" s="1" t="s">
+      <c r="AF14" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="85">
+      <c r="A15" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="S15" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="V15" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="X15" s="1">
+      <c r="X15" s="7">
         <v>1901</v>
       </c>
-      <c r="Y15" s="1" t="s">
+      <c r="Y15" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" ht="51">
-      <c r="A16" s="1" t="s">
+      <c r="AF15" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="51">
+      <c r="A16" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="Q16" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="T16" s="1" t="s">
+      <c r="T16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="V16" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="X16" s="1">
+      <c r="X16" s="7">
         <v>1904</v>
       </c>
-      <c r="Y16" s="1" t="s">
+      <c r="Y16" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="68">
-      <c r="A17" s="1" t="s">
+      <c r="AF16" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="68">
+      <c r="A17" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S17" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="T17" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V17" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W17" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="X17" s="1">
+      <c r="X17" s="7">
         <v>1912</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="Y17" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="153">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:34" ht="153">
+      <c r="A18" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="Q18" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="S18" s="1" t="s">
+      <c r="S18" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U18" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="W18" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X18" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="Y18" s="1" t="s">
+      <c r="Y18" s="7" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" ht="85">
-      <c r="A19" s="1" t="s">
+      <c r="AF18" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="AG18" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH18" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="85">
+      <c r="A19" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="Q19" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="S19" s="1" t="s">
+      <c r="S19" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="T19" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="V19" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19" s="7">
         <v>1887</v>
       </c>
-      <c r="Y19" s="1" t="s">
+      <c r="Y19" s="7" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" ht="51">
-      <c r="A20" s="1" t="s">
+      <c r="AF19" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="51">
+      <c r="A20" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="Q20" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="R20" s="5" t="s">
+      <c r="R20" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="S20" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="T20" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V20" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="X20" s="1">
+      <c r="X20" s="7">
         <v>1903</v>
       </c>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="7" t="s">
         <v>212</v>
+      </c>
+      <c r="AF20" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="51">
+      <c r="A21" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF21" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="51">
+      <c r="A22" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF22" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" ht="153">
+      <c r="A23" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" ht="51">
+      <c r="A24" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="136">
+      <c r="A25" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M25" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="51">
+      <c r="A26" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="N26" s="7">
+        <v>1911</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="68">
+      <c r="A27" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for alt semane text
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B93BE2-2784-1248-9BF6-47B0152061BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1562907-6E57-4247-ACC3-80020C234E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="370">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1112,6 +1112,36 @@
   </si>
   <si>
     <t>Tshekedi and Semane Khama, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Verso of image, stating that image is of "Tshekedi and his mother Semane" and "Photo by Miss Gilbert."</t>
+  </si>
+  <si>
+    <t>Stamped verso of image, stating that image is of "Khama's wife, children" and dates to "Khama's Jubilee 1911"</t>
+  </si>
+  <si>
+    <t>Full-body portrait of Tshekedi Khama in three-quarters profile turning to his left, and Semane Khama facing forward, standing.</t>
+  </si>
+  <si>
+    <t>The Khamas standing: Semane in seven-eights profile turned to her left, Seretse facing forward, and Tshekedi in three-quarters profile turned to his right.</t>
+  </si>
+  <si>
+    <t>Stamped verso of image, stating that image is of "Tshekedi with the small chief for whom he acts as regent, &amp; Tshekedi's mother"</t>
+  </si>
+  <si>
+    <t>Semane Khama in half-body portrait, facing to her right</t>
+  </si>
+  <si>
+    <t>Verso of image, stating that image is of "Semane, Khama's wife" and "Photo by Neville Jones."</t>
+  </si>
+  <si>
+    <t>Semane Khama at right, seated, with two children to her at left, one of whom is standing, one of whom is seated.</t>
+  </si>
+  <si>
+    <t>Montage: Semane Khama seated, surrounded by children; Semane Khama in half profile to her right, but facing forward</t>
+  </si>
+  <si>
+    <t>Verso of image, stating that image is of "Semane."</t>
   </si>
 </sst>
 </file>
@@ -2459,8 +2489,8 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3417,6 +3447,12 @@
       <c r="O23" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="AF23" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="AG23" s="7" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="24" spans="1:34" ht="51">
       <c r="A24" s="7" t="s">
@@ -3452,6 +3488,12 @@
       <c r="O24" s="7" t="s">
         <v>341</v>
       </c>
+      <c r="AF24" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="AG24" s="11" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="25" spans="1:34" ht="136">
       <c r="A25" s="7" t="s">
@@ -3487,6 +3529,12 @@
       <c r="O25" s="7" t="s">
         <v>352</v>
       </c>
+      <c r="AF25" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="AG25" s="7" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="26" spans="1:34" ht="51">
       <c r="A26" s="7" t="s">
@@ -3522,6 +3570,12 @@
       <c r="O26" s="7" t="s">
         <v>352</v>
       </c>
+      <c r="AF26" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="AG26" s="7" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="27" spans="1:34" ht="68">
       <c r="A27" s="7" t="s">
@@ -3556,6 +3610,12 @@
       </c>
       <c r="O27" s="7" t="s">
         <v>341</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="AG27" s="11" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for semane alts
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1ACD081-E6AB-5541-8AA2-64FB258CBEE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2338D6DD-73A4-0447-9038-319438D7ABED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1129,19 +1129,19 @@
     <t>Stamped verso of image, stating that image is of "Tshekedi with the small chief for whom he acts as regent, &amp; Tshekedi's mother"</t>
   </si>
   <si>
-    <t>Semane Khama in half-body portrait, facing to her right</t>
-  </si>
-  <si>
     <t>Verso of image, stating that image is of "Semane, Khama's wife" and "Photo by Neville Jones."</t>
   </si>
   <si>
-    <t>Semane Khama at right, seated, with two children to her at left, one of whom is standing, one of whom is seated.</t>
-  </si>
-  <si>
-    <t>Montage: Semane Khama seated, surrounded by children; Semane Khama in half profile to her right, but facing forward</t>
-  </si>
-  <si>
     <t>Verso of image, stating that image is of "Semane."</t>
+  </si>
+  <si>
+    <t>Montage: Semane Khama seated, surrounded by children; Semane Khama in half profile turned to her right, but facing forward.</t>
+  </si>
+  <si>
+    <t>Half-body portrait of Semane Khama, facing to her right.</t>
+  </si>
+  <si>
+    <t>Semane Khama at right, seated, with two children at left, one of whom is standing, one of whom is seated.</t>
   </si>
 </sst>
 </file>
@@ -2488,9 +2488,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomLeft" activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3448,10 +3448,10 @@
         <v>341</v>
       </c>
       <c r="AF23" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="51">
@@ -3489,10 +3489,10 @@
         <v>341</v>
       </c>
       <c r="AF24" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="AG24" s="11" t="s">
         <v>365</v>
-      </c>
-      <c r="AG24" s="11" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="136">
@@ -3571,7 +3571,7 @@
         <v>352</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AG26" s="7" t="s">
         <v>361</v>

</xml_diff>

<commit_message>
update MODS with Johnson/Sarasvati
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5436E6D-A178-F840-8CDF-6C4F7D3DF1C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D359ED-C305-0749-863E-0017DFF647F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="460" windowWidth="24960" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="6960" windowWidth="24880" windowHeight="9040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
     <sheet name="Artifacts" sheetId="1" r:id="rId2"/>
+    <sheet name="dev" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="438">
   <si>
     <t>liv_000017</t>
   </si>
@@ -763,9 +772,6 @@
     <t>[1920?]</t>
   </si>
   <si>
-    <t>n.pag.</t>
-  </si>
-  <si>
     <t>[periodicals/artifacts]</t>
   </si>
   <si>
@@ -1142,13 +1148,220 @@
   </si>
   <si>
     <t>The Khamas standing: Semane in seven-eighths profile turned to her left, Seretse facing forward, and Tshekedi in three-quarters profile turned to his right.</t>
+  </si>
+  <si>
+    <t>liv_021026</t>
+  </si>
+  <si>
+    <t>liv_021027</t>
+  </si>
+  <si>
+    <t>liv_021028</t>
+  </si>
+  <si>
+    <t>liv_021029</t>
+  </si>
+  <si>
+    <t>liv_021030</t>
+  </si>
+  <si>
+    <t>liv_021031</t>
+  </si>
+  <si>
+    <t>liv_021032</t>
+  </si>
+  <si>
+    <t>liv_021033</t>
+  </si>
+  <si>
+    <t>liv_021034</t>
+  </si>
+  <si>
+    <t>[Late nineteenth century]</t>
+  </si>
+  <si>
+    <t>[British India/Britain/United States?]</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Missionary Portraits/Box 12 - Ramabai/1b</t>
+  </si>
+  <si>
+    <t>CWM/LMS/Home/Missionary Portraits/Box 12 - Ramabai/2</t>
+  </si>
+  <si>
+    <t>[British India/Britain?]</t>
+  </si>
+  <si>
+    <t>J. Paul</t>
+  </si>
+  <si>
+    <t>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</t>
+  </si>
+  <si>
+    <t>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai,” [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati, [late nineteenth century]</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Pandita Ramabai Sarasvati with paper border.</t>
+  </si>
+  <si>
+    <t>Pandita Ramabai Sarasvati seated and reading a book, with Monramabai standing behind and looking over Sarasvati's shoulder.</t>
+  </si>
+  <si>
+    <t>Verso of image, stating that image is of “Pandita Ramabai &amp; her gifted daughter Manoramabai” and “Photo J. Paul.”</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson, standing with back to viewer, but with head in half profile to the right.</t>
+  </si>
+  <si>
+    <t>Johnson, E. Pauline, 1861-1913</t>
+  </si>
+  <si>
+    <t>“And He Said ‘Fight On’”</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>The Musson Book Co., Limited</t>
+  </si>
+  <si>
+    <t>n.p.</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>“And He Said ‘Fight On’” (facsimile of manuscript)</t>
+  </si>
+  <si>
+    <t>“And He Said ‘Fight On’” (facsimile of manuscript), [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Canadian Born</t>
+  </si>
+  <si>
+    <t>George N. Morang &amp; Co., Limited</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson (with Facsimile Signature)</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson (with Facsimile Signature), [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Legends of Vancouver</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>Geo. S. Forsyth &amp; Co.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of E. Pauline Johnson, facing left.</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson, standing in half profile, with her head turned to her left, signed "Faithfully" and with her name.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of E. Pauline Johnson, facing left, signed "Yours Faithfully" and with her name.</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of E. Pauline Johnson, facing left. Johnson wears a hat and fur coat.</t>
+  </si>
+  <si>
+    <t>The Moccasin Maker</t>
+  </si>
+  <si>
+    <t>William Briggs</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson, 1904</t>
+  </si>
+  <si>
+    <t>“When George Was King” and Other Poems</t>
+  </si>
+  <si>
+    <t>The Brockville Times</t>
+  </si>
+  <si>
+    <t>Brockville</t>
+  </si>
+  <si>
+    <t>Images Related to E. Pauline Johnson's Grave</t>
+  </si>
+  <si>
+    <t>Images Related to E. Pauline Johnson's Grave, [early twentieth century]</t>
+  </si>
+  <si>
+    <t>Marega, Sergison, 1871-1939</t>
+  </si>
+  <si>
+    <t>E. Pauline Johnson's grave with a railing in front of it.</t>
+  </si>
+  <si>
+    <t>Siwash Rock.</t>
+  </si>
+  <si>
+    <t>Sculpted memorial for E. Pauline Johnson, including one figure at left and two figures at right.</t>
+  </si>
+  <si>
+    <t>opposite 10, opposite 17, opposite 19</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021026_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;/a&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;li&gt;</t>
+  </si>
+  <si>
+    <t>.&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021027_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021028_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021029_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021030_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021031_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021032_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021033_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="transcriptions/liv_021034_ART.html"&gt;</t>
+  </si>
+  <si>
+    <t>Facsimile of E. Pauline Johnson's manuscript of “And He Said ‘Fight On’”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1189,8 +1402,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,6 +1426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1237,7 +1463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1276,6 +1502,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1593,11 +1826,11 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
@@ -1615,7 +1848,7 @@
     <col min="33" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="2" customFormat="1" ht="34">
+    <row r="1" spans="1:32" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>115</v>
       </c>
@@ -1659,7 +1892,7 @@
         <v>124</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>133</v>
@@ -1677,16 +1910,16 @@
         <v>123</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>201</v>
@@ -1713,7 +1946,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="51">
+    <row r="2" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1748,7 +1981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="34">
+    <row r="3" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +2016,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="51">
+    <row r="4" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1818,7 +2051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="51">
+    <row r="5" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +2086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="34">
+    <row r="6" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1888,7 +2121,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="34">
+    <row r="7" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1923,7 +2156,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="68">
+    <row r="8" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1961,7 +2194,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="68">
+    <row r="9" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1993,7 +2226,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="68">
+    <row r="10" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2025,7 +2258,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="51">
+    <row r="11" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2293,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="68">
+    <row r="12" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2095,7 +2328,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="68">
+    <row r="13" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2130,7 +2363,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="34">
+    <row r="14" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2162,7 +2395,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="68">
+    <row r="15" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2191,7 +2424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="85">
+    <row r="16" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2226,7 +2459,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="85">
+    <row r="17" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -2259,16 +2492,16 @@
         <v>67</v>
       </c>
       <c r="Z17" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA17" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="AA17" s="4" t="s">
+      <c r="AB17" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="AB17" s="4" t="s">
+      <c r="AC17" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="AE17" s="4">
         <v>1906</v>
@@ -2277,7 +2510,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="85">
+    <row r="18" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>176</v>
       </c>
@@ -2312,7 +2545,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="51">
+    <row r="19" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>179</v>
       </c>
@@ -2350,56 +2583,56 @@
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="68">
+    <row r="20" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>120</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S20" s="1">
         <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="68">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>120</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q21" s="1">
         <v>1</v>
@@ -2408,21 +2641,21 @@
         <v>82</v>
       </c>
       <c r="T21" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" ht="68">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>119</v>
@@ -2437,13 +2670,13 @@
         <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="N22" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="P22" s="1" t="s">
         <v>82</v>
@@ -2452,27 +2685,27 @@
         <v>89</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" ht="51">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>120</v>
@@ -2486,14 +2719,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH27"/>
+  <dimension ref="A1:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG25" sqref="AG25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="7" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="7" customWidth="1"/>
@@ -2514,7 +2747,7 @@
     <col min="35" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="6" customFormat="1" ht="34">
+    <row r="1" spans="1:33" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>115</v>
       </c>
@@ -2561,16 +2794,16 @@
         <v>124</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>201</v>
@@ -2591,7 +2824,7 @@
         <v>129</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AA1" s="6" t="s">
         <v>133</v>
@@ -2606,94 +2839,37 @@
         <v>129</v>
       </c>
       <c r="AF1" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" ht="102">
-      <c r="A2" s="7" t="s">
+      <c r="AF2" s="11" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF3" s="11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="7">
-        <v>1874</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="51">
-      <c r="A3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="N3" s="7">
-        <v>1874</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="AF3" s="11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="51">
-      <c r="A4" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>121</v>
@@ -2701,31 +2877,37 @@
       <c r="J4" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="K4" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="L4" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1874</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" ht="51">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>272</v>
+        <v>105</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>271</v>
+        <v>114</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>121</v>
@@ -2734,36 +2916,33 @@
         <v>16</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>94</v>
+        <v>134</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1874</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>136</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" ht="34">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>121</v>
@@ -2771,37 +2950,31 @@
       <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="L6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>136</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="119">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>90</v>
+        <v>271</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>91</v>
+        <v>270</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>121</v>
@@ -2810,13 +2983,13 @@
         <v>16</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>94</v>
@@ -2825,12 +2998,12 @@
         <v>136</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="68">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>98</v>
@@ -2848,13 +3021,13 @@
         <v>16</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>161</v>
+        <v>100</v>
       </c>
       <c r="N8" s="7" t="s">
         <v>101</v>
@@ -2863,24 +3036,21 @@
         <v>136</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="AG8" s="11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" ht="51">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>158</v>
+        <v>90</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>255</v>
+        <v>91</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>174</v>
+        <v>89</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>121</v>
@@ -2892,30 +3062,30 @@
         <v>67</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>162</v>
+        <v>87</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>159</v>
+        <v>94</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" ht="102">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>256</v>
+        <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>174</v>
@@ -2933,27 +3103,30 @@
         <v>156</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="AF10" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" ht="136">
+        <v>319</v>
+      </c>
+      <c r="AG10" s="11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>174</v>
@@ -2961,46 +3134,37 @@
       <c r="G11" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q11" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="R11" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="U11" s="7" t="s">
+      <c r="J11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="W11" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="X11" s="7">
-        <v>1904</v>
-      </c>
-      <c r="Y11" s="7" t="s">
-        <v>200</v>
+      <c r="L11" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="AG11" s="11" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" ht="68">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>174</v>
@@ -3008,46 +3172,37 @@
       <c r="G12" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="T12" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="U12" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="V12" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="W12" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="X12" s="7">
-        <v>1920</v>
-      </c>
-      <c r="Y12" s="7" t="s">
-        <v>212</v>
+      <c r="J12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" ht="68">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>254</v>
+        <v>197</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>174</v>
@@ -3059,42 +3214,42 @@
         <v>120</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="T13" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="U13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="U13" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>215</v>
-      </c>
       <c r="W13" s="7" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="X13" s="7">
-        <v>1912</v>
+        <v>1904</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="AF13" s="11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="51">
+        <v>323</v>
+      </c>
+      <c r="AG13" s="11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>174</v>
@@ -3106,39 +3261,45 @@
         <v>120</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>221</v>
+        <v>208</v>
+      </c>
+      <c r="U14" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>222</v>
+        <v>210</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="X14" s="7">
-        <v>1901</v>
+        <v>1920</v>
       </c>
       <c r="Y14" s="7" t="s">
         <v>212</v>
       </c>
       <c r="AF14" s="11" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" ht="85">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>250</v>
+        <v>174</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>121</v>
@@ -3147,39 +3308,45 @@
         <v>120</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>67</v>
       </c>
+      <c r="U15" s="7" t="s">
+        <v>209</v>
+      </c>
       <c r="V15" s="7" t="s">
-        <v>225</v>
+        <v>215</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="X15" s="7">
-        <v>1901</v>
+        <v>1912</v>
       </c>
       <c r="Y15" s="7" t="s">
         <v>212</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="51">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>121</v>
@@ -3188,39 +3355,39 @@
         <v>120</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>67</v>
+        <v>221</v>
       </c>
       <c r="V16" s="7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="X16" s="7">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="Y16" s="7" t="s">
         <v>212</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" ht="68">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>121</v>
@@ -3228,49 +3395,40 @@
       <c r="H17" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q17" s="7" t="s">
-        <v>230</v>
+      <c r="Q17" s="10" t="s">
+        <v>223</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="U17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="W17" s="7" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="X17" s="7">
-        <v>1912</v>
+        <v>1901</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" ht="153">
+        <v>212</v>
+      </c>
+      <c r="AF17" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>121</v>
@@ -3278,52 +3436,40 @@
       <c r="H18" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q18" s="13" t="s">
-        <v>236</v>
+      <c r="Q18" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="U18" s="7" t="s">
-        <v>209</v>
+        <v>67</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="W18" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="X18" s="7" t="s">
-        <v>242</v>
+        <v>226</v>
+      </c>
+      <c r="X18" s="7">
+        <v>1904</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>331</v>
-      </c>
-      <c r="AG18" s="11" t="s">
-        <v>332</v>
-      </c>
-      <c r="AH18" s="11" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" ht="85">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>295</v>
+        <v>195</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>297</v>
+        <v>264</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>298</v>
+        <v>265</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>299</v>
+        <v>230</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>121</v>
@@ -3331,40 +3477,49 @@
       <c r="H19" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q19" s="10" t="s">
-        <v>300</v>
+      <c r="Q19" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>301</v>
+        <v>231</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>302</v>
+        <v>232</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>303</v>
+        <v>233</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="X19" s="7">
-        <v>1887</v>
+        <v>1912</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="AF19" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" ht="51">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>296</v>
+        <v>196</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>304</v>
+        <v>262</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>174</v>
+        <v>236</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>121</v>
@@ -3372,56 +3527,134 @@
       <c r="H20" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q20" s="10" t="s">
+      <c r="Q20" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="W20" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="X20" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="AF20" s="11" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG20" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="AH20" s="11" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q21" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="S21" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="R20" s="10" t="s">
+      <c r="T21" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="X21" s="7">
+        <v>1887</v>
+      </c>
+      <c r="Y21" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF21" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="R22" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="S22" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="S20" s="7" t="s">
+      <c r="T22" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="V22" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="T20" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="X20" s="7">
+      <c r="X22" s="7">
         <v>1903</v>
       </c>
-      <c r="Y20" s="7" t="s">
+      <c r="Y22" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="AF20" s="11" t="s">
+      <c r="AF22" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" ht="153" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="21" spans="1:34" ht="51">
-      <c r="A21" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="AF21" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" ht="51">
-      <c r="A22" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="AF22" s="11" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="23" spans="1:34" ht="153">
-      <c r="A23" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="B23" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>347</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>348</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>174</v>
@@ -3439,33 +3672,33 @@
         <v>156</v>
       </c>
       <c r="M23" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="N23" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>341</v>
-      </c>
       <c r="AF23" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" ht="51">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>121</v>
@@ -3480,30 +3713,30 @@
         <v>156</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AG24" s="11" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="136">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>349</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>350</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>174</v>
@@ -3521,30 +3754,30 @@
         <v>156</v>
       </c>
       <c r="M25" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="O25" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="N25" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>352</v>
-      </c>
       <c r="AF25" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AG25" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" ht="51">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>354</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>355</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>174</v>
@@ -3562,33 +3795,33 @@
         <v>156</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N26" s="7">
         <v>1911</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="68">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>359</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>121</v>
@@ -3603,27 +3836,697 @@
         <v>156</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="O27" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG27" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M28" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="AF28" s="14" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="N29" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="AF27" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="AG27" s="11" t="s">
-        <v>360</v>
+      <c r="O29" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="AF29" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="AG29" s="7" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S30" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X30" s="7">
+        <v>1913</v>
+      </c>
+      <c r="Y30" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="X31" s="7">
+        <v>1913</v>
+      </c>
+      <c r="Y31" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="AF31" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q32" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S32" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="V32" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="X32" s="7">
+        <v>1913</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF32" s="7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="33" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="T33" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="X33" s="7">
+        <v>1913</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q34" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="V34" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="X34" s="7">
+        <v>1904</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q35" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="X35" s="7">
+        <v>1904</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="AF35" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG35" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="AH35" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q36" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="S36" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="T36" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="V36" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="X36" s="7">
+        <v>1908</v>
+      </c>
+      <c r="Y36" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF36" s="7" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE7">
-    <sortCondition ref="A2:A7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35043C1-934F-2441-9036-DCF88E610249}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" t="str">
+        <f>Artifacts!D28</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1" t="str">
+        <f>Artifacts!B28</f>
+        <v>Pandita Ramabai Sarasvati</v>
+      </c>
+      <c r="F1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" t="str">
+        <f>Artifacts!N28</f>
+        <v>[Late nineteenth century]</v>
+      </c>
+      <c r="H1" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1" s="16" t="str">
+        <f>A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1</f>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021026_ART.html"&gt;Pandita Ramabai Sarasvati&lt;/a&gt;. [Late nineteenth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" t="str">
+        <f>Artifacts!D29</f>
+        <v>J. Paul</v>
+      </c>
+      <c r="C2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E2" t="str">
+        <f>Artifacts!B29</f>
+        <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
+      </c>
+      <c r="F2" t="s">
+        <v>426</v>
+      </c>
+      <c r="G2" t="str">
+        <f>Artifacts!N29</f>
+        <v>[Early twentieth century]</v>
+      </c>
+      <c r="H2" t="s">
+        <v>428</v>
+      </c>
+      <c r="I2" s="16" t="str">
+        <f t="shared" ref="I2:I9" si="0">A2&amp;B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2</f>
+        <v>&lt;li&gt;J. Paul. &lt;a href="transcriptions/liv_021027_ART.html"&gt;“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B3" t="str">
+        <f>Artifacts!D30</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D3" t="s">
+        <v>430</v>
+      </c>
+      <c r="E3" t="str">
+        <f>Artifacts!B30</f>
+        <v>E. Pauline Johnson</v>
+      </c>
+      <c r="F3" t="s">
+        <v>426</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H3" t="s">
+        <v>428</v>
+      </c>
+      <c r="I3" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021028_ART.html"&gt;E. Pauline Johnson&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" t="str">
+        <f>Artifacts!D31</f>
+        <v>Johnson, E. Pauline, 1861-1913</v>
+      </c>
+      <c r="C4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E4" t="str">
+        <f>Artifacts!B31</f>
+        <v>“And He Said ‘Fight On’” (facsimile of manuscript)</v>
+      </c>
+      <c r="F4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H4" t="s">
+        <v>428</v>
+      </c>
+      <c r="I4" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Johnson, E. Pauline, 1861-1913. &lt;a href="transcriptions/liv_021029_ART.html"&gt;“And He Said ‘Fight On’” (facsimile of manuscript)&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" t="str">
+        <f>Artifacts!D32</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E5" t="str">
+        <f>Artifacts!B32</f>
+        <v>E. Pauline Johnson (with Facsimile Signature)</v>
+      </c>
+      <c r="F5" t="s">
+        <v>426</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H5" t="s">
+        <v>428</v>
+      </c>
+      <c r="I5" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021030_ART.html"&gt;E. Pauline Johnson (with Facsimile Signature)&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B6" t="str">
+        <f>Artifacts!D33</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C6" t="s">
+        <v>425</v>
+      </c>
+      <c r="D6" t="s">
+        <v>433</v>
+      </c>
+      <c r="E6" t="str">
+        <f>Artifacts!B33</f>
+        <v>E. Pauline Johnson (with Facsimile Signature)</v>
+      </c>
+      <c r="F6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="H6" t="s">
+        <v>428</v>
+      </c>
+      <c r="I6" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021031_ART.html"&gt;E. Pauline Johnson (with Facsimile Signature)&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B7" t="str">
+        <f>Artifacts!D34</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C7" t="s">
+        <v>425</v>
+      </c>
+      <c r="D7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E7" t="str">
+        <f>Artifacts!B34</f>
+        <v>E. Pauline Johnson</v>
+      </c>
+      <c r="F7" t="s">
+        <v>426</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1904</v>
+      </c>
+      <c r="H7" t="s">
+        <v>428</v>
+      </c>
+      <c r="I7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021032_ART.html"&gt;E. Pauline Johnson&lt;/a&gt;. 1904.&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B8" t="str">
+        <f>Artifacts!D35</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C8" t="s">
+        <v>425</v>
+      </c>
+      <c r="D8" t="s">
+        <v>435</v>
+      </c>
+      <c r="E8" t="str">
+        <f>Artifacts!B35</f>
+        <v>Images Related to E. Pauline Johnson's Grave</v>
+      </c>
+      <c r="F8" t="s">
+        <v>426</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="H8" t="s">
+        <v>428</v>
+      </c>
+      <c r="I8" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021033_ART.html"&gt;Images Related to E. Pauline Johnson's Grave&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B9" t="str">
+        <f>Artifacts!D36</f>
+        <v>Anonymous</v>
+      </c>
+      <c r="C9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" t="str">
+        <f>Artifacts!B36</f>
+        <v>E. Pauline Johnson</v>
+      </c>
+      <c r="F9" t="s">
+        <v>426</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="H9" t="s">
+        <v>428</v>
+      </c>
+      <c r="I9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021034_ART.html"&gt;E. Pauline Johnson&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update MODS for new Aga item
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7832E673-9616-4E41-8DED-7EE03C0171F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F776CF8-84C4-2845-8126-7A316BA0AAB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="445">
   <si>
     <t>liv_000017</t>
   </si>
@@ -577,9 +577,6 @@
     <t>“Gleanings and Glances” (Excerpt); “Letter from an African Chief”</t>
   </si>
   <si>
-    <t>“Gleanings and Glances” (Excerpt); “Letter from an African Chief,” 1 June 1894, 12 June 1893</t>
-  </si>
-  <si>
     <t>liv_003027</t>
   </si>
   <si>
@@ -868,9 +865,6 @@
     <t>Kaffrarian Watchman</t>
   </si>
   <si>
-    <t>14 February 1867</t>
-  </si>
-  <si>
     <t>liv_020024</t>
   </si>
   <si>
@@ -898,15 +892,9 @@
     <t>“Jubilee of the Venerable Patriarch Brownlee”</t>
   </si>
   <si>
-    <t xml:space="preserve">“Jubilee of the Venerable Patriarch Brownlee,” 14 February 1867, 17 January 1867 </t>
-  </si>
-  <si>
     <t>“The Niger Expedtion”</t>
   </si>
   <si>
-    <t xml:space="preserve">“The Niger Expedition,” 25 September 1858, 24 June 1858 </t>
-  </si>
-  <si>
     <t>“Letter of Gratitude from a Kafir Woman”</t>
   </si>
   <si>
@@ -1355,6 +1343,39 @@
   </si>
   <si>
     <t xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock”; 1913, 1913, 1913 </t>
+  </si>
+  <si>
+    <t>liv_020027</t>
+  </si>
+  <si>
+    <t>publications (documents)</t>
+  </si>
+  <si>
+    <t>Anti-Slavery Reporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 February 1867, 17 January 1867 </t>
+  </si>
+  <si>
+    <t>“Original Correspondence: West Africa”</t>
+  </si>
+  <si>
+    <t>“Original Correspondence: West Africa,” 1 February 1864</t>
+  </si>
+  <si>
+    <t>Chamerovzow, Louis-Alexis, 1800-1899</t>
+  </si>
+  <si>
+    <t>1 February 1864, 16 November 1863</t>
+  </si>
+  <si>
+    <t>“Jubilee of the Venerable Patriarch Brownlee,” 14 February 1867</t>
+  </si>
+  <si>
+    <t>“The Niger Expedition,” 25 September 1858</t>
+  </si>
+  <si>
+    <t>“Gleanings and Glances” (Excerpt); “Letter from an African Chief,” 1 June 1894</t>
   </si>
 </sst>
 </file>
@@ -1823,11 +1844,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF23"/>
+  <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1892,7 +1913,7 @@
         <v>124</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>133</v>
@@ -1910,34 +1931,34 @@
         <v>123</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="AE1" s="2" t="s">
         <v>123</v>
@@ -2211,7 +2232,7 @@
         <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>53</v>
@@ -2243,7 +2264,7 @@
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>56</v>
@@ -2278,7 +2299,7 @@
         <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>62</v>
@@ -2319,7 +2340,7 @@
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>69</v>
@@ -2354,7 +2375,7 @@
         <v>68</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>74</v>
@@ -2383,7 +2404,7 @@
         <v>78</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>79</v>
@@ -2409,7 +2430,7 @@
         <v>81</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>82</v>
@@ -2476,7 +2497,7 @@
         <v>154</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -2492,16 +2513,16 @@
         <v>67</v>
       </c>
       <c r="Z17" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA17" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="AA17" s="4" t="s">
+      <c r="AB17" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="AB17" s="4" t="s">
+      <c r="AC17" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>247</v>
       </c>
       <c r="AE17" s="4">
         <v>1906</v>
@@ -2510,7 +2531,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>176</v>
       </c>
@@ -2518,7 +2539,7 @@
         <v>177</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>178</v>
+        <v>444</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>174</v>
@@ -2527,7 +2548,7 @@
         <v>175</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P18" s="1" t="s">
         <v>169</v>
@@ -2547,19 +2568,19 @@
     </row>
     <row r="19" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>119</v>
@@ -2574,65 +2595,65 @@
         <v>68</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>287</v>
+        <v>443</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S20" s="1">
         <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>285</v>
+        <v>442</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="Q21" s="1">
         <v>1</v>
@@ -2641,21 +2662,21 @@
         <v>82</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>275</v>
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>279</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>119</v>
@@ -2670,45 +2691,74 @@
         <v>68</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="M22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R22" s="1">
-        <v>89</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="B23" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>120</v>
+        <v>435</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R23" s="1">
+        <v>89</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="S24" s="1">
+        <v>2</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -2721,7 +2771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
@@ -2794,28 +2844,28 @@
         <v>124</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="X1" s="6" t="s">
         <v>123</v>
@@ -2824,7 +2874,7 @@
         <v>129</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AA1" s="6" t="s">
         <v>133</v>
@@ -2839,23 +2889,23 @@
         <v>129</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="102" x14ac:dyDescent="0.2">
@@ -2893,7 +2943,7 @@
         <v>113</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -2928,7 +2978,7 @@
         <v>136</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -2960,7 +3010,7 @@
         <v>136</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -2968,10 +3018,10 @@
         <v>95</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>174</v>
@@ -2998,7 +3048,7 @@
         <v>136</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="34" x14ac:dyDescent="0.2">
@@ -3036,7 +3086,7 @@
         <v>136</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="119" x14ac:dyDescent="0.2">
@@ -3074,7 +3124,7 @@
         <v>136</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="68" x14ac:dyDescent="0.2">
@@ -3112,10 +3162,10 @@
         <v>136</v>
       </c>
       <c r="AF10" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AG10" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -3126,7 +3176,7 @@
         <v>158</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>174</v>
@@ -3153,7 +3203,7 @@
         <v>160</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="102" x14ac:dyDescent="0.2">
@@ -3164,7 +3214,7 @@
         <v>164</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>174</v>
@@ -3191,18 +3241,18 @@
         <v>168</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>174</v>
@@ -3214,42 +3264,42 @@
         <v>120</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="R13" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="S13" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>199</v>
       </c>
       <c r="U13" s="7" t="s">
         <v>67</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X13" s="7">
         <v>1904</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF13" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="AG13" s="11" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>174</v>
@@ -3261,42 +3311,42 @@
         <v>120</v>
       </c>
       <c r="Q14" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="S14" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="T14" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="T14" s="7" t="s">
+      <c r="U14" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="U14" s="7" t="s">
+      <c r="V14" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="W14" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="X14" s="7">
         <v>1920</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF14" s="11" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>174</v>
@@ -3308,42 +3358,42 @@
         <v>120</v>
       </c>
       <c r="Q15" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="S15" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>67</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V15" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="W15" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="W15" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="X15" s="7">
         <v>1912</v>
       </c>
       <c r="Y15" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>174</v>
@@ -3355,39 +3405,39 @@
         <v>120</v>
       </c>
       <c r="Q16" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="S16" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="T16" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="T16" s="7" t="s">
+      <c r="V16" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="X16" s="7">
         <v>1901</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>261</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>121</v>
@@ -3396,39 +3446,39 @@
         <v>120</v>
       </c>
       <c r="Q17" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="S17" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X17" s="7">
         <v>1901</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF17" s="11" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>229</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>121</v>
@@ -3437,39 +3487,39 @@
         <v>120</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T18" s="7" t="s">
         <v>67</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="X18" s="7">
         <v>1904</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="D19" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>121</v>
@@ -3478,48 +3528,48 @@
         <v>120</v>
       </c>
       <c r="Q19" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="S19" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="S19" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="U19" s="7" t="s">
         <v>67</v>
       </c>
       <c r="V19" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="W19" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="X19" s="7">
         <v>1912</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>263</v>
-      </c>
       <c r="D20" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>121</v>
@@ -3528,51 +3578,51 @@
         <v>120</v>
       </c>
       <c r="Q20" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S20" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="T20" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="T20" s="7" t="s">
+      <c r="U20" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="W20" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="U20" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="W20" s="7" t="s">
+      <c r="X20" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="X20" s="7" t="s">
-        <v>242</v>
-      </c>
       <c r="Y20" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="AF20" s="11" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="AG20" s="11" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="AH20" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>121</v>
@@ -3581,36 +3631,36 @@
         <v>120</v>
       </c>
       <c r="Q21" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="X21" s="7">
         <v>1887</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF21" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>174</v>
@@ -3622,39 +3672,39 @@
         <v>120</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V22" s="7" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="X22" s="7">
         <v>1903</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF22" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>174</v>
@@ -3672,33 +3722,33 @@
         <v>156</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="AF23" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>121</v>
@@ -3713,30 +3763,30 @@
         <v>156</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="AG24" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>174</v>
@@ -3754,30 +3804,30 @@
         <v>156</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="AF25" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="AG25" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>174</v>
@@ -3795,33 +3845,33 @@
         <v>156</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="N26" s="7">
         <v>1911</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>121</v>
@@ -3836,30 +3886,30 @@
         <v>156</v>
       </c>
       <c r="M27" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="AF27" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="AG27" s="11" t="s">
         <v>355</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="AF27" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="AG27" s="11" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>174</v>
@@ -3877,30 +3927,30 @@
         <v>156</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="AF28" s="14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>121</v>
@@ -3915,30 +3965,30 @@
         <v>156</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="AF29" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="AG29" s="7" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>174</v>
@@ -3947,39 +3997,39 @@
         <v>121</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S30" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V30" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="X30" s="7">
         <v>1913</v>
       </c>
       <c r="Y30" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="AF30" s="7" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>121</v>
@@ -3988,36 +4038,36 @@
         <v>120</v>
       </c>
       <c r="Q31" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="X31" s="7">
         <v>1913</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="AF31" s="7" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>174</v>
@@ -4026,36 +4076,36 @@
         <v>121</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="X32" s="7">
         <v>1913</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>174</v>
@@ -4064,36 +4114,36 @@
         <v>121</v>
       </c>
       <c r="Q33" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="X33" s="7">
         <v>1913</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF33" s="7" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="34" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>174</v>
@@ -4102,36 +4152,36 @@
         <v>121</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V34" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="X34" s="7">
         <v>1913</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AF34" s="7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>174</v>
@@ -4140,48 +4190,48 @@
         <v>174</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G35" s="7" t="s">
         <v>121</v>
       </c>
       <c r="Q35" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="X35" s="7">
         <v>1913</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="AF35" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AG35" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="AH35" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>174</v>
@@ -4190,16 +4240,16 @@
         <v>121</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="V36" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="X36" s="7">
         <v>1908</v>
@@ -4208,7 +4258,7 @@
         <v>2</v>
       </c>
       <c r="AF36" s="7" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -4238,31 +4288,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B1" t="str">
         <f>Artifacts!D28</f>
         <v>Anonymous</v>
       </c>
       <c r="C1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E1" t="str">
         <f>Artifacts!B28</f>
         <v>Pandita Ramabai Sarasvati</v>
       </c>
       <c r="F1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G1" t="str">
         <f>Artifacts!N28</f>
         <v>[Late nineteenth century]</v>
       </c>
       <c r="H1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I1" s="16" t="str">
         <f>A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1</f>
@@ -4271,31 +4321,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B2" t="str">
         <f>Artifacts!D29</f>
         <v>J. Paul</v>
       </c>
       <c r="C2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" t="s">
         <v>421</v>
-      </c>
-      <c r="D2" t="s">
-        <v>425</v>
       </c>
       <c r="E2" t="str">
         <f>Artifacts!B29</f>
         <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
       </c>
       <c r="F2" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G2" t="str">
         <f>Artifacts!N29</f>
         <v>[Early twentieth century]</v>
       </c>
       <c r="H2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I2" s="16" t="str">
         <f t="shared" ref="I2:I9" si="0">A2&amp;B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2</f>
@@ -4304,30 +4354,30 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B3" t="str">
         <f>Artifacts!D30</f>
         <v>Anonymous</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E3" t="str">
         <f>Artifacts!B30</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4336,30 +4386,30 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B4" t="str">
         <f>Artifacts!D31</f>
         <v>Johnson, E. Pauline, 1861-1913</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D4" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E4" t="str">
         <f>Artifacts!B31</f>
         <v>“And He Said ‘Fight On’” (Manuscript Facsimile)</v>
       </c>
       <c r="F4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4368,30 +4418,30 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B5" t="str">
         <f>Artifacts!D32</f>
         <v>Anonymous</v>
       </c>
       <c r="C5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D5" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E5" t="str">
         <f>Artifacts!B32</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F5" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4400,30 +4450,30 @@
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B6" t="str">
         <f>Artifacts!D33</f>
         <v>Anonymous</v>
       </c>
       <c r="C6" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D6" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E6" t="str">
         <f>Artifacts!B33</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F6" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H6" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I6" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4432,30 +4482,30 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B7" t="str">
         <f>Artifacts!D34</f>
         <v>Anonymous</v>
       </c>
       <c r="C7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E7" t="str">
         <f>Artifacts!B34</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G7" s="7">
         <v>1904</v>
       </c>
       <c r="H7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4464,30 +4514,30 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B8" t="str">
         <f>Artifacts!D35</f>
         <v>Anonymous</v>
       </c>
       <c r="C8" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D8" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E8" t="str">
         <f>Artifacts!B35</f>
         <v xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock” </v>
       </c>
       <c r="F8" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H8" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -4496,30 +4546,30 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B9" t="str">
         <f>Artifacts!D36</f>
         <v>Anonymous</v>
       </c>
       <c r="C9" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D9" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E9" t="str">
         <f>Artifacts!B36</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F9" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H9" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="I9" s="16" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
update mods for aga
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E50FB0-AF48-5D4F-9B36-3500BAD529DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919E0A04-4F3B-4B49-8B09-6CD847F1044E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1363,9 +1363,6 @@
     <t>“Original Correspondence: West Africa,” 1 February 1864</t>
   </si>
   <si>
-    <t>Chamerovzow, Louis-Alexis, 1800-1899</t>
-  </si>
-  <si>
     <t>1 February 1864, 16 November 1863</t>
   </si>
   <si>
@@ -1379,6 +1376,9 @@
   </si>
   <si>
     <t>27-28</t>
+  </si>
+  <si>
+    <t>Chamerovzow, Louis-Alexis, 1816-1875</t>
   </si>
 </sst>
 </file>
@@ -1849,9 +1849,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S24" sqref="S24"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2542,7 +2542,7 @@
         <v>177</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>174</v>
@@ -2615,7 +2615,7 @@
         <v>283</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>174</v>
@@ -2644,7 +2644,7 @@
         <v>282</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>174</v>
@@ -2746,7 +2746,7 @@
         <v>439</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>268</v>
@@ -2758,10 +2758,10 @@
         <v>436</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for tippu tip
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919E0A04-4F3B-4B49-8B09-6CD847F1044E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D687C1-9646-9C43-A003-FC21F9CB2B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="451">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1379,6 +1379,21 @@
   </si>
   <si>
     <t>Chamerovzow, Louis-Alexis, 1816-1875</t>
+  </si>
+  <si>
+    <t>liv_020028</t>
+  </si>
+  <si>
+    <t>“Tippoo Tib”</t>
+  </si>
+  <si>
+    <t>“Tippoo Tib,” 17 May 1887</t>
+  </si>
+  <si>
+    <t>Tippu Tip, 1837-1905</t>
+  </si>
+  <si>
+    <t>17 May 1887, 30 March 1887</t>
   </si>
 </sst>
 </file>
@@ -1847,11 +1862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF24"/>
+  <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2412,7 +2427,7 @@
       <c r="P14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="S14" s="1">
         <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
@@ -2762,6 +2777,35 @@
       </c>
       <c r="T24" s="1" t="s">
         <v>440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S25" s="1">
+        <v>5</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for sechele letter
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D687C1-9646-9C43-A003-FC21F9CB2B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8372E59A-C0AC-384E-8CE5-0E3AEDC940F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="456">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1394,6 +1394,21 @@
   </si>
   <si>
     <t>17 May 1887, 30 March 1887</t>
+  </si>
+  <si>
+    <t>liv_020020</t>
+  </si>
+  <si>
+    <t>“Statement of Sechele, Paramount Chief of the Bakwaina”</t>
+  </si>
+  <si>
+    <t>Edwards, Samuel</t>
+  </si>
+  <si>
+    <t>Cape Town Mail</t>
+  </si>
+  <si>
+    <t>30 April 1853; 21 April 1853</t>
   </si>
 </sst>
 </file>
@@ -1862,11 +1877,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ25" sqref="AJ25"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL25" sqref="AL25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2806,6 +2821,32 @@
       </c>
       <c r="T25" s="1" t="s">
         <v>450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for Watanna item
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFFC183-3431-D745-8EA1-95CF769CD0C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D961BE6-64F8-C544-B9B9-0849C7C6A36A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1549,12 +1549,6 @@
     <t>Head and shoulders portrait of Dhan Gopal Mukerji in half profile, facing left.</t>
   </si>
   <si>
-    <t>Page Inscribed to Lia W. Yindolph</t>
-  </si>
-  <si>
-    <t>Page Inscribed to Lia W. Yindolph, 17 June 1899</t>
-  </si>
-  <si>
     <t>Watanna, Onoto, 1875-1954</t>
   </si>
   <si>
@@ -1573,9 +1567,6 @@
     <t>Onoto Watanna and Illustration of Numè, Koto, and Matsu</t>
   </si>
   <si>
-    <t>Page inscribed by Onoto Watanna to Lia W. Yindolph and dated “Chicago June 17 1899.”</t>
-  </si>
-  <si>
     <t>Headshot of Onoto Watanna below illustration of Numè, Koto, and Matsu.</t>
   </si>
   <si>
@@ -1598,6 +1589,15 @@
   </si>
   <si>
     <t>Head and shoulders portrait of Jacob Wainwright, in three-quarters profile facing to his left.</t>
+  </si>
+  <si>
+    <t>Page Inscribed to Lea W. Lindolph</t>
+  </si>
+  <si>
+    <t>Page Inscribed to Lea W. Lindolph, 17 June 1899</t>
+  </si>
+  <si>
+    <t>Page inscribed by Onoto Watanna to Lea W. Lindolph and dated “Chicago June 17 1899.”</t>
   </si>
 </sst>
 </file>
@@ -3168,9 +3168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF6" sqref="AF6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3407,7 +3407,7 @@
         <v>136</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -4783,13 +4783,13 @@
         <v>491</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>502</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>504</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>119</v>
@@ -4798,28 +4798,28 @@
         <v>120</v>
       </c>
       <c r="Q40" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="T40" s="7" t="s">
         <v>504</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>506</v>
       </c>
       <c r="U40" s="7" t="s">
         <v>208</v>
       </c>
       <c r="V40" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="X40" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="Y40" s="7" t="s">
         <v>390</v>
       </c>
       <c r="AF40" s="7" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="AG40" s="11"/>
     </row>
@@ -4828,10 +4828,10 @@
         <v>492</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>509</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>512</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>174</v>
@@ -4846,19 +4846,19 @@
         <v>120</v>
       </c>
       <c r="Q41" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="T41" s="7" t="s">
         <v>504</v>
-      </c>
-      <c r="S41" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="T41" s="7" t="s">
-        <v>506</v>
       </c>
       <c r="U41" s="7" t="s">
         <v>208</v>
       </c>
       <c r="V41" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="X41" s="7">
         <v>1899</v>
@@ -4867,7 +4867,7 @@
         <v>211</v>
       </c>
       <c r="AF41" s="7" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="42" spans="1:34" ht="68" x14ac:dyDescent="0.2">
@@ -4875,10 +4875,10 @@
         <v>493</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>174</v>
@@ -4890,10 +4890,10 @@
         <v>120</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="T42" s="7" t="s">
         <v>208</v>
@@ -4902,7 +4902,7 @@
         <v>67</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="X42" s="7">
         <v>1902</v>
@@ -4911,7 +4911,7 @@
         <v>211</v>
       </c>
       <c r="AF42" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for watanna title
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D961BE6-64F8-C544-B9B9-0849C7C6A36A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE97220-FCFD-264B-9A3E-5FA44ACA4DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1564,15 +1564,9 @@
     <t>1899, 17 June 1899</t>
   </si>
   <si>
-    <t>Onoto Watanna and Illustration of Numè, Koto, and Matsu</t>
-  </si>
-  <si>
     <t>Headshot of Onoto Watanna below illustration of Numè, Koto, and Matsu.</t>
   </si>
   <si>
-    <t>Onoto Watanna and Illustration of Numè, Koto, and Matsu, [late nineteenth century]</t>
-  </si>
-  <si>
     <t>The Wooing of Wistaria</t>
   </si>
   <si>
@@ -1598,6 +1592,12 @@
   </si>
   <si>
     <t>Page inscribed by Onoto Watanna to Lea W. Lindolph and dated “Chicago June 17 1899.”</t>
+  </si>
+  <si>
+    <t>Onoto Watanna; Illustration of Numè, Koto, and Matsu</t>
+  </si>
+  <si>
+    <t>Onoto Watanna; Illustration of Numè, Koto, and Matsu, [late nineteenth century], 1899</t>
   </si>
 </sst>
 </file>
@@ -3169,8 +3169,8 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3407,7 +3407,7 @@
         <v>136</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -4783,10 +4783,10 @@
         <v>491</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>502</v>
@@ -4819,7 +4819,7 @@
         <v>390</v>
       </c>
       <c r="AF40" s="7" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AG40" s="11"/>
     </row>
@@ -4828,10 +4828,10 @@
         <v>492</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>507</v>
+        <v>517</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>174</v>
@@ -4867,7 +4867,7 @@
         <v>211</v>
       </c>
       <c r="AF41" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="42" spans="1:34" ht="68" x14ac:dyDescent="0.2">
@@ -4875,10 +4875,10 @@
         <v>493</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>174</v>
@@ -4893,7 +4893,7 @@
         <v>502</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="T42" s="7" t="s">
         <v>208</v>
@@ -4902,7 +4902,7 @@
         <v>67</v>
       </c>
       <c r="V42" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="X42" s="7">
         <v>1902</v>
@@ -4911,7 +4911,7 @@
         <v>211</v>
       </c>
       <c r="AF42" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for watanna
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE97220-FCFD-264B-9A3E-5FA44ACA4DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B5D0C0-87C2-C447-81DA-8BC62168ECD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="519">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1579,9 +1579,6 @@
     <t>Onoto Watanna with Facsimile Signature in Japanese</t>
   </si>
   <si>
-    <t>Onoto Watanna with Facsimile Signature in Japanese, [early twentieth century]</t>
-  </si>
-  <si>
     <t>Head and shoulders portrait of Jacob Wainwright, in three-quarters profile facing to his left.</t>
   </si>
   <si>
@@ -1598,6 +1595,9 @@
   </si>
   <si>
     <t>Onoto Watanna; Illustration of Numè, Koto, and Matsu, [late nineteenth century], 1899</t>
+  </si>
+  <si>
+    <t>Onoto Watanna with Facsimile Signature in Japanese, [early twentieth century], [early twentieth century]</t>
   </si>
 </sst>
 </file>
@@ -3168,9 +3168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3407,7 +3407,7 @@
         <v>136</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -4783,10 +4783,10 @@
         <v>491</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>514</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>515</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>502</v>
@@ -4819,7 +4819,7 @@
         <v>390</v>
       </c>
       <c r="AF40" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AG40" s="11"/>
     </row>
@@ -4828,10 +4828,10 @@
         <v>492</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>517</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>518</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>174</v>
@@ -4870,7 +4870,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>493</v>
       </c>
@@ -4878,10 +4878,13 @@
         <v>511</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>174</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>502</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
update mods for habib
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABD805F-C571-FF4D-94D7-8B3D28667798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB172663-704E-884D-AD6A-A685E1D83DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="531">
   <si>
     <t>liv_000017</t>
   </si>
@@ -196,9 +196,6 @@
     <t>[Central Africa]</t>
   </si>
   <si>
-    <t>[Said Bin Habeeb]</t>
-  </si>
-  <si>
     <t>[British] / [Bombay] Government</t>
   </si>
   <si>
@@ -1616,6 +1613,27 @@
   </si>
   <si>
     <t>Kasanga</t>
+  </si>
+  <si>
+    <t>liv_020041</t>
+  </si>
+  <si>
+    <t>Lists of Headmen in Manyema and Urundi (Excerpt from David Livingstone's Notebook, [March 1866-March 1870])</t>
+  </si>
+  <si>
+    <t>Lists of Headmen in Manyema and Urundi (Excerpt from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
+  </si>
+  <si>
+    <t>[Said Bin Habib]</t>
+  </si>
+  <si>
+    <t>[Said Bin Habib?]</t>
+  </si>
+  <si>
+    <t>[Unnamed Arab and African Informants?]</t>
+  </si>
+  <si>
+    <t>4 July 1869, [c.1869]</t>
   </si>
 </sst>
 </file>
@@ -2084,11 +2102,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE30" sqref="AE30"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2111,100 +2129,100 @@
   <sheetData>
     <row r="1" spans="1:32" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="Q1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="AE1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -2212,16 +2230,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -2256,7 +2274,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -2291,7 +2309,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -2326,7 +2344,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -2361,7 +2379,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -2396,7 +2414,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -2434,7 +2452,7 @@
         <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>45</v>
@@ -2460,31 +2478,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="Q9" s="1">
         <v>15</v>
       </c>
       <c r="S9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -2492,10 +2510,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
@@ -2504,19 +2522,19 @@
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q10" s="1">
         <v>18</v>
       </c>
       <c r="S10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -2524,31 +2542,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="Q11" s="1">
         <v>15</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T11" s="1">
         <v>1845</v>
@@ -2559,34 +2577,34 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -2594,34 +2612,34 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="34" x14ac:dyDescent="0.2">
@@ -2629,31 +2647,31 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="S14" s="1">
         <v>10</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="68" x14ac:dyDescent="0.2">
@@ -2661,28 +2679,28 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="R15" s="1">
         <v>93</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T15" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="85" x14ac:dyDescent="0.2">
@@ -2690,31 +2708,31 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>23</v>
@@ -2722,47 +2740,47 @@
     </row>
     <row r="17" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="4"/>
       <c r="V17" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Z17" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA17" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AA17" s="4" t="s">
+      <c r="AB17" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="AB17" s="4" t="s">
+      <c r="AC17" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="AE17" s="4">
         <v>1906</v>
@@ -2773,25 +2791,25 @@
     </row>
     <row r="18" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q18" s="1">
         <v>28</v>
@@ -2800,100 +2818,100 @@
         <v>6</v>
       </c>
       <c r="S18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="T18" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P20" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="S20" s="1">
         <v>3</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P21" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="Q21" s="1">
         <v>1</v>
@@ -2902,298 +2920,298 @@
         <v>82</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L22" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="M22" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="N22" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R23" s="1">
         <v>89</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="P24" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="T24" s="1" t="s">
         <v>438</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>443</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>448</v>
-      </c>
       <c r="G25" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S25" s="1">
         <v>5</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="P26" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="P26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>460</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L27" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>462</v>
-      </c>
       <c r="N27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>466</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L28" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="M28" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="N28" s="1" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="L29" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="30" spans="1:32" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>522</v>
-      </c>
       <c r="E30" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>16</v>
@@ -3202,16 +3220,57 @@
         <v>17</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L30" s="1">
         <v>807</v>
       </c>
       <c r="M30" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="N30" s="1" t="s">
+    </row>
+    <row r="31" spans="1:32" ht="102" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>524</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L31" s="1">
+        <v>807</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -3252,130 +3311,130 @@
   <sheetData>
     <row r="1" spans="1:33" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="AC1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="AD1" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="AF1" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF2" s="11" t="s">
         <v>305</v>
-      </c>
-      <c r="AF2" s="11" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="AF3" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="AF3" s="11" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>16</v>
@@ -3384,103 +3443,103 @@
         <v>17</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N4" s="7">
         <v>1874</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N5" s="7">
         <v>1874</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>16</v>
@@ -3489,36 +3548,36 @@
         <v>17</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M7" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O7" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="AF7" s="11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>16</v>
@@ -3527,1182 +3586,1182 @@
         <v>17</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="O8" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M9" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N9" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="O9" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AF10" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="AG10" s="11" t="s">
         <v>314</v>
-      </c>
-      <c r="AG10" s="11" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N11" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="O11" s="7" t="s">
-        <v>160</v>
-      </c>
       <c r="AF11" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>164</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="R13" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="R13" s="10" t="s">
+      <c r="S13" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="S13" s="7" t="s">
-        <v>198</v>
-      </c>
       <c r="U13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X13" s="7">
         <v>1904</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AF13" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="AG13" s="11" t="s">
         <v>318</v>
-      </c>
-      <c r="AG13" s="11" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q14" s="10" t="s">
+      <c r="S14" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="S14" s="7" t="s">
+      <c r="T14" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="T14" s="7" t="s">
+      <c r="U14" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="U14" s="7" t="s">
+      <c r="V14" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="W14" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>210</v>
       </c>
       <c r="X14" s="7">
         <v>1920</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF14" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q15" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="S15" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="T15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="V15" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="T15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="V15" s="7" t="s">
+      <c r="W15" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="W15" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="X15" s="7">
         <v>1912</v>
       </c>
       <c r="Y15" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q16" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q16" s="10" t="s">
+      <c r="S16" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="S16" s="7" t="s">
+      <c r="T16" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="T16" s="7" t="s">
+      <c r="V16" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>221</v>
       </c>
       <c r="X16" s="7">
         <v>1901</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>260</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q17" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="S17" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="S17" s="7" t="s">
+      <c r="T17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V17" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V17" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="X17" s="7">
         <v>1901</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF17" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>228</v>
-      </c>
       <c r="G18" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X18" s="7">
         <v>1904</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="D19" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="S19" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="S19" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="T19" s="7" t="s">
+      <c r="U19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V19" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="U19" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V19" s="7" t="s">
+      <c r="W19" s="7" t="s">
         <v>232</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>233</v>
       </c>
       <c r="X19" s="7">
         <v>1912</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>262</v>
-      </c>
       <c r="D20" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="G20" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q20" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="S20" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q20" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="S20" s="7" t="s">
+      <c r="T20" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="T20" s="7" t="s">
+      <c r="U20" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="W20" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="U20" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="W20" s="7" t="s">
+      <c r="X20" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="X20" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="Y20" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF20" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="AG20" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="AG20" s="11" t="s">
+      <c r="AH20" s="11" t="s">
         <v>326</v>
-      </c>
-      <c r="AH20" s="11" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="G21" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q21" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q21" s="10" t="s">
+      <c r="S21" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="S21" s="7" t="s">
+      <c r="T21" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="T21" s="7" t="s">
+      <c r="V21" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="V21" s="7" t="s">
-        <v>298</v>
       </c>
       <c r="X21" s="7">
         <v>1887</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF21" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q22" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="R22" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="R22" s="10" t="s">
+      <c r="S22" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="S22" s="7" t="s">
+      <c r="T22" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="V22" s="7" t="s">
         <v>302</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="V22" s="7" t="s">
-        <v>303</v>
       </c>
       <c r="X22" s="7">
         <v>1903</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF22" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>342</v>
-      </c>
       <c r="D23" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J23" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M23" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O23" s="7" t="s">
         <v>334</v>
       </c>
-      <c r="N23" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>335</v>
-      </c>
       <c r="AF23" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AG24" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>344</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M25" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O25" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="N25" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>346</v>
-      </c>
       <c r="AF25" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AG25" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>349</v>
-      </c>
       <c r="D26" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N26" s="7">
         <v>1911</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>353</v>
-      </c>
       <c r="D27" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AF27" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AG27" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N28" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="O28" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="O28" s="7" t="s">
-        <v>374</v>
-      </c>
       <c r="AF28" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>379</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>380</v>
-      </c>
       <c r="D29" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M29" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O29" s="7" t="s">
         <v>376</v>
       </c>
-      <c r="N29" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>377</v>
-      </c>
       <c r="AF29" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="AG29" s="7" t="s">
         <v>383</v>
-      </c>
-      <c r="AG29" s="7" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>392</v>
-      </c>
       <c r="D30" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q30" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="S30" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="S30" s="7" t="s">
+      <c r="T30" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="T30" s="7" t="s">
+      <c r="V30" s="7" t="s">
         <v>388</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>389</v>
       </c>
       <c r="X30" s="7">
         <v>1913</v>
       </c>
       <c r="Y30" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF30" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D31" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q31" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="S31" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q31" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="S31" s="7" t="s">
+      <c r="T31" s="7" t="s">
         <v>387</v>
       </c>
-      <c r="T31" s="7" t="s">
+      <c r="V31" s="7" t="s">
         <v>388</v>
-      </c>
-      <c r="V31" s="7" t="s">
-        <v>389</v>
       </c>
       <c r="X31" s="7">
         <v>1913</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AF31" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>396</v>
-      </c>
       <c r="D32" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S32" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="V32" s="7" t="s">
         <v>393</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="V32" s="7" t="s">
-        <v>394</v>
       </c>
       <c r="X32" s="7">
         <v>1913</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="D33" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q33" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="S33" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q33" s="10" t="s">
-        <v>386</v>
-      </c>
-      <c r="S33" s="7" t="s">
+      <c r="T33" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="T33" s="7" t="s">
+      <c r="V33" s="7" t="s">
         <v>398</v>
-      </c>
-      <c r="V33" s="7" t="s">
-        <v>399</v>
       </c>
       <c r="X33" s="7">
         <v>1913</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF33" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="34" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q34" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S34" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="T34" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="V34" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="T34" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>405</v>
       </c>
       <c r="X34" s="7">
         <v>1913</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF34" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>432</v>
-      </c>
       <c r="D35" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q35" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S35" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="V35" s="7" t="s">
         <v>404</v>
-      </c>
-      <c r="T35" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="V35" s="7" t="s">
-        <v>405</v>
       </c>
       <c r="X35" s="7">
         <v>1913</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF35" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="AG35" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="AG35" s="7" t="s">
+      <c r="AH35" s="7" t="s">
         <v>412</v>
-      </c>
-      <c r="AH35" s="7" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="36" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>392</v>
-      </c>
       <c r="D36" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S36" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="T36" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="V36" s="7" t="s">
         <v>407</v>
-      </c>
-      <c r="T36" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="V36" s="7" t="s">
-        <v>408</v>
       </c>
       <c r="X36" s="7">
         <v>1908</v>
@@ -4711,266 +4770,266 @@
         <v>2</v>
       </c>
       <c r="AF36" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>488</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>489</v>
-      </c>
       <c r="D37" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J37" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K37" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="L37" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="L37" s="7" t="s">
-        <v>479</v>
-      </c>
       <c r="M37" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N37" s="7">
         <v>1874</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AF37" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AG37" s="7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="38" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="D38" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>487</v>
-      </c>
       <c r="G38" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K38" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="L38" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>479</v>
-      </c>
       <c r="M38" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N38" s="7">
         <v>1874</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AF38" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AG38" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="39" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q39" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q39" s="10" t="s">
+      <c r="S39" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="S39" s="7" t="s">
+      <c r="T39" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="T39" s="7" t="s">
+      <c r="V39" s="7" t="s">
         <v>498</v>
-      </c>
-      <c r="V39" s="7" t="s">
-        <v>499</v>
       </c>
       <c r="X39" s="7">
         <v>1917</v>
       </c>
       <c r="Y39" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="AF39" s="7" t="s">
         <v>500</v>
-      </c>
-      <c r="AF39" s="7" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="40" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>513</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="S40" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="T40" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="U40" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="V40" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="X40" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y40" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="AF40" s="7" t="s">
         <v>514</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q40" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="U40" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="X40" s="7" t="s">
-        <v>506</v>
-      </c>
-      <c r="Y40" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="AF40" s="7" t="s">
-        <v>515</v>
       </c>
       <c r="AG40" s="11"/>
     </row>
     <row r="41" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>517</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q41" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="S41" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="S41" s="7" t="s">
+      <c r="T41" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="T41" s="7" t="s">
+      <c r="U41" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="V41" s="7" t="s">
         <v>504</v>
-      </c>
-      <c r="U41" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="V41" s="7" t="s">
-        <v>505</v>
       </c>
       <c r="X41" s="7">
         <v>1899</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF41" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="42" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="S42" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V42" s="7" t="s">
         <v>508</v>
-      </c>
-      <c r="T42" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="U42" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="V42" s="7" t="s">
-        <v>509</v>
       </c>
       <c r="X42" s="7">
         <v>1902</v>
       </c>
       <c r="Y42" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AF42" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -5000,31 +5059,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" t="str">
         <f>Artifacts!D28</f>
         <v>Anonymous</v>
       </c>
       <c r="C1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E1" t="str">
         <f>Artifacts!B28</f>
         <v>Pandita Ramabai Sarasvati</v>
       </c>
       <c r="F1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G1" t="str">
         <f>Artifacts!N28</f>
         <v>[Late nineteenth century]</v>
       </c>
       <c r="H1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I1" s="16" t="str">
         <f>A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1</f>
@@ -5033,31 +5092,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B2" t="str">
         <f>Artifacts!D29</f>
         <v>J. Paul</v>
       </c>
       <c r="C2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E2" t="str">
         <f>Artifacts!B29</f>
         <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
       </c>
       <c r="F2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G2" t="str">
         <f>Artifacts!N29</f>
         <v>[Early twentieth century]</v>
       </c>
       <c r="H2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I2" s="16" t="str">
         <f t="shared" ref="I2:I9" si="0">A2&amp;B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2</f>
@@ -5066,30 +5125,30 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B3" t="str">
         <f>Artifacts!D30</f>
         <v>Anonymous</v>
       </c>
       <c r="C3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E3" t="str">
         <f>Artifacts!B30</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5098,30 +5157,30 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B4" t="str">
         <f>Artifacts!D31</f>
         <v>Johnson, E. Pauline, 1861-1913</v>
       </c>
       <c r="C4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E4" t="str">
         <f>Artifacts!B31</f>
         <v>“And He Said ‘Fight On’” (Manuscript Facsimile)</v>
       </c>
       <c r="F4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5130,30 +5189,30 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B5" t="str">
         <f>Artifacts!D32</f>
         <v>Anonymous</v>
       </c>
       <c r="C5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E5" t="str">
         <f>Artifacts!B32</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5162,30 +5221,30 @@
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B6" t="str">
         <f>Artifacts!D33</f>
         <v>Anonymous</v>
       </c>
       <c r="C6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E6" t="str">
         <f>Artifacts!B33</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I6" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5194,30 +5253,30 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B7" t="str">
         <f>Artifacts!D34</f>
         <v>Anonymous</v>
       </c>
       <c r="C7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E7" t="str">
         <f>Artifacts!B34</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G7" s="7">
         <v>1904</v>
       </c>
       <c r="H7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5226,30 +5285,30 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B8" t="str">
         <f>Artifacts!D35</f>
         <v>Anonymous</v>
       </c>
       <c r="C8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E8" t="str">
         <f>Artifacts!B35</f>
         <v xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock” </v>
       </c>
       <c r="F8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5258,30 +5317,30 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B9" t="str">
         <f>Artifacts!D36</f>
         <v>Anonymous</v>
       </c>
       <c r="C9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E9" t="str">
         <f>Artifacts!B36</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I9" s="16" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
update mods for fables
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB172663-704E-884D-AD6A-A685E1D83DB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87B9FD3-D8A3-924E-8052-B9204E391F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="535">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1618,12 +1618,6 @@
     <t>liv_020041</t>
   </si>
   <si>
-    <t>Lists of Headmen in Manyema and Urundi (Excerpt from David Livingstone's Notebook, [March 1866-March 1870])</t>
-  </si>
-  <si>
-    <t>Lists of Headmen in Manyema and Urundi (Excerpt from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
-  </si>
-  <si>
     <t>[Said Bin Habib]</t>
   </si>
   <si>
@@ -1634,6 +1628,24 @@
   </si>
   <si>
     <t>4 July 1869, [c.1869]</t>
+  </si>
+  <si>
+    <t>Central African Fables (Excerpts from David Livingstone's Notebook, [March 1866-March 1870])</t>
+  </si>
+  <si>
+    <t>Central African Fables (Excerpts from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
+  </si>
+  <si>
+    <t>Lists of Headmen in Manyema and Urundi (Excerpts from David Livingstone's Notebook, [March 1866-March 1870])</t>
+  </si>
+  <si>
+    <t>Lists of Headmen in Manyema and Urundi (Excerpts from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
+  </si>
+  <si>
+    <t>[Unnamed African Informants]</t>
+  </si>
+  <si>
+    <t>[c.1868-1870]</t>
   </si>
 </sst>
 </file>
@@ -2102,11 +2114,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF31"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,7 +2499,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>433</v>
@@ -3237,16 +3249,16 @@
         <v>524</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>526</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>528</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>180</v>
@@ -3267,9 +3279,47 @@
         <v>807</v>
       </c>
       <c r="M31" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="D32" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L32" s="1">
+        <v>807</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update mods for wainwright
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5320396-33C0-9A4C-B75D-FA55CC43E7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C32155-3C2D-A247-9FE0-7513ED3E2250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="542">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1664,6 +1664,9 @@
   </si>
   <si>
     <t>Lists of Headmen in Manyema and Urundi (Excerpts from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869; [c.1869]</t>
+  </si>
+  <si>
+    <t>Head and shoulders portrait of Jacob Wainwright, in three-quarters profile facing to his right.</t>
   </si>
 </sst>
 </file>
@@ -2134,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -3387,11 +3390,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH42"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3631,18 +3634,18 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>268</v>
+        <v>101</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>173</v>
+        <v>102</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>120</v>
@@ -3651,13 +3654,10 @@
         <v>16</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>134</v>
+        <v>34</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>93</v>
@@ -3666,18 +3666,18 @@
         <v>135</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>97</v>
+        <v>269</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>98</v>
+        <v>268</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>173</v>
@@ -3694,31 +3694,31 @@
       <c r="L8" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>99</v>
+      <c r="M8" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>135</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" ht="119" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>88</v>
+        <v>173</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>120</v>
@@ -3727,36 +3727,36 @@
         <v>16</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>92</v>
+        <v>95</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>135</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>173</v>
+        <v>88</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>120</v>
@@ -3768,33 +3768,30 @@
         <v>66</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>160</v>
+        <v>86</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>135</v>
       </c>
       <c r="AF10" s="11" t="s">
-        <v>313</v>
-      </c>
-      <c r="AG10" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>252</v>
+        <v>98</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>173</v>
@@ -3812,27 +3809,30 @@
         <v>155</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" ht="102" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+      <c r="AG11" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>173</v>
@@ -3850,27 +3850,27 @@
         <v>155</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" ht="136" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>173</v>
@@ -3878,46 +3878,37 @@
       <c r="G13" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="R13" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="U13" s="7" t="s">
+      <c r="J13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="W13" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="X13" s="7">
-        <v>1904</v>
-      </c>
-      <c r="Y13" s="7" t="s">
-        <v>198</v>
+      <c r="L13" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="AF13" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="AG13" s="11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>173</v>
@@ -3929,42 +3920,42 @@
         <v>119</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>196</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V14" s="7" t="s">
-        <v>208</v>
+        <v>66</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="X14" s="7">
-        <v>1920</v>
+        <v>1904</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="AF14" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
+      </c>
+      <c r="AG14" s="11" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>173</v>
@@ -3976,42 +3967,42 @@
         <v>119</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>66</v>
+        <v>206</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>207</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="X15" s="7">
-        <v>1912</v>
+        <v>1920</v>
       </c>
       <c r="Y15" s="7" t="s">
         <v>210</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>215</v>
+        <v>251</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>173</v>
@@ -4023,39 +4014,45 @@
         <v>119</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>219</v>
+        <v>66</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="V16" s="7" t="s">
-        <v>220</v>
+        <v>213</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>214</v>
       </c>
       <c r="X16" s="7">
-        <v>1901</v>
+        <v>1912</v>
       </c>
       <c r="Y16" s="7" t="s">
         <v>210</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" ht="85" x14ac:dyDescent="0.2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>258</v>
+        <v>215</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>259</v>
+        <v>216</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>247</v>
+        <v>173</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>120</v>
@@ -4064,16 +4061,16 @@
         <v>119</v>
       </c>
       <c r="Q17" s="10" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="S17" s="7" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>66</v>
+        <v>219</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="X17" s="7">
         <v>1901</v>
@@ -4082,21 +4079,21 @@
         <v>210</v>
       </c>
       <c r="AF17" s="11" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>226</v>
+        <v>258</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>120</v>
@@ -4105,39 +4102,39 @@
         <v>119</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="T18" s="7" t="s">
         <v>66</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="X18" s="7">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="Y18" s="7" t="s">
         <v>210</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>120</v>
@@ -4145,49 +4142,40 @@
       <c r="H19" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="Q19" s="7" t="s">
+      <c r="Q19" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="X19" s="7">
+        <v>1904</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF19" s="11" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="U19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="V19" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="X19" s="7">
-        <v>1912</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" ht="153" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>120</v>
@@ -4195,52 +4183,49 @@
       <c r="H20" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="Q20" s="13" t="s">
+      <c r="Q20" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V20" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="W20" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="X20" s="7">
+        <v>1912</v>
+      </c>
+      <c r="Y20" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="153" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="S20" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="X20" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y20" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="AF20" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="AG20" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="AH20" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>293</v>
+      <c r="E21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>120</v>
@@ -4248,40 +4233,52 @@
       <c r="H21" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="Q21" s="10" t="s">
-        <v>294</v>
+      <c r="Q21" s="13" t="s">
+        <v>234</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>295</v>
+        <v>237</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>296</v>
+        <v>238</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="X21" s="7">
-        <v>1887</v>
+        <v>264</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>210</v>
+        <v>389</v>
       </c>
       <c r="AF21" s="11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+      <c r="AG21" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="AH21" s="11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>173</v>
+        <v>293</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>120</v>
@@ -4292,20 +4289,17 @@
       <c r="Q22" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="R22" s="10" t="s">
-        <v>300</v>
-      </c>
       <c r="S22" s="7" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>244</v>
+        <v>296</v>
       </c>
       <c r="V22" s="7" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="X22" s="7">
-        <v>1903</v>
+        <v>1887</v>
       </c>
       <c r="Y22" s="7" t="s">
         <v>210</v>
@@ -4314,15 +4308,15 @@
         <v>327</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="153" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>173</v>
@@ -4330,43 +4324,46 @@
       <c r="G23" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="J23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="M23" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="AF23" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="AG23" s="7" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="H23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="X23" s="7">
+        <v>1903</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF23" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>337</v>
+        <v>173</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>120</v>
@@ -4381,7 +4378,7 @@
         <v>155</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N24" s="7" t="s">
         <v>335</v>
@@ -4390,24 +4387,24 @@
         <v>334</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="AG24" s="11" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" ht="136" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+      <c r="AG24" s="7" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>173</v>
+        <v>337</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>120</v>
@@ -4422,30 +4419,30 @@
         <v>155</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>335</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="AF25" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="AG25" s="7" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="26" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+      <c r="AG25" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>173</v>
@@ -4463,33 +4460,33 @@
         <v>155</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="N26" s="7">
-        <v>1911</v>
+        <v>344</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>335</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>345</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>350</v>
+        <v>173</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>120</v>
@@ -4504,33 +4501,33 @@
         <v>155</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>335</v>
+        <v>346</v>
+      </c>
+      <c r="N27" s="7">
+        <v>1911</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>334</v>
-      </c>
-      <c r="AF27" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="AG27" s="11" t="s">
-        <v>353</v>
+        <v>345</v>
+      </c>
+      <c r="AF27" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG27" s="7" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>363</v>
+        <v>332</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>298</v>
+        <v>351</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>173</v>
+        <v>350</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>120</v>
@@ -4545,30 +4542,33 @@
         <v>155</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>372</v>
+        <v>335</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="AF28" s="14" t="s">
-        <v>381</v>
+        <v>334</v>
+      </c>
+      <c r="AF28" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG28" s="11" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>378</v>
+        <v>298</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>377</v>
+        <v>173</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>120</v>
@@ -4583,78 +4583,75 @@
         <v>155</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="AF29" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="AG29" s="7" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+      <c r="AF29" s="14" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>173</v>
+        <v>377</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q30" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>388</v>
-      </c>
-      <c r="X30" s="7">
-        <v>1913</v>
-      </c>
-      <c r="Y30" s="7" t="s">
-        <v>389</v>
+      <c r="J30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>376</v>
       </c>
       <c r="AF30" s="7" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+        <v>382</v>
+      </c>
+      <c r="AG30" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>428</v>
+        <v>390</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>427</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>385</v>
+        <v>391</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="Q31" s="10" t="s">
         <v>385</v>
       </c>
@@ -4674,50 +4671,53 @@
         <v>389</v>
       </c>
       <c r="AF31" s="7" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>394</v>
+        <v>428</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>173</v>
+        <v>427</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>385</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>120</v>
       </c>
+      <c r="H32" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="Q32" s="10" t="s">
         <v>385</v>
       </c>
       <c r="S32" s="7" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="T32" s="7" t="s">
         <v>387</v>
       </c>
       <c r="V32" s="7" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="X32" s="7">
         <v>1913</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>210</v>
+        <v>389</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>400</v>
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>394</v>
@@ -4735,13 +4735,13 @@
         <v>385</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="X33" s="7">
         <v>1913</v>
@@ -4750,18 +4750,18 @@
         <v>210</v>
       </c>
       <c r="AF33" s="7" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="34" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>173</v>
@@ -4773,13 +4773,13 @@
         <v>385</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="V34" s="7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="X34" s="7">
         <v>1913</v>
@@ -4788,28 +4788,22 @@
         <v>210</v>
       </c>
       <c r="AF34" s="7" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="35" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="35" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>431</v>
+        <v>405</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>409</v>
-      </c>
       <c r="G35" s="7" t="s">
         <v>120</v>
       </c>
@@ -4829,31 +4823,31 @@
         <v>1913</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>413</v>
+        <v>210</v>
       </c>
       <c r="AF35" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="AG35" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="AH35" s="7" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="36" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>390</v>
+        <v>430</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>391</v>
+        <v>431</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>173</v>
       </c>
+      <c r="E36" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>409</v>
+      </c>
       <c r="G36" s="7" t="s">
         <v>120</v>
       </c>
@@ -4861,74 +4855,77 @@
         <v>385</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="V36" s="7" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="X36" s="7">
-        <v>1908</v>
-      </c>
-      <c r="Y36" s="7">
-        <v>2</v>
+        <v>1913</v>
+      </c>
+      <c r="Y36" s="7" t="s">
+        <v>413</v>
       </c>
       <c r="AF36" s="7" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="37" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+      <c r="AG36" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="AH36" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>474</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>487</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>488</v>
+        <v>371</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>391</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>486</v>
+        <v>173</v>
       </c>
       <c r="G37" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="J37" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K37" s="7" t="s">
-        <v>477</v>
-      </c>
-      <c r="L37" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="M37" s="7" t="s">
-        <v>480</v>
-      </c>
-      <c r="N37" s="7">
-        <v>1874</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>479</v>
-      </c>
-      <c r="AF37" s="11" t="s">
-        <v>312</v>
-      </c>
-      <c r="AG37" s="7" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="38" spans="1:34" ht="136" x14ac:dyDescent="0.2">
+      <c r="Q37" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="T37" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="X37" s="7">
+        <v>1908</v>
+      </c>
+      <c r="Y37" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF37" s="7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>484</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>485</v>
+        <v>474</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>488</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>486</v>
@@ -4946,7 +4943,7 @@
         <v>478</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="N38" s="7">
         <v>1874</v>
@@ -4954,114 +4951,107 @@
       <c r="O38" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="AF38" s="7" t="s">
-        <v>476</v>
+      <c r="AF38" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="AG38" s="7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="39" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>173</v>
+        <v>486</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Q39" s="10" t="s">
+      <c r="J39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="M39" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="N39" s="7">
+        <v>1874</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="AF39" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="AG39" s="7" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="40" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q40" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="S39" s="7" t="s">
+      <c r="S40" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="T39" s="7" t="s">
+      <c r="T40" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="V39" s="7" t="s">
+      <c r="V40" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="X39" s="7">
+      <c r="X40" s="7">
         <v>1917</v>
       </c>
-      <c r="Y39" s="7" t="s">
+      <c r="Y40" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="AF39" s="7" t="s">
+      <c r="AF40" s="7" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="40" spans="1:34" ht="85" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>490</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>512</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>513</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q40" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="U40" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="X40" s="7" t="s">
-        <v>505</v>
-      </c>
-      <c r="Y40" s="7" t="s">
-        <v>389</v>
-      </c>
-      <c r="AF40" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="AG40" s="11"/>
     </row>
     <row r="41" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>173</v>
+        <v>501</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>119</v>
@@ -5081,31 +5071,32 @@
       <c r="V41" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="X41" s="7">
-        <v>1899</v>
+      <c r="X41" s="7" t="s">
+        <v>505</v>
       </c>
       <c r="Y41" s="7" t="s">
-        <v>210</v>
+        <v>389</v>
       </c>
       <c r="AF41" s="7" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="42" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+        <v>514</v>
+      </c>
+      <c r="AG41" s="11"/>
+    </row>
+    <row r="42" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>173</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>501</v>
+        <v>173</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>120</v>
@@ -5117,30 +5108,77 @@
         <v>501</v>
       </c>
       <c r="S42" s="7" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="T42" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="U42" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="U42" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="V42" s="7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="X42" s="7">
-        <v>1902</v>
+        <v>1899</v>
       </c>
       <c r="Y42" s="7" t="s">
         <v>210</v>
       </c>
       <c r="AF42" s="7" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="T43" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="X43" s="7">
+        <v>1902</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AF43" s="7" t="s">
         <v>509</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH35">
-    <sortCondition ref="A2:A35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH36">
+    <sortCondition ref="A2:A36"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5168,7 +5206,7 @@
         <v>417</v>
       </c>
       <c r="B1" t="str">
-        <f>Artifacts!D28</f>
+        <f>Artifacts!D29</f>
         <v>Anonymous</v>
       </c>
       <c r="C1" t="s">
@@ -5178,14 +5216,14 @@
         <v>414</v>
       </c>
       <c r="E1" t="str">
-        <f>Artifacts!B28</f>
+        <f>Artifacts!B29</f>
         <v>Pandita Ramabai Sarasvati</v>
       </c>
       <c r="F1" t="s">
         <v>416</v>
       </c>
       <c r="G1" t="str">
-        <f>Artifacts!N28</f>
+        <f>Artifacts!N29</f>
         <v>[Late nineteenth century]</v>
       </c>
       <c r="H1" t="s">
@@ -5201,7 +5239,7 @@
         <v>417</v>
       </c>
       <c r="B2" t="str">
-        <f>Artifacts!D29</f>
+        <f>Artifacts!D30</f>
         <v>J. Paul</v>
       </c>
       <c r="C2" t="s">
@@ -5211,14 +5249,14 @@
         <v>419</v>
       </c>
       <c r="E2" t="str">
-        <f>Artifacts!B29</f>
+        <f>Artifacts!B30</f>
         <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
       </c>
       <c r="F2" t="s">
         <v>416</v>
       </c>
       <c r="G2" t="str">
-        <f>Artifacts!N29</f>
+        <f>Artifacts!N30</f>
         <v>[Early twentieth century]</v>
       </c>
       <c r="H2" t="s">
@@ -5234,7 +5272,7 @@
         <v>417</v>
       </c>
       <c r="B3" t="str">
-        <f>Artifacts!D30</f>
+        <f>Artifacts!D31</f>
         <v>Anonymous</v>
       </c>
       <c r="C3" t="s">
@@ -5244,7 +5282,7 @@
         <v>420</v>
       </c>
       <c r="E3" t="str">
-        <f>Artifacts!B30</f>
+        <f>Artifacts!B31</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F3" t="s">
@@ -5266,7 +5304,7 @@
         <v>417</v>
       </c>
       <c r="B4" t="str">
-        <f>Artifacts!D31</f>
+        <f>Artifacts!D32</f>
         <v>Johnson, E. Pauline, 1861-1913</v>
       </c>
       <c r="C4" t="s">
@@ -5276,7 +5314,7 @@
         <v>421</v>
       </c>
       <c r="E4" t="str">
-        <f>Artifacts!B31</f>
+        <f>Artifacts!B32</f>
         <v>“And He Said ‘Fight On’” (Manuscript Facsimile)</v>
       </c>
       <c r="F4" t="s">
@@ -5298,7 +5336,7 @@
         <v>417</v>
       </c>
       <c r="B5" t="str">
-        <f>Artifacts!D32</f>
+        <f>Artifacts!D33</f>
         <v>Anonymous</v>
       </c>
       <c r="C5" t="s">
@@ -5308,7 +5346,7 @@
         <v>422</v>
       </c>
       <c r="E5" t="str">
-        <f>Artifacts!B32</f>
+        <f>Artifacts!B33</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F5" t="s">
@@ -5330,7 +5368,7 @@
         <v>417</v>
       </c>
       <c r="B6" t="str">
-        <f>Artifacts!D33</f>
+        <f>Artifacts!D34</f>
         <v>Anonymous</v>
       </c>
       <c r="C6" t="s">
@@ -5340,7 +5378,7 @@
         <v>423</v>
       </c>
       <c r="E6" t="str">
-        <f>Artifacts!B33</f>
+        <f>Artifacts!B34</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F6" t="s">
@@ -5362,7 +5400,7 @@
         <v>417</v>
       </c>
       <c r="B7" t="str">
-        <f>Artifacts!D34</f>
+        <f>Artifacts!D35</f>
         <v>Anonymous</v>
       </c>
       <c r="C7" t="s">
@@ -5372,7 +5410,7 @@
         <v>424</v>
       </c>
       <c r="E7" t="str">
-        <f>Artifacts!B34</f>
+        <f>Artifacts!B35</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F7" t="s">
@@ -5394,7 +5432,7 @@
         <v>417</v>
       </c>
       <c r="B8" t="str">
-        <f>Artifacts!D35</f>
+        <f>Artifacts!D36</f>
         <v>Anonymous</v>
       </c>
       <c r="C8" t="s">
@@ -5404,7 +5442,7 @@
         <v>425</v>
       </c>
       <c r="E8" t="str">
-        <f>Artifacts!B35</f>
+        <f>Artifacts!B36</f>
         <v xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock” </v>
       </c>
       <c r="F8" t="s">
@@ -5426,7 +5464,7 @@
         <v>417</v>
       </c>
       <c r="B9" t="str">
-        <f>Artifacts!D36</f>
+        <f>Artifacts!D37</f>
         <v>Anonymous</v>
       </c>
       <c r="C9" t="s">
@@ -5436,7 +5474,7 @@
         <v>426</v>
       </c>
       <c r="E9" t="str">
-        <f>Artifacts!B36</f>
+        <f>Artifacts!B37</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F9" t="s">

</xml_diff>

<commit_message>
update mods for new chuma/susi
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C32155-3C2D-A247-9FE0-7513ED3E2250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146DDB0B-777D-3C4D-98BC-DB6F975224E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="546">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1667,6 +1667,18 @@
   </si>
   <si>
     <t>Head and shoulders portrait of Jacob Wainwright, in three-quarters profile facing to his right.</t>
+  </si>
+  <si>
+    <t>liv_012001</t>
+  </si>
+  <si>
+    <t>Agnes Livingstone, Thomas Livingstone, Abdullah Susi, James Chuma, and Horace Waller with David Livingstone’s manuscripts</t>
+  </si>
+  <si>
+    <t>“Agnes and Thomas Livingstone (Daughter and Son of David Livingstone), Abdullah Susi, James Chuma, and Rev. Horace Waller at Newstead Abbey, Nottingham, Discussing the Journals, Maps, and Plans Made by the Late David Livingstone”</t>
+  </si>
+  <si>
+    <t>“Agnes and Thomas Livingstone (Daughter and Son of David Livingstone), Abdullah Susi, James Chuma, and Rev. Horace Waller at Newstead Abbey, Nottingham, Discussing the Journals, Maps, and Plans Made by the Late David Livingstone,” 1874</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2150,7 @@
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -3390,11 +3402,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH43"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AF7" sqref="AF7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5174,6 +5186,47 @@
       </c>
       <c r="AF43" s="7" t="s">
         <v>509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="187" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="N44" s="7">
+        <v>1874</v>
+      </c>
+      <c r="O44" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="AF44" s="7" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for nosutu
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD60C0D0-8A85-7B4D-910C-4796D0124BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2B8D7D-8082-2D4A-B911-2C38B109F010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="567">
   <si>
     <t>liv_000017</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Saleh Bin Osman</t>
   </si>
   <si>
-    <t>[Glave, Edward J., 1863-1895]</t>
-  </si>
-  <si>
     <t>United States</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>MacQueen, James, 1778-1870</t>
   </si>
   <si>
-    <t>[Lief Ben Saeid]</t>
-  </si>
-  <si>
     <t>[Wogga, Thomas]</t>
   </si>
   <si>
@@ -283,9 +277,6 @@
     <t>Jacob Wainwright</t>
   </si>
   <si>
-    <t>[Wainwright, Jacob, c.1851/2-1892]</t>
-  </si>
-  <si>
     <t>Wesleyan Juvenile Offering: A Miscellany of Missionary Info</t>
   </si>
   <si>
@@ -1618,15 +1609,6 @@
     <t>liv_020041</t>
   </si>
   <si>
-    <t>[Said Bin Habib]</t>
-  </si>
-  <si>
-    <t>[Said Bin Habib?]</t>
-  </si>
-  <si>
-    <t>[Unnamed Arab and African Informants?]</t>
-  </si>
-  <si>
     <t>4 July 1869, [c.1869]</t>
   </si>
   <si>
@@ -1639,9 +1621,6 @@
     <t>Lists of Headmen in Manyema and Urundi (Excerpts from David Livingstone's Notebook, [March 1866-March 1870])</t>
   </si>
   <si>
-    <t>[Unnamed African Informants]</t>
-  </si>
-  <si>
     <t>[c.1868-1870]</t>
   </si>
   <si>
@@ -1721,6 +1700,48 @@
   </si>
   <si>
     <t>liv_099999</t>
+  </si>
+  <si>
+    <t>liv_020042</t>
+  </si>
+  <si>
+    <t>liv_020043</t>
+  </si>
+  <si>
+    <t>“Nosutu's Letter”</t>
+  </si>
+  <si>
+    <t>Missionary Record of the United Presbyterian Church</t>
+  </si>
+  <si>
+    <t>“Nosutu's Letter,” 2 March 1874</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 March 1874; October 1873 </t>
+  </si>
+  <si>
+    <t>New Series, 5</t>
+  </si>
+  <si>
+    <t>Glave, Edward J., 1863-1895</t>
+  </si>
+  <si>
+    <t>Lief Ben Saeid</t>
+  </si>
+  <si>
+    <t>Said Bin Habib[?]</t>
+  </si>
+  <si>
+    <t>Unnamed Arab and African Informants[?]</t>
+  </si>
+  <si>
+    <t>Unnamed African Informants</t>
+  </si>
+  <si>
+    <t>Tause</t>
+  </si>
+  <si>
+    <t>Cumming, John</t>
   </si>
 </sst>
 </file>
@@ -2189,11 +2210,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF33"/>
+  <dimension ref="A1:AF34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,100 +2237,100 @@
   <sheetData>
     <row r="1" spans="1:32" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="Y1" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="51" x14ac:dyDescent="0.2">
@@ -2317,16 +2338,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>16</v>
@@ -2361,7 +2382,7 @@
         <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>16</v>
@@ -2396,7 +2417,7 @@
         <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -2431,7 +2452,7 @@
         <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>16</v>
@@ -2466,7 +2487,7 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -2501,7 +2522,7 @@
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -2522,824 +2543,821 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>176</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>48</v>
+        <v>179</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="153" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>15</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>141</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>143</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>18</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="J10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
+        <v>529</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="Q11" s="1">
         <v>15</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="T11" s="1">
-        <v>1845</v>
+        <v>52</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>18</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>15</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T13" s="1">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="L14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S14" s="1">
-        <v>10</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S16" s="1">
+        <v>10</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R17" s="1">
+        <v>93</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>28</v>
+      </c>
+      <c r="R19" s="1">
+        <v>6</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="R15" s="1">
-        <v>93</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="T15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="V17" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="X17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z17" s="4" t="s">
+      <c r="G20" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="V20" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC20" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="AA17" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="AB17" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="AC17" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="AE17" s="4">
+      <c r="AE20" s="4">
         <v>1906</v>
       </c>
-      <c r="AF17" s="4">
+      <c r="AF20" s="4">
         <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>28</v>
-      </c>
-      <c r="R18" s="1">
-        <v>6</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="68" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="S20" s="1">
-        <v>3</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>1</v>
-      </c>
-      <c r="R21" s="1">
-        <v>82</v>
+        <v>263</v>
+      </c>
+      <c r="S21" s="1">
+        <v>3</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>435</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>276</v>
+        <v>170</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>282</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>279</v>
+        <v>430</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R22" s="1">
+        <v>89</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>280</v>
+        <v>452</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>283</v>
+        <v>455</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>284</v>
+        <v>454</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>285</v>
+        <v>456</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="R23" s="1">
-        <v>89</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" ht="51" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>437</v>
+        <v>459</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>443</v>
+        <v>170</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>267</v>
+        <v>178</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>445</v>
+        <v>461</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>446</v>
+        <v>460</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>447</v>
+        <v>448</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>462</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="S25" s="1">
-        <v>5</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>448</v>
+        <v>115</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>449</v>
+        <v>267</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>450</v>
+        <v>278</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>451</v>
+        <v>268</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>452</v>
+        <v>269</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>82</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
     </row>
     <row r="27" spans="1:32" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>455</v>
+        <v>270</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>458</v>
+        <v>271</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>457</v>
+        <v>272</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>459</v>
+        <v>273</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>461</v>
+        <v>274</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>275</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>454</v>
+        <v>429</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>464</v>
+        <v>433</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>463</v>
+        <v>434</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>181</v>
+        <v>440</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>465</v>
+        <v>264</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="M28" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S29" s="1">
+        <v>5</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="N28" s="1" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" ht="68" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" ht="102" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L30" s="1">
-        <v>807</v>
+        <v>65</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>522</v>
+        <v>469</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" ht="119" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" ht="102" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>540</v>
+        <v>517</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>16</v>
@@ -3348,36 +3366,39 @@
         <v>17</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L31" s="1">
         <v>807</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="85" x14ac:dyDescent="0.2">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>532</v>
+        <v>563</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>180</v>
+        <v>562</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>16</v>
@@ -3386,69 +3407,111 @@
         <v>17</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L32" s="1">
         <v>807</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>534</v>
+        <v>553</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>539</v>
+        <v>524</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>536</v>
+        <v>564</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>537</v>
+        <v>92</v>
+      </c>
+      <c r="L33" s="1">
+        <v>807</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="R34" s="1">
+        <v>44</v>
+      </c>
+      <c r="S34" s="1">
+        <v>53</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF33">
+    <sortCondition ref="A2:A33"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH46"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3474,130 +3537,130 @@
   <sheetData>
     <row r="1" spans="1:33" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="E1" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="AC1" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AD1" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="AF1" s="6" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AF3" s="11" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>110</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>16</v>
@@ -3606,103 +3669,103 @@
         <v>17</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="N4" s="7">
         <v>1874</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AF4" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N5" s="7">
         <v>1874</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF5" s="11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF6" s="11" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J7" s="7" t="s">
         <v>16</v>
@@ -3714,30 +3777,30 @@
         <v>34</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>16</v>
@@ -3746,36 +3809,36 @@
         <v>17</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF8" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:33" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>16</v>
@@ -3784,1182 +3847,1182 @@
         <v>17</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF9" s="11" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:33" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF10" s="11" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="AF11" s="11" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AG11" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:33" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L12" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="N12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="M12" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>158</v>
-      </c>
       <c r="O12" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:33" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="O13" s="7" t="s">
-        <v>167</v>
-      </c>
       <c r="AF13" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="W14" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="X14" s="7">
         <v>1904</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AF14" s="11" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="AG14" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="T15" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q15" s="10" t="s">
+      <c r="U15" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="V15" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="T15" s="7" t="s">
+      <c r="W15" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V15" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="W15" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="X15" s="7">
         <v>1920</v>
       </c>
       <c r="Y15" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF15" s="11" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:33" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q16" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="W16" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="U16" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V16" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="X16" s="7">
         <v>1912</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="S17" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="T17" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q17" s="10" t="s">
+      <c r="V17" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="V17" s="7" t="s">
-        <v>220</v>
       </c>
       <c r="X17" s="7">
         <v>1901</v>
       </c>
       <c r="Y17" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF17" s="11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q18" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="X18" s="7">
         <v>1901</v>
       </c>
       <c r="Y18" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q19" s="10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="X19" s="7">
         <v>1904</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF19" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="T20" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="U20" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="V20" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q20" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="S20" s="7" t="s">
+      <c r="W20" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="T20" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="U20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="V20" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="X20" s="7">
         <v>1912</v>
       </c>
       <c r="Y20" s="7" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="T21" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="V21" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="W21" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="S21" s="7" t="s">
+      <c r="X21" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="T21" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="U21" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V21" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="W21" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="X21" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="Y21" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AF21" s="11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="AG21" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="AH21" s="11" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="D22" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q22" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="S22" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="T22" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q22" s="10" t="s">
+      <c r="V22" s="7" t="s">
         <v>294</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="V22" s="7" t="s">
-        <v>297</v>
       </c>
       <c r="X22" s="7">
         <v>1887</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF22" s="11" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="S23" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="T23" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="V23" s="7" t="s">
         <v>299</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q23" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="R23" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="S23" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="V23" s="7" t="s">
-        <v>302</v>
       </c>
       <c r="X23" s="7">
         <v>1903</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF23" s="11" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J24" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AF24" s="7" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="AG24" s="7" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J25" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K25" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M25" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O25" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AF25" s="7" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="AG25" s="11" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J26" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AF26" s="7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="AG26" s="7" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J27" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="N27" s="7">
         <v>1911</v>
       </c>
       <c r="O27" s="7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AF27" s="7" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="AG27" s="7" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K28" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AF28" s="11" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="AG28" s="11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AF29" s="14" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J30" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O30" s="7" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="AF30" s="7" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="AG30" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q31" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T31" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="V31" s="7" t="s">
         <v>385</v>
-      </c>
-      <c r="S31" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="T31" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="V31" s="7" t="s">
-        <v>388</v>
       </c>
       <c r="X31" s="7">
         <v>1913</v>
       </c>
       <c r="Y31" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AF31" s="7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q32" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="S32" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="V32" s="7" t="s">
         <v>385</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q32" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="T32" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="V32" s="7" t="s">
-        <v>388</v>
       </c>
       <c r="X32" s="7">
         <v>1913</v>
       </c>
       <c r="Y32" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AF32" s="7" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="33" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q33" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="X33" s="7">
         <v>1913</v>
       </c>
       <c r="Y33" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF33" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q34" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="T34" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="V34" s="7" t="s">
         <v>395</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q34" s="10" t="s">
-        <v>385</v>
-      </c>
-      <c r="S34" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="T34" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="V34" s="7" t="s">
-        <v>398</v>
       </c>
       <c r="X34" s="7">
         <v>1913</v>
       </c>
       <c r="Y34" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF34" s="7" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q35" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="X35" s="7">
         <v>1913</v>
       </c>
       <c r="Y35" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF35" s="7" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="S36" s="7" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="V36" s="7" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="X36" s="7">
         <v>1913</v>
       </c>
       <c r="Y36" s="7" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="AF36" s="7" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="AG36" s="7" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="AH36" s="7" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="37" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q37" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="X37" s="7">
         <v>1908</v>
@@ -4968,383 +5031,307 @@
         <v>2</v>
       </c>
       <c r="AF37" s="7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J38" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K38" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="L38" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="M38" s="7" t="s">
         <v>477</v>
-      </c>
-      <c r="L38" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>480</v>
       </c>
       <c r="N38" s="7">
         <v>1874</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="AF38" s="11" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="AG38" s="7" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="39" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K39" s="7" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="L39" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="M39" s="7" t="s">
         <v>478</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>481</v>
       </c>
       <c r="N39" s="7">
         <v>1874</v>
       </c>
       <c r="O39" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="AF39" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="AG39" s="7" t="s">
         <v>479</v>
-      </c>
-      <c r="AF39" s="7" t="s">
-        <v>476</v>
-      </c>
-      <c r="AG39" s="7" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="40" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q40" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="S40" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="T40" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q40" s="10" t="s">
+      <c r="V40" s="7" t="s">
         <v>495</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="T40" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="V40" s="7" t="s">
-        <v>498</v>
       </c>
       <c r="X40" s="7">
         <v>1917</v>
       </c>
       <c r="Y40" s="7" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="AF40" s="7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D41" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="T41" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="V41" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q41" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="S41" s="7" t="s">
+      <c r="X41" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="T41" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="U41" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V41" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="X41" s="7" t="s">
-        <v>505</v>
-      </c>
       <c r="Y41" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="AF41" s="7" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="AG41" s="11"/>
     </row>
     <row r="42" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q42" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="S42" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="U42" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="V42" s="7" t="s">
         <v>501</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>502</v>
-      </c>
-      <c r="T42" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="U42" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="V42" s="7" t="s">
-        <v>504</v>
       </c>
       <c r="X42" s="7">
         <v>1899</v>
       </c>
       <c r="Y42" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF42" s="7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="U43" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="X43" s="7">
         <v>1902</v>
       </c>
       <c r="Y43" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AF43" s="7" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="44" spans="1:34" ht="187" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J44" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L44" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N44" s="7">
         <v>1874</v>
       </c>
       <c r="O44" s="15" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="AF44" s="7" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="45" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>547</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>555</v>
-      </c>
-      <c r="N45" s="7" t="s">
-        <v>553</v>
-      </c>
-      <c r="O45" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="AF45" s="7" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="46" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>559</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>551</v>
-      </c>
-      <c r="J46" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K46" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L46" s="7" t="s">
-        <v>552</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>556</v>
-      </c>
-      <c r="N46" s="7" t="s">
-        <v>553</v>
-      </c>
-      <c r="O46" s="7" t="s">
-        <v>554</v>
-      </c>
-      <c r="AF46" s="7" t="s">
-        <v>558</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -5359,10 +5346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F35043C1-934F-2441-9036-DCF88E610249}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5374,31 +5361,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B1" t="str">
         <f>Artifacts!D29</f>
         <v>Anonymous</v>
       </c>
       <c r="C1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="E1" t="str">
         <f>Artifacts!B29</f>
         <v>Pandita Ramabai Sarasvati</v>
       </c>
       <c r="F1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G1" t="str">
         <f>Artifacts!N29</f>
         <v>[Late nineteenth century]</v>
       </c>
       <c r="H1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I1" s="16" t="str">
         <f>A1&amp;B1&amp;C1&amp;D1&amp;E1&amp;F1&amp;G1&amp;H1</f>
@@ -5407,31 +5394,31 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B2" t="str">
         <f>Artifacts!D30</f>
         <v>J. Paul</v>
       </c>
       <c r="C2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E2" t="str">
         <f>Artifacts!B30</f>
         <v>“Pandita Ramabai &amp; Her Gifted Daughter Manoramabai”</v>
       </c>
       <c r="F2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G2" t="str">
         <f>Artifacts!N30</f>
         <v>[Early twentieth century]</v>
       </c>
       <c r="H2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I2" s="16" t="str">
         <f t="shared" ref="I2:I9" si="0">A2&amp;B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2</f>
@@ -5440,30 +5427,30 @@
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B3" t="str">
         <f>Artifacts!D31</f>
         <v>Anonymous</v>
       </c>
       <c r="C3" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E3" t="str">
         <f>Artifacts!B31</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H3" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I3" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5472,30 +5459,30 @@
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B4" t="str">
         <f>Artifacts!D32</f>
         <v>Johnson, E. Pauline, 1861-1913</v>
       </c>
       <c r="C4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D4" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E4" t="str">
         <f>Artifacts!B32</f>
         <v>“And He Said ‘Fight On’” (Manuscript Facsimile)</v>
       </c>
       <c r="F4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I4" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5504,30 +5491,30 @@
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B5" t="str">
         <f>Artifacts!D33</f>
         <v>Anonymous</v>
       </c>
       <c r="C5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E5" t="str">
         <f>Artifacts!B33</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H5" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I5" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5536,30 +5523,30 @@
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B6" t="str">
         <f>Artifacts!D34</f>
         <v>Anonymous</v>
       </c>
       <c r="C6" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D6" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E6" t="str">
         <f>Artifacts!B34</f>
         <v>E. Pauline Johnson (with Facsimile Signature)</v>
       </c>
       <c r="F6" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H6" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I6" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5568,30 +5555,30 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B7" t="str">
         <f>Artifacts!D35</f>
         <v>Anonymous</v>
       </c>
       <c r="C7" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D7" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E7" t="str">
         <f>Artifacts!B35</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F7" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G7" s="7">
         <v>1904</v>
       </c>
       <c r="H7" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I7" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5600,30 +5587,30 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B8" t="str">
         <f>Artifacts!D36</f>
         <v>Anonymous</v>
       </c>
       <c r="C8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D8" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E8" t="str">
         <f>Artifacts!B36</f>
         <v xml:space="preserve">“The Grave of Pauline Johnson in Stanley Park, Near Siwash Rock”; “Siwash Rock”; “The Spirit of Siwash Rock” </v>
       </c>
       <c r="F8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I8" s="16" t="str">
         <f t="shared" si="0"/>
@@ -5632,34 +5619,124 @@
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B9" t="str">
         <f>Artifacts!D37</f>
         <v>Anonymous</v>
       </c>
       <c r="C9" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D9" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E9" t="str">
         <f>Artifacts!B37</f>
         <v>E. Pauline Johnson</v>
       </c>
       <c r="F9" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="H9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="I9" s="16" t="str">
         <f t="shared" si="0"/>
         <v>&lt;li&gt;Anonymous. &lt;a href="transcriptions/liv_021034_ART.html"&gt;E. Pauline Johnson&lt;/a&gt;. [Early twentieth century].&lt;/li&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="Z21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="7" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" s="7" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="Z22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="7" t="s">
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for nosutu and ranavalona
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2B8D7D-8082-2D4A-B911-2C38B109F010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED22BF9-C1A4-134F-A106-B306338C4BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="575">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1591,12 +1591,6 @@
     <t>liv_020040</t>
   </si>
   <si>
-    <t>History of Warori or Basango (Excerpt from David Livingstone's Notebook, [March 1866-March 1870])</t>
-  </si>
-  <si>
-    <t>History of Warori or Basango (Excerpt from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
-  </si>
-  <si>
     <t>Bogharib, Mohammed</t>
   </si>
   <si>
@@ -1708,15 +1702,9 @@
     <t>liv_020043</t>
   </si>
   <si>
-    <t>“Nosutu's Letter”</t>
-  </si>
-  <si>
     <t>Missionary Record of the United Presbyterian Church</t>
   </si>
   <si>
-    <t>“Nosutu's Letter,” 2 March 1874</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 March 1874; October 1873 </t>
   </si>
   <si>
@@ -1742,6 +1730,42 @@
   </si>
   <si>
     <t>Cumming, John</t>
+  </si>
+  <si>
+    <t>liv_020044</t>
+  </si>
+  <si>
+    <t>Ranavalonamanjaka, c.1788-1861</t>
+  </si>
+  <si>
+    <t>Moss, Charles Frederick Arrowsmith</t>
+  </si>
+  <si>
+    <t>Cape Monthly Magazine</t>
+  </si>
+  <si>
+    <t>178-79</t>
+  </si>
+  <si>
+    <t>1 March 1876; 1875</t>
+  </si>
+  <si>
+    <t>“History of Warori or Basango” (Excerpt from David Livingstone's Notebook, [March 1866-March 1870])</t>
+  </si>
+  <si>
+    <t>“History of Warori or Basango” (Excerpt from David Livingstone's Notebook, [March 1866-March 1870]), 19 July 1869</t>
+  </si>
+  <si>
+    <t>“Foreign Missions. Caffreland” (Excerpt)</t>
+  </si>
+  <si>
+    <t>“Foreign Missions. Caffrelan” (Excerpt) 2 March 1874</t>
+  </si>
+  <si>
+    <t>“The Late Mr. James Cameron of Madagascar” (Excerpt)</t>
+  </si>
+  <si>
+    <t>“The Late Mr. James Cameron of Madagascar” (Excerpt), 1 March 1876</t>
   </si>
 </sst>
 </file>
@@ -2210,11 +2234,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF34"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2583,16 +2607,16 @@
     </row>
     <row r="9" spans="1:32" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>527</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>177</v>
@@ -2610,10 +2634,10 @@
         <v>34</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>49</v>
@@ -2633,7 +2657,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>115</v>
@@ -2671,7 +2695,7 @@
         <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>430</v>
@@ -2703,7 +2727,7 @@
         <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>430</v>
@@ -2735,7 +2759,7 @@
         <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>58</v>
@@ -3345,13 +3369,13 @@
         <v>515</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>516</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>518</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>177</v>
@@ -3372,27 +3396,27 @@
         <v>807</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="32" spans="1:32" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>177</v>
@@ -3413,7 +3437,7 @@
         <v>807</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>49</v>
@@ -3421,16 +3445,16 @@
     </row>
     <row r="33" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>177</v>
@@ -3451,7 +3475,7 @@
         <v>807</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>49</v>
@@ -3459,31 +3483,31 @@
     </row>
     <row r="34" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>555</v>
+        <v>571</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>557</v>
+        <v>572</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>282</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>430</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="R34" s="1">
         <v>44</v>
@@ -3492,7 +3516,36 @@
         <v>53</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>12</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>568</v>
       </c>
     </row>
   </sheetData>
@@ -3783,7 +3836,7 @@
         <v>132</v>
       </c>
       <c r="AF7" s="11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="8" spans="1:33" ht="51" x14ac:dyDescent="0.2">
@@ -5295,13 +5348,13 @@
     </row>
     <row r="44" spans="1:34" ht="187" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>535</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>537</v>
-      </c>
       <c r="C44" s="7" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>483</v>
@@ -5331,7 +5384,7 @@
         <v>476</v>
       </c>
       <c r="AF44" s="7" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -5651,19 +5704,19 @@
     </row>
     <row r="21" spans="1:32" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>542</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>543</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>544</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
@@ -5674,16 +5727,16 @@
         <v>45</v>
       </c>
       <c r="L21" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>545</v>
-      </c>
-      <c r="M21" s="7" t="s">
-        <v>548</v>
-      </c>
-      <c r="N21" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>547</v>
       </c>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
@@ -5691,24 +5744,24 @@
       <c r="Z21" s="9"/>
       <c r="AE21" s="9"/>
       <c r="AF21" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="22" spans="1:32" s="7" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>539</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>543</v>
-      </c>
       <c r="G22" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
@@ -5719,16 +5772,16 @@
         <v>45</v>
       </c>
       <c r="L22" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>545</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="N22" s="7" t="s">
-        <v>546</v>
-      </c>
-      <c r="O22" s="7" t="s">
-        <v>547</v>
       </c>
       <c r="P22" s="9"/>
       <c r="Q22" s="10"/>
@@ -5736,7 +5789,7 @@
       <c r="Z22" s="9"/>
       <c r="AE22" s="9"/>
       <c r="AF22" s="7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MODS for douglass
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532846E5-45C8-E544-881F-BE0B21366E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D0FE33-3DFB-2244-8FDD-4EB7483F1EE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="611">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1750,9 +1750,6 @@
     <t>“Foreign Missions. Caffreland” (Excerpt)</t>
   </si>
   <si>
-    <t>“Foreign Missions. Caffrelan” (Excerpt) 2 March 1874</t>
-  </si>
-  <si>
     <t>“The Late Mr. James Cameron of Madagascar” (Excerpt)</t>
   </si>
   <si>
@@ -1835,6 +1832,48 @@
   </si>
   <si>
     <t>608w,</t>
+  </si>
+  <si>
+    <t>liv_020031</t>
+  </si>
+  <si>
+    <t>liv_020032</t>
+  </si>
+  <si>
+    <t>Letter to John Scoble</t>
+  </si>
+  <si>
+    <t>“Foreign Missions. Caffrelan” (Excerpt), 2 March 1874</t>
+  </si>
+  <si>
+    <t>Letter to John Scoble, 9 May 1846</t>
+  </si>
+  <si>
+    <t>Letter to Catherine Impey</t>
+  </si>
+  <si>
+    <t>Letter to Catherine Impey, 9 July 1888</t>
+  </si>
+  <si>
+    <t>Douglass, Frederick, 1818-1895</t>
+  </si>
+  <si>
+    <t>MSS. Brit. Emp. s. 18, C16/75</t>
+  </si>
+  <si>
+    <t>MSS. Brit. Emp. s. 20, E5/7</t>
+  </si>
+  <si>
+    <t>9 May 1846</t>
+  </si>
+  <si>
+    <t>9 July 1888</t>
+  </si>
+  <si>
+    <t>York Temperance Hotel, Edinburgh</t>
+  </si>
+  <si>
+    <t>Cedar Hill. Anacostia, D.C.</t>
   </si>
 </sst>
 </file>
@@ -2303,11 +2342,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG37" sqref="AG37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3144,7 +3183,7 @@
         <v>170</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>429</v>
@@ -3558,10 +3597,10 @@
         <v>568</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>569</v>
+        <v>600</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>559</v>
@@ -3593,13 +3632,13 @@
         <v>561</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>571</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>572</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>562</v>
@@ -3615,6 +3654,70 @@
       </c>
       <c r="T35" s="1" t="s">
         <v>565</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -3631,7 +3734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AF46" sqref="AF46"/>
     </sheetView>
@@ -5453,21 +5556,21 @@
         <v>475</v>
       </c>
       <c r="AF44" s="7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="45" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>580</v>
       </c>
-      <c r="C45" s="7" t="s">
-        <v>581</v>
-      </c>
       <c r="D45" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>540</v>
@@ -5491,21 +5594,21 @@
         <v>543</v>
       </c>
       <c r="AF45" s="7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="46" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>540</v>
@@ -5529,7 +5632,7 @@
         <v>543</v>
       </c>
       <c r="AF46" s="7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -5849,10 +5952,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G12" t="str">
         <f>E12&amp;" "&amp;F12</f>
@@ -5861,10 +5964,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F13" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ref="G13:G18" si="1">E13&amp;" "&amp;F13</f>
@@ -5873,10 +5976,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -5885,10 +5988,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F15" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -5897,10 +6000,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F16" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -5909,10 +6012,10 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
@@ -5921,10 +6024,10 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
update mods for read
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C285D564-67F6-7E49-B83C-6767DB21A8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241B092-0900-8C44-854F-810F894C68F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="628">
   <si>
     <t>liv_000017</t>
   </si>
@@ -1907,6 +1907,24 @@
   </si>
   <si>
     <t>Signatures, 1875[?], 1874</t>
+  </si>
+  <si>
+    <t>liv_020033</t>
+  </si>
+  <si>
+    <t>“Kat River Mission, South Africa”</t>
+  </si>
+  <si>
+    <t>“Kat River Mission, South Africa,” 1 April 1839</t>
+  </si>
+  <si>
+    <t>Missionary Magazine and Chronicle</t>
+  </si>
+  <si>
+    <t>55-57</t>
+  </si>
+  <si>
+    <t>1 Apri 1839, 9 October 1838</t>
   </si>
 </sst>
 </file>
@@ -2375,11 +2393,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3753,6 +3771,38 @@
         <v>610</v>
       </c>
     </row>
+    <row r="38" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>3</v>
+      </c>
+      <c r="R38" s="1">
+        <v>25</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF33">
     <sortCondition ref="A2:A33"/>
@@ -3767,8 +3817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update mods for moshoeshoe
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39A53B5-69E5-B742-8407-111791C66B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2479B4-E5E0-3D4A-8A38-2753AC092804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="676">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2039,6 +2039,36 @@
   </si>
   <si>
     <t>1 January 1838; July 1837; 24 November 1837</t>
+  </si>
+  <si>
+    <t>liv_020045</t>
+  </si>
+  <si>
+    <t>“The Cape of Good Hope”</t>
+  </si>
+  <si>
+    <t>“The Cape of Good Hope,” 22 January 1856</t>
+  </si>
+  <si>
+    <t>Boshoff, Jacobus Nicolaas, 1808-1881</t>
+  </si>
+  <si>
+    <t>Moshoeshoe, c.1786-1870</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>22 January 1856; 5 October 1855</t>
+  </si>
+  <si>
+    <t>Nehemiah</t>
+  </si>
+  <si>
+    <t>Arbousset, Thomas, 1810-1887</t>
+  </si>
+  <si>
+    <t>Grey, George, 1812-1898</t>
   </si>
 </sst>
 </file>
@@ -2147,7 +2177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2193,9 +2223,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2510,11 +2537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AG40"/>
+  <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2522,20 +2549,20 @@
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
-    <col min="4" max="7" width="20.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" style="3" customWidth="1"/>
-    <col min="10" max="12" width="21.83203125" style="1" customWidth="1"/>
-    <col min="13" max="15" width="20.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" style="3" customWidth="1"/>
-    <col min="17" max="20" width="15.83203125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="20.83203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12.83203125" style="3" customWidth="1"/>
-    <col min="23" max="33" width="15.83203125" style="4" customWidth="1"/>
-    <col min="34" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="9" width="20.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" style="3" customWidth="1"/>
+    <col min="12" max="14" width="21.83203125" style="1" customWidth="1"/>
+    <col min="15" max="17" width="20.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" style="3" customWidth="1"/>
+    <col min="19" max="22" width="15.83203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="20.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="12.83203125" style="3" customWidth="1"/>
+    <col min="25" max="35" width="15.83203125" style="4" customWidth="1"/>
+    <col min="36" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
@@ -2558,64 +2585,64 @@
         <v>114</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>196</v>
@@ -2624,19 +2651,25 @@
         <v>196</v>
       </c>
       <c r="AD1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,29 +2682,29 @@
       <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>360</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2684,29 +2717,29 @@
       <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <v>801</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2719,29 +2752,29 @@
       <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>833</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2754,29 +2787,29 @@
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <v>836</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2789,29 +2822,29 @@
       <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2824,29 +2857,29 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>174</v>
       </c>
@@ -2862,29 +2895,29 @@
       <c r="E8" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="153" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>524</v>
       </c>
@@ -2900,29 +2933,29 @@
       <c r="E9" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2938,29 +2971,29 @@
       <c r="E10" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2976,23 +3009,23 @@
       <c r="E11" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R11" s="1">
+      <c r="T11" s="1">
         <v>15</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="V11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -3008,23 +3041,23 @@
       <c r="E12" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R12" s="1">
+      <c r="T12" s="1">
         <v>18</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="V12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="W12" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -3040,26 +3073,29 @@
       <c r="E13" s="1" t="s">
         <v>555</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R13" s="1">
+      <c r="T13" s="1">
         <v>15</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="V13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="U13" s="1">
+      <c r="W13" s="1">
         <v>1845</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -3072,29 +3108,29 @@
       <c r="D14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -3107,29 +3143,29 @@
       <c r="D15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3145,23 +3181,26 @@
       <c r="E16" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="F16" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T16" s="1">
+      <c r="V16" s="1">
         <v>10</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="W16" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3174,23 +3213,23 @@
       <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S17" s="1">
+      <c r="U17" s="1">
         <v>93</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="V17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="W17" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -3203,29 +3242,29 @@
       <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>172</v>
       </c>
@@ -3241,26 +3280,26 @@
       <c r="E19" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="R19" s="1">
+      <c r="T19" s="1">
         <v>28</v>
       </c>
-      <c r="S19" s="1">
+      <c r="U19" s="1">
         <v>6</v>
       </c>
-      <c r="T19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="W19" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>136</v>
       </c>
@@ -3276,42 +3315,42 @@
       <c r="E20" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
-      <c r="W20" s="1" t="s">
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="Y20" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="Y20" s="4" t="s">
+      <c r="AA20" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="Z20" s="4" t="s">
+      <c r="AB20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AA20" s="4" t="s">
+      <c r="AC20" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="AB20" s="4" t="s">
+      <c r="AD20" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="AC20" s="4" t="s">
+      <c r="AE20" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AD20" s="4" t="s">
+      <c r="AF20" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="AF20" s="4">
+      <c r="AH20" s="4">
         <v>1906</v>
       </c>
-      <c r="AG20" s="4">
+      <c r="AI20" s="4">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>262</v>
       </c>
@@ -3327,20 +3366,20 @@
       <c r="E21" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="T21" s="1">
+      <c r="V21" s="1">
         <v>3</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="W21" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>277</v>
       </c>
@@ -3356,23 +3395,23 @@
       <c r="E22" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="S22" s="1">
+      <c r="U22" s="1">
         <v>89</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="U22" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>451</v>
       </c>
@@ -3388,29 +3427,29 @@
       <c r="E23" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="P23" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>445</v>
       </c>
@@ -3426,20 +3465,23 @@
       <c r="E24" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="F24" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G24" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="U24" s="1" t="s">
+      <c r="W24" s="1" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>450</v>
       </c>
@@ -3455,32 +3497,35 @@
       <c r="E25" s="1" t="s">
         <v>447</v>
       </c>
+      <c r="F25" s="1" t="s">
+        <v>461</v>
+      </c>
       <c r="G25" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>267</v>
       </c>
@@ -3496,23 +3541,23 @@
       <c r="E26" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q26" s="1" t="s">
+      <c r="S26" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="R26" s="1">
+      <c r="T26" s="1">
         <v>1</v>
       </c>
-      <c r="S26" s="1">
+      <c r="U26" s="1">
         <v>82</v>
       </c>
-      <c r="U26" s="1" t="s">
+      <c r="W26" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>270</v>
       </c>
@@ -3525,29 +3570,29 @@
       <c r="D27" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="J27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="P27" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>428</v>
       </c>
@@ -3563,20 +3608,20 @@
       <c r="E28" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="J28" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="S28" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="T28" s="1" t="s">
+      <c r="V28" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="U28" s="1" t="s">
+      <c r="W28" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>440</v>
       </c>
@@ -3592,20 +3637,20 @@
       <c r="E29" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="J29" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T29" s="1">
+      <c r="V29" s="1">
         <v>5</v>
       </c>
-      <c r="U29" s="1" t="s">
+      <c r="W29" s="1" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>452</v>
       </c>
@@ -3621,29 +3666,29 @@
       <c r="E30" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="P30" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="O30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="102" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35" ht="102" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>514</v>
       </c>
@@ -3659,29 +3704,29 @@
       <c r="E31" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="J31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M31" s="1">
+      <c r="O31" s="1">
         <v>807</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="119" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>518</v>
       </c>
@@ -3697,32 +3742,32 @@
       <c r="E32" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="L32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M32" s="1">
+      <c r="O32" s="1">
         <v>807</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="P32" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="O32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>549</v>
       </c>
@@ -3738,29 +3783,29 @@
       <c r="E33" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M33" s="1">
+      <c r="O33" s="1">
         <v>807</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="Q33" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35" ht="85" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>550</v>
       </c>
@@ -3776,29 +3821,29 @@
       <c r="E34" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="T34" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="S34" s="1">
+      <c r="U34" s="1">
         <v>44</v>
       </c>
-      <c r="T34" s="1">
+      <c r="V34" s="1">
         <v>53</v>
       </c>
-      <c r="U34" s="1" t="s">
+      <c r="W34" s="1" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="68" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>561</v>
       </c>
@@ -3814,23 +3859,23 @@
       <c r="E35" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="S35" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="R35" s="1">
+      <c r="T35" s="1">
         <v>12</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="V35" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="W35" s="1" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>597</v>
       </c>
@@ -3843,29 +3888,29 @@
       <c r="D36" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="P36" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="O36" s="1" t="s">
+      <c r="Q36" s="1" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>598</v>
       </c>
@@ -3878,29 +3923,29 @@
       <c r="D37" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="P37" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="O37" s="1" t="s">
+      <c r="Q37" s="1" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>622</v>
       </c>
@@ -3916,26 +3961,26 @@
       <c r="E38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="S38" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="R38" s="1">
+      <c r="T38" s="1">
         <v>3</v>
       </c>
-      <c r="S38" s="1">
+      <c r="U38" s="1">
         <v>25</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="V38" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="U38" s="1" t="s">
+      <c r="W38" s="1" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="119" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35" ht="119" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>651</v>
       </c>
@@ -3948,29 +3993,29 @@
       <c r="D39" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="W39" s="1" t="s">
+      <c r="Y39" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="Y39" s="4" t="s">
+      <c r="AA39" s="4" t="s">
         <v>658</v>
       </c>
-      <c r="Z39" s="4" t="s">
+      <c r="AB39" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="AD39" s="4" t="s">
+      <c r="AF39" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="AF39" s="4">
+      <c r="AH39" s="4">
         <v>1855</v>
       </c>
-      <c r="AG39" s="4" t="s">
+      <c r="AI39" s="4" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>660</v>
       </c>
@@ -3992,27 +4037,68 @@
       <c r="G40" s="1" t="s">
         <v>664</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="S40" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="R40" s="1">
+      <c r="T40" s="1">
         <v>2</v>
       </c>
-      <c r="S40" s="1">
+      <c r="U40" s="1">
         <v>20</v>
       </c>
-      <c r="T40" s="17">
-        <v>44049</v>
-      </c>
-      <c r="U40" s="1" t="s">
+      <c r="V40" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="W40" s="1" t="s">
         <v>665</v>
       </c>
     </row>
+    <row r="41" spans="1:35" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V41" s="1">
+        <v>5</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>672</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI33">
     <sortCondition ref="A2:A33"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update mods for farrar
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B47B31B-8EDA-3649-9A42-B2BD1B9CC222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C26575-877F-8542-AD8B-F13A46AC4B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="835">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2525,6 +2525,27 @@
   </si>
   <si>
     <t>Bain News Service</t>
+  </si>
+  <si>
+    <t>liv_020061</t>
+  </si>
+  <si>
+    <t>“The History of Caras Farrar of Finding Dr Livingstone, in Central Africa”</t>
+  </si>
+  <si>
+    <t>“The History of Caras Farrar of Finding Dr Livingstone, in Central Africa,” 9 September 1874</t>
+  </si>
+  <si>
+    <t>Farrar, Caras, ?-c.1906</t>
+  </si>
+  <si>
+    <t>9 September 1874</t>
+  </si>
+  <si>
+    <t>Bombay</t>
+  </si>
+  <si>
+    <t>CMS/Z 19</t>
   </si>
 </sst>
 </file>
@@ -2996,11 +3017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AI45"/>
+  <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4696,6 +4717,44 @@
         <v>688</v>
       </c>
     </row>
+    <row r="46" spans="1:35" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L46" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI33">
     <sortCondition ref="A2:A33"/>
@@ -4710,9 +4769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M47" sqref="M47:O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update mods for new art
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/One-More-Voice/transcriptions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20EF8DB-5A3F-DB4D-8C90-03BCC438A936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F088FF-84E6-DF44-BD08-6C12F63E2C3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="881">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2359,9 +2359,6 @@
     <t>Liberia</t>
   </si>
   <si>
-    <t>Harry Johnston</t>
-  </si>
-  <si>
     <t>1:231</t>
   </si>
   <si>
@@ -2431,9 +2428,6 @@
     <t>Sc 811.09-K (Kerlin, R. Negro poets and their poems. 1923)</t>
   </si>
   <si>
-    <t>Robert Thomas Kerlin</t>
-  </si>
-  <si>
     <t>Negro Poets and Their Poems</t>
   </si>
   <si>
@@ -2552,6 +2546,144 @@
   </si>
   <si>
     <t>Soga Jotelo, Nosuthu, c.1805-1887</t>
+  </si>
+  <si>
+    <t>liv_021065</t>
+  </si>
+  <si>
+    <t>liv_021066</t>
+  </si>
+  <si>
+    <t>liv_021067</t>
+  </si>
+  <si>
+    <t>liv_021068</t>
+  </si>
+  <si>
+    <t>liv_021069</t>
+  </si>
+  <si>
+    <t>Frederick Douglass</t>
+  </si>
+  <si>
+    <t>Male Figure (Nkisi Nkondi)</t>
+  </si>
+  <si>
+    <t>Tausé Soga and Her Family</t>
+  </si>
+  <si>
+    <t>Male Face Mask (Chihongo)</t>
+  </si>
+  <si>
+    <t>Mask for Egungun (Ere Egungun)</t>
+  </si>
+  <si>
+    <t>Anonymous Vili Artist</t>
+  </si>
+  <si>
+    <t>Anonymous Chokwe Artist</t>
+  </si>
+  <si>
+    <t>Anonymous Yoruba Artist</t>
+  </si>
+  <si>
+    <t>Miller, Samuel J., 1822-1888</t>
+  </si>
+  <si>
+    <t>Tausé Soga and Her Family, 1894</t>
+  </si>
+  <si>
+    <t>Black and white head and shoulder portrait of Frederick Douglass in a gold frame.</t>
+  </si>
+  <si>
+    <t>Wooden carving of male figure with body covered in shells, bones, feathers, fabric, metal nails.</t>
+  </si>
+  <si>
+    <t>Tausé Soga standing with man and child at her sides and with older woman seated with child on lap.</t>
+  </si>
+  <si>
+    <t>A work made of wood, raffia, burlap, turaco feathers, guinea fowl feathers, and pigment.</t>
+  </si>
+  <si>
+    <t>A work made of wood and pigment.</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Iseyin, Nigeria</t>
+  </si>
+  <si>
+    <t>CC0 Public Domain Designation</t>
+  </si>
+  <si>
+    <t>Offices of the United Presbyterian Church</t>
+  </si>
+  <si>
+    <t>The Story of Our Kaffrarian Mission. Missions of the United Presbyterian Church Described in a Series of Stories, Vol. 3</t>
+  </si>
+  <si>
+    <t>Johnston, Harry, 1858-1927</t>
+  </si>
+  <si>
+    <t>Kerlin, Robert Thomas, 1866-1950</t>
+  </si>
+  <si>
+    <t>Slowan, William J.</t>
+  </si>
+  <si>
+    <t>Art Institute of Chicago</t>
+  </si>
+  <si>
+    <t>Major Acquisitions Centennial Endowment, 1996.433</t>
+  </si>
+  <si>
+    <t>Ada Turnbull Hertle Endowment , 1998.502</t>
+  </si>
+  <si>
+    <t>Restricted gift of Mrs. James W. Alsdorf, 2003.174</t>
+  </si>
+  <si>
+    <t>Tillie C. Cohn Endowment Fund, 1976.308</t>
+  </si>
+  <si>
+    <t>https://www.artic.edu/artworks/145681/frederick-douglass</t>
+  </si>
+  <si>
+    <t>https://www.artic.edu/artworks/151358/male-figure-nkisi-nkondi</t>
+  </si>
+  <si>
+    <t>https://www.artic.edu/artworks/181740/male-face-mask-chihongo</t>
+  </si>
+  <si>
+    <t>https://www.artic.edu/artworks/51194/mask-for-egungun-ere-egungun</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/missionsofunited00unit/page/56/mode/2up</t>
+  </si>
+  <si>
+    <t>Male Face Mask (Chihongo), [mid/late nineteenth century]</t>
+  </si>
+  <si>
+    <t>Mask for Egungun (Ere Egungun), [late nineteenth century]</t>
+  </si>
+  <si>
+    <t>Male Figure (Nkisi Nkondi), [early/mid-nineteenth century (1801-1875)]</t>
+  </si>
+  <si>
+    <t>Frederick Douglass, [c.1847-c.1852]</t>
+  </si>
+  <si>
+    <t>[c.1847-c.1852]</t>
+  </si>
+  <si>
+    <t>[Early/mid-nineteenth century (1801-1875)]</t>
+  </si>
+  <si>
+    <t>[Mid/late nineteenth century]</t>
   </si>
 </sst>
 </file>
@@ -3025,8 +3157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -4296,16 +4428,16 @@
         <v>550</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>170</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>170</v>
@@ -4314,7 +4446,7 @@
         <v>559</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>429</v>
@@ -4731,16 +4863,16 @@
     </row>
     <row r="46" spans="1:35" ht="85" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>825</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>827</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>170</v>
@@ -4758,13 +4890,13 @@
         <v>612</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
@@ -4779,11 +4911,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM68"/>
+  <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S73" sqref="S73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4807,7 +4939,7 @@
     <col min="31" max="31" width="15.83203125" style="9" customWidth="1"/>
     <col min="32" max="35" width="15.83203125" style="7" customWidth="1"/>
     <col min="36" max="36" width="15.83203125" style="9" customWidth="1"/>
-    <col min="37" max="37" width="10.83203125" style="17"/>
+    <col min="37" max="39" width="10.83203125" style="17"/>
     <col min="40" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
@@ -7058,7 +7190,7 @@
         <v>756</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L55" s="7" t="s">
         <v>117</v>
@@ -7102,7 +7234,7 @@
         <v>762</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L56" s="7" t="s">
         <v>117</v>
@@ -7134,13 +7266,13 @@
         <v>710</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>725</v>
@@ -7152,7 +7284,7 @@
         <v>728</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L57" s="7" t="s">
         <v>117</v>
@@ -7196,7 +7328,7 @@
         <v>734</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L58" s="7" t="s">
         <v>117</v>
@@ -7240,7 +7372,7 @@
         <v>738</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="L59" s="7" t="s">
         <v>117</v>
@@ -7354,7 +7486,7 @@
         <v>765</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F62" s="7" t="s">
         <v>767</v>
@@ -7378,7 +7510,7 @@
         <v>204</v>
       </c>
       <c r="Q62" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="R62" s="7" t="s">
         <v>769</v>
@@ -7390,7 +7522,7 @@
         <v>703</v>
       </c>
       <c r="V62" s="10" t="s">
-        <v>772</v>
+        <v>861</v>
       </c>
       <c r="X62" s="7" t="s">
         <v>771</v>
@@ -7405,30 +7537,30 @@
         <v>1906</v>
       </c>
       <c r="AD62" s="16" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="63" spans="1:30" ht="119" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>778</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>774</v>
+      </c>
+      <c r="G63" s="7" t="s">
         <v>776</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>781</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>779</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>775</v>
-      </c>
-      <c r="G63" s="7" t="s">
+      <c r="H63" s="7" t="s">
         <v>777</v>
       </c>
-      <c r="H63" s="7" t="s">
-        <v>778</v>
-      </c>
       <c r="I63" s="7" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="L63" s="7" t="s">
         <v>117</v>
@@ -7440,10 +7572,10 @@
         <v>204</v>
       </c>
       <c r="Q63" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="R63" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="S63" s="7">
         <v>1910</v>
@@ -7452,16 +7584,16 @@
         <v>703</v>
       </c>
       <c r="V63" s="10" t="s">
-        <v>772</v>
+        <v>861</v>
       </c>
       <c r="X63" s="7" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="Y63" s="7" t="s">
         <v>64</v>
       </c>
       <c r="AA63" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="AC63" s="7">
         <v>1910</v>
@@ -7472,22 +7604,22 @@
     </row>
     <row r="64" spans="1:30" ht="136" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>786</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>774</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>799</v>
-      </c>
-      <c r="F64" s="7" t="s">
-        <v>787</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>386</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="I64" s="7" t="s">
         <v>170</v>
@@ -7502,10 +7634,10 @@
         <v>204</v>
       </c>
       <c r="Q64" s="7" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="R64" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="S64" s="7" t="s">
         <v>368</v>
@@ -7516,22 +7648,22 @@
     </row>
     <row r="65" spans="1:30" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
+        <v>790</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>791</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>781</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>800</v>
-      </c>
-      <c r="F65" s="7" t="s">
+      <c r="G65" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>793</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>794</v>
       </c>
       <c r="I65" s="7" t="s">
         <v>170</v>
@@ -7546,10 +7678,10 @@
         <v>204</v>
       </c>
       <c r="Q65" s="7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="R65" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="S65" s="7">
         <v>1923</v>
@@ -7558,16 +7690,16 @@
         <v>703</v>
       </c>
       <c r="V65" s="10" t="s">
-        <v>796</v>
+        <v>862</v>
       </c>
       <c r="X65" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="Y65" s="7" t="s">
         <v>45</v>
       </c>
       <c r="AA65" s="7" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="AC65" s="7">
         <v>1923</v>
@@ -7578,22 +7710,22 @@
     </row>
     <row r="66" spans="1:30" ht="136" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>801</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>774</v>
-      </c>
-      <c r="C66" s="7" t="s">
+      <c r="G66" s="7" t="s">
+        <v>792</v>
+      </c>
+      <c r="H66" s="7" t="s">
         <v>802</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>803</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>793</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>804</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>170</v>
@@ -7608,13 +7740,13 @@
         <v>204</v>
       </c>
       <c r="Q66" s="7" t="s">
+        <v>803</v>
+      </c>
+      <c r="R66" s="7" t="s">
+        <v>804</v>
+      </c>
+      <c r="S66" s="7" t="s">
         <v>805</v>
-      </c>
-      <c r="R66" s="7" t="s">
-        <v>806</v>
-      </c>
-      <c r="S66" s="7" t="s">
-        <v>807</v>
       </c>
       <c r="T66" s="7" t="s">
         <v>703</v>
@@ -7622,22 +7754,22 @@
     </row>
     <row r="67" spans="1:30" ht="136" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>170</v>
@@ -7646,7 +7778,7 @@
         <v>117</v>
       </c>
       <c r="M67" s="11" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="O67" s="7" t="s">
         <v>44</v>
@@ -7655,10 +7787,10 @@
         <v>204</v>
       </c>
       <c r="Q67" s="7" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="R67" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="S67" s="7">
         <v>1903</v>
@@ -7669,22 +7801,22 @@
     </row>
     <row r="68" spans="1:30" ht="136" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>773</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>809</v>
+      </c>
+      <c r="G68" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>774</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>821</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>811</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>814</v>
-      </c>
       <c r="H68" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>170</v>
@@ -7699,28 +7831,254 @@
         <v>204</v>
       </c>
       <c r="Q68" s="7" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="R68" s="7" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="S68" s="7" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="T68" s="7" t="s">
         <v>703</v>
       </c>
-      <c r="V68" s="10" t="s">
-        <v>814</v>
+      <c r="V68" s="7" t="s">
+        <v>497</v>
       </c>
       <c r="X68" s="7" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="AC68" s="7">
         <v>1903</v>
       </c>
       <c r="AD68" s="7" t="s">
-        <v>820</v>
+        <v>818</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
+        <v>869</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>850</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>840</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="I69" s="17" t="s">
+        <v>848</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O69" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P69" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q69" s="17" t="s">
+        <v>864</v>
+      </c>
+      <c r="R69" s="17" t="s">
+        <v>865</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="T69" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
+        <v>870</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>851</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="G70" s="17" t="s">
+        <v>841</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="I70" s="17" t="s">
+        <v>845</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O70" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P70" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q70" s="17" t="s">
+        <v>864</v>
+      </c>
+      <c r="R70" s="17" t="s">
+        <v>866</v>
+      </c>
+      <c r="S70" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="T70" s="17" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>873</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>852</v>
+      </c>
+      <c r="F71" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>842</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="L71" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M71" s="11" t="s">
+        <v>814</v>
+      </c>
+      <c r="Q71" s="17"/>
+      <c r="R71" s="17"/>
+      <c r="T71" s="17"/>
+      <c r="V71" s="10" t="s">
+        <v>863</v>
+      </c>
+      <c r="X71" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="Y71" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA71" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="AC71" s="7">
+        <v>1894</v>
+      </c>
+      <c r="AD71" s="7">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>871</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>853</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>843</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="I72" s="17" t="s">
+        <v>846</v>
+      </c>
+      <c r="L72" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O72" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P72" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q72" s="17" t="s">
+        <v>864</v>
+      </c>
+      <c r="R72" s="17" t="s">
+        <v>867</v>
+      </c>
+      <c r="S72" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="T72" s="17" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
+        <v>872</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>858</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>854</v>
+      </c>
+      <c r="F73" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>844</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>847</v>
+      </c>
+      <c r="L73" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O73" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P73" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q73" s="17" t="s">
+        <v>864</v>
+      </c>
+      <c r="R73" s="17" t="s">
+        <v>868</v>
+      </c>
+      <c r="S73" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="T73" s="17" t="s">
+        <v>857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MODS for new wainwright
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE9A110-E4B4-0145-9130-D0039F345AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA1804-F8EE-314B-B309-B8544DD91B5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="894">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2684,6 +2684,45 @@
   </si>
   <si>
     <t>Male Figure (Nkisi Nkondi), [early/mid-nineteenth century]</t>
+  </si>
+  <si>
+    <t>liv_020051</t>
+  </si>
+  <si>
+    <t>liv_020052</t>
+  </si>
+  <si>
+    <t>Letter to [Horace Waller?]</t>
+  </si>
+  <si>
+    <t>Letter to [Horace Waller?], 15 September 1875</t>
+  </si>
+  <si>
+    <t>Wainwright, Jacob, c.1851/2-1893</t>
+  </si>
+  <si>
+    <t>Letter to William Salter Price</t>
+  </si>
+  <si>
+    <t>Letter to William Salter Price, 2 May 1876</t>
+  </si>
+  <si>
+    <t>2 May 1876</t>
+  </si>
+  <si>
+    <t>15 September 1875</t>
+  </si>
+  <si>
+    <t>CMS/B/OMS/C A5 O1/19</t>
+  </si>
+  <si>
+    <t>CMS/B/OMS/C A5 O23/54c</t>
+  </si>
+  <si>
+    <t>[Mombasa, East Africa]</t>
+  </si>
+  <si>
+    <t>Mombasa. East Africa</t>
   </si>
 </sst>
 </file>
@@ -3155,11 +3194,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AI46"/>
+  <dimension ref="A1:AI48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA47" sqref="AA47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4899,6 +4938,76 @@
         <v>827</v>
       </c>
     </row>
+    <row r="47" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="N47" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="48" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>892</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AI33">
     <sortCondition ref="A2:A33"/>
@@ -4913,7 +5022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
     </sheetView>

</xml_diff>

<commit_message>
update mods for new labatt
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034CA7E-2C01-DC47-B194-972AF31B15F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D787B7-A3F3-CD4E-9A51-02E5C1B2E59F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="919">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2783,6 +2783,21 @@
   </si>
   <si>
     <t>W. Bennett, Printer</t>
+  </si>
+  <si>
+    <t>liv_020036</t>
+  </si>
+  <si>
+    <t>“An Incident in the Late Rebellion in Jamaica”</t>
+  </si>
+  <si>
+    <t>“An Incident in the Late Rebellion in Jamaica,” 1855</t>
+  </si>
+  <si>
+    <t>36-47</t>
+  </si>
+  <si>
+    <t>R.J. DeCordova</t>
   </si>
 </sst>
 </file>
@@ -3254,11 +3269,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
-  <dimension ref="A1:AK50"/>
+  <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="AH51" sqref="AH51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5157,6 +5172,41 @@
       </c>
       <c r="AJ50" s="4">
         <v>1846</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" ht="119" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="AC51" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="AD51" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="AH51" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="AJ51" s="4">
+        <v>1855</v>
+      </c>
+      <c r="AK51" s="4" t="s">
+        <v>917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mods for new Soga image
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D787B7-A3F3-CD4E-9A51-02E5C1B2E59F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF7865E-87AF-A04D-8BE3-A3DB1FD6BC8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="932">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2798,6 +2798,45 @@
   </si>
   <si>
     <t>R.J. DeCordova</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/tiyosogapageofso00chal/page/n7/mode/2up</t>
+  </si>
+  <si>
+    <t>Tiyo Soga seat in quarter profile facing forward and holding a book.</t>
+  </si>
+  <si>
+    <t>liv_021070</t>
+  </si>
+  <si>
+    <t>Tiyo Soga (with Facsimile Signature)</t>
+  </si>
+  <si>
+    <t>Tiyo Soga (with Facsimile Signature), [late nineteenth century]</t>
+  </si>
+  <si>
+    <t>Chalmers, John A.</t>
+  </si>
+  <si>
+    <t>Tiyo Soga: A Page of South African Mission Work</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Grahamstown, Cape Colony</t>
+  </si>
+  <si>
+    <t>Andrew Elliot</t>
+  </si>
+  <si>
+    <t>Hodder &amp; Stoughton</t>
+  </si>
+  <si>
+    <t>David Bryce &amp; Son</t>
+  </si>
+  <si>
+    <t>James Kay</t>
   </si>
 </sst>
 </file>
@@ -3271,7 +3310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97A9DD5-2802-8C46-B4DE-35FF576EF7FC}">
   <dimension ref="A1:AK51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AH51" sqref="AH51"/>
     </sheetView>
@@ -5221,11 +5260,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM73"/>
+  <dimension ref="A1:AQ74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS74" sqref="AS74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5245,15 +5284,15 @@
     <col min="19" max="20" width="15.83203125" style="7" customWidth="1"/>
     <col min="21" max="21" width="15.83203125" style="9" customWidth="1"/>
     <col min="22" max="23" width="16.5" style="10" customWidth="1"/>
-    <col min="24" max="30" width="15.83203125" style="7" customWidth="1"/>
-    <col min="31" max="31" width="15.83203125" style="9" customWidth="1"/>
-    <col min="32" max="35" width="15.83203125" style="7" customWidth="1"/>
-    <col min="36" max="36" width="15.83203125" style="9" customWidth="1"/>
-    <col min="37" max="39" width="10.83203125" style="17"/>
-    <col min="40" max="16384" width="10.83203125" style="7"/>
+    <col min="24" max="34" width="15.83203125" style="7" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" style="9" customWidth="1"/>
+    <col min="36" max="39" width="15.83203125" style="7" customWidth="1"/>
+    <col min="40" max="40" width="15.83203125" style="9" customWidth="1"/>
+    <col min="41" max="43" width="10.83203125" style="17"/>
+    <col min="44" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>723</v>
       </c>
@@ -5332,35 +5371,35 @@
       <c r="Z1" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AM1" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" ht="85" x14ac:dyDescent="0.2">
       <c r="C2" s="11" t="s">
         <v>301</v>
       </c>
@@ -5368,7 +5407,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" ht="68" x14ac:dyDescent="0.2">
       <c r="C3" s="11" t="s">
         <v>303</v>
       </c>
@@ -5376,7 +5415,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" ht="102" x14ac:dyDescent="0.2">
       <c r="C4" s="11" t="s">
         <v>304</v>
       </c>
@@ -5414,7 +5453,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" ht="68" x14ac:dyDescent="0.2">
       <c r="C5" s="11" t="s">
         <v>305</v>
       </c>
@@ -5449,7 +5488,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="C6" s="11" t="s">
         <v>507</v>
       </c>
@@ -5481,7 +5520,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="C7" s="11" t="s">
         <v>531</v>
       </c>
@@ -5516,7 +5555,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" ht="68" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
         <v>306</v>
       </c>
@@ -5554,7 +5593,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="C9" s="11" t="s">
         <v>307</v>
       </c>
@@ -5592,7 +5631,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" ht="119" x14ac:dyDescent="0.2">
       <c r="C10" s="11" t="s">
         <v>308</v>
       </c>
@@ -5630,7 +5669,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="C11" s="11" t="s">
         <v>309</v>
       </c>
@@ -5671,7 +5710,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" ht="51" x14ac:dyDescent="0.2">
       <c r="C12" s="11" t="s">
         <v>311</v>
       </c>
@@ -5709,7 +5748,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:35" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" ht="102" x14ac:dyDescent="0.2">
       <c r="C13" s="11" t="s">
         <v>312</v>
       </c>
@@ -5747,7 +5786,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:35" ht="136" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:39" ht="136" x14ac:dyDescent="0.2">
       <c r="C14" s="11" t="s">
         <v>313</v>
       </c>
@@ -5784,17 +5823,17 @@
       <c r="Z14" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AB14" s="7" t="s">
+      <c r="AD14" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="AC14" s="7">
+      <c r="AG14" s="7">
         <v>1904</v>
       </c>
-      <c r="AD14" s="7" t="s">
+      <c r="AH14" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" ht="68" x14ac:dyDescent="0.2">
       <c r="C15" s="11" t="s">
         <v>315</v>
       </c>
@@ -5828,20 +5867,20 @@
       <c r="Z15" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AA15" s="7" t="s">
+      <c r="AC15" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="AB15" s="7" t="s">
+      <c r="AD15" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="AC15" s="7">
+      <c r="AG15" s="7">
         <v>1920</v>
       </c>
-      <c r="AD15" s="7" t="s">
+      <c r="AH15" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" ht="68" x14ac:dyDescent="0.2">
       <c r="C16" s="11" t="s">
         <v>316</v>
       </c>
@@ -5875,20 +5914,20 @@
       <c r="Z16" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AA16" s="7" t="s">
+      <c r="AC16" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="AB16" s="7" t="s">
+      <c r="AD16" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="AC16" s="7">
+      <c r="AG16" s="7">
         <v>1912</v>
       </c>
-      <c r="AD16" s="7" t="s">
+      <c r="AH16" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C17" s="11" t="s">
         <v>317</v>
       </c>
@@ -5919,17 +5958,17 @@
       <c r="Y17" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="AA17" s="7" t="s">
+      <c r="AC17" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="AC17" s="7">
+      <c r="AG17" s="7">
         <v>1901</v>
       </c>
-      <c r="AD17" s="7" t="s">
+      <c r="AH17" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="3:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:34" ht="85" x14ac:dyDescent="0.2">
       <c r="C18" s="11" t="s">
         <v>318</v>
       </c>
@@ -5960,17 +5999,17 @@
       <c r="Y18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA18" s="7" t="s">
+      <c r="AC18" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="AC18" s="7">
+      <c r="AG18" s="7">
         <v>1901</v>
       </c>
-      <c r="AD18" s="7" t="s">
+      <c r="AH18" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C19" s="11" t="s">
         <v>319</v>
       </c>
@@ -6001,17 +6040,17 @@
       <c r="Y19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA19" s="7" t="s">
+      <c r="AC19" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="AC19" s="7">
+      <c r="AG19" s="7">
         <v>1904</v>
       </c>
-      <c r="AD19" s="7" t="s">
+      <c r="AH19" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="F20" s="7" t="s">
         <v>190</v>
       </c>
@@ -6042,20 +6081,20 @@
       <c r="Z20" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA20" s="7" t="s">
+      <c r="AC20" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="AB20" s="7" t="s">
+      <c r="AD20" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="AG20" s="7">
         <v>1912</v>
       </c>
-      <c r="AD20" s="7" t="s">
+      <c r="AH20" s="7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="3:30" ht="153" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:34" ht="153" x14ac:dyDescent="0.2">
       <c r="C21" s="11" t="s">
         <v>320</v>
       </c>
@@ -6101,20 +6140,20 @@
       <c r="Z21" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AA21" s="7" t="s">
+      <c r="AC21" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="AB21" s="7" t="s">
+      <c r="AD21" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="AC21" s="7" t="s">
+      <c r="AG21" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="AD21" s="7" t="s">
+      <c r="AH21" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="22" spans="3:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:34" ht="85" x14ac:dyDescent="0.2">
       <c r="C22" s="11" t="s">
         <v>323</v>
       </c>
@@ -6145,17 +6184,17 @@
       <c r="Y22" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="AA22" s="7" t="s">
+      <c r="AC22" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="AC22" s="7">
+      <c r="AG22" s="7">
         <v>1887</v>
       </c>
-      <c r="AD22" s="7" t="s">
+      <c r="AH22" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C23" s="11" t="s">
         <v>323</v>
       </c>
@@ -6189,17 +6228,17 @@
       <c r="Y23" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="AA23" s="7" t="s">
+      <c r="AC23" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="AC23" s="7">
+      <c r="AG23" s="7">
         <v>1903</v>
       </c>
-      <c r="AD23" s="7" t="s">
+      <c r="AH23" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="3:30" ht="153" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:34" ht="153" x14ac:dyDescent="0.2">
       <c r="C24" s="7" t="s">
         <v>355</v>
       </c>
@@ -6240,7 +6279,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C25" s="7" t="s">
         <v>356</v>
       </c>
@@ -6281,7 +6320,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="3:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:34" ht="136" x14ac:dyDescent="0.2">
       <c r="C26" s="7" t="s">
         <v>358</v>
       </c>
@@ -6322,7 +6361,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="27" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C27" s="7" t="s">
         <v>357</v>
       </c>
@@ -6363,7 +6402,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="28" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C28" s="11" t="s">
         <v>351</v>
       </c>
@@ -6404,7 +6443,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C29" s="13" t="s">
         <v>377</v>
       </c>
@@ -6442,7 +6481,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C30" s="7" t="s">
         <v>378</v>
       </c>
@@ -6483,7 +6522,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="31" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C31" s="7" t="s">
         <v>380</v>
       </c>
@@ -6511,17 +6550,17 @@
       <c r="Y31" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="AA31" s="7" t="s">
+      <c r="AC31" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="AC31" s="7">
+      <c r="AG31" s="7">
         <v>1913</v>
       </c>
-      <c r="AD31" s="7" t="s">
+      <c r="AH31" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="32" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C32" s="7" t="s">
         <v>425</v>
       </c>
@@ -6552,17 +6591,17 @@
       <c r="Y32" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="AA32" s="7" t="s">
+      <c r="AC32" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="AC32" s="7">
+      <c r="AG32" s="7">
         <v>1913</v>
       </c>
-      <c r="AD32" s="7" t="s">
+      <c r="AH32" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="33" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C33" s="7" t="s">
         <v>396</v>
       </c>
@@ -6590,17 +6629,17 @@
       <c r="Y33" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="AA33" s="7" t="s">
+      <c r="AC33" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="AC33" s="7">
+      <c r="AG33" s="7">
         <v>1913</v>
       </c>
-      <c r="AD33" s="7" t="s">
+      <c r="AH33" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C34" s="7" t="s">
         <v>397</v>
       </c>
@@ -6628,17 +6667,17 @@
       <c r="Y34" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="AA34" s="7" t="s">
+      <c r="AC34" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="AC34" s="7">
+      <c r="AG34" s="7">
         <v>1913</v>
       </c>
-      <c r="AD34" s="7" t="s">
+      <c r="AH34" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C35" s="7" t="s">
         <v>398</v>
       </c>
@@ -6666,17 +6705,17 @@
       <c r="Y35" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="AA35" s="7" t="s">
+      <c r="AC35" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="AC35" s="7">
+      <c r="AG35" s="7">
         <v>1913</v>
       </c>
-      <c r="AD35" s="7" t="s">
+      <c r="AH35" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="3:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:34" ht="102" x14ac:dyDescent="0.2">
       <c r="C36" s="7" t="s">
         <v>406</v>
       </c>
@@ -6716,17 +6755,17 @@
       <c r="Y36" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="AA36" s="7" t="s">
+      <c r="AC36" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="AC36" s="7">
+      <c r="AG36" s="7">
         <v>1913</v>
       </c>
-      <c r="AD36" s="7" t="s">
+      <c r="AH36" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="37" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C37" s="7" t="s">
         <v>395</v>
       </c>
@@ -6754,17 +6793,17 @@
       <c r="Y37" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="AA37" s="7" t="s">
+      <c r="AC37" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="AC37" s="7">
+      <c r="AG37" s="7">
         <v>1908</v>
       </c>
-      <c r="AD37" s="7">
+      <c r="AH37" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="3:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:34" ht="102" x14ac:dyDescent="0.2">
       <c r="C38" s="11" t="s">
         <v>308</v>
       </c>
@@ -6805,7 +6844,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="39" spans="3:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:34" ht="136" x14ac:dyDescent="0.2">
       <c r="C39" s="7" t="s">
         <v>472</v>
       </c>
@@ -6846,7 +6885,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="40" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C40" s="7" t="s">
         <v>496</v>
       </c>
@@ -6874,17 +6913,17 @@
       <c r="Y40" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="AA40" s="7" t="s">
+      <c r="AC40" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="AC40" s="7">
+      <c r="AG40" s="7">
         <v>1917</v>
       </c>
-      <c r="AD40" s="7" t="s">
+      <c r="AH40" s="7" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="41" spans="3:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:34" ht="85" x14ac:dyDescent="0.2">
       <c r="C41" s="7" t="s">
         <v>510</v>
       </c>
@@ -6919,17 +6958,17 @@
       <c r="Z41" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AA41" s="7" t="s">
+      <c r="AC41" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="AC41" s="7" t="s">
+      <c r="AG41" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="AD41" s="7" t="s">
+      <c r="AH41" s="7" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="42" spans="3:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:34" ht="85" x14ac:dyDescent="0.2">
       <c r="C42" s="7" t="s">
         <v>502</v>
       </c>
@@ -6966,17 +7005,17 @@
       <c r="Z42" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AA42" s="7" t="s">
+      <c r="AC42" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="AC42" s="7">
+      <c r="AG42" s="7">
         <v>1899</v>
       </c>
-      <c r="AD42" s="7" t="s">
+      <c r="AH42" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="3:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:34" ht="102" x14ac:dyDescent="0.2">
       <c r="C43" s="7" t="s">
         <v>505</v>
       </c>
@@ -7013,17 +7052,17 @@
       <c r="Z43" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA43" s="7" t="s">
+      <c r="AC43" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="AC43" s="7">
+      <c r="AG43" s="7">
         <v>1902</v>
       </c>
-      <c r="AD43" s="7" t="s">
+      <c r="AH43" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="3:30" ht="187" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:34" ht="187" x14ac:dyDescent="0.2">
       <c r="C44" s="7" t="s">
         <v>574</v>
       </c>
@@ -7064,7 +7103,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="45" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C45" s="7" t="s">
         <v>573</v>
       </c>
@@ -7102,7 +7141,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="46" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C46" s="7" t="s">
         <v>575</v>
       </c>
@@ -7140,7 +7179,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="47" spans="3:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C47" s="7" t="s">
         <v>616</v>
       </c>
@@ -7181,7 +7220,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="48" spans="3:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:34" ht="51" x14ac:dyDescent="0.2">
       <c r="C48" s="7" t="s">
         <v>632</v>
       </c>
@@ -7219,7 +7258,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C49" s="7" t="s">
         <v>633</v>
       </c>
@@ -7257,7 +7296,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C50" s="7" t="s">
         <v>646</v>
       </c>
@@ -7295,7 +7334,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="51" spans="1:30" ht="153" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" ht="153" x14ac:dyDescent="0.2">
       <c r="C51" s="7" t="s">
         <v>695</v>
       </c>
@@ -7344,17 +7383,17 @@
       <c r="Y51" s="7" t="s">
         <v>693</v>
       </c>
-      <c r="AA51" s="7" t="s">
+      <c r="AC51" s="7" t="s">
         <v>694</v>
       </c>
-      <c r="AC51" s="7">
+      <c r="AG51" s="7">
         <v>1913</v>
       </c>
-      <c r="AD51" s="7" t="s">
+      <c r="AH51" s="7" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="C52" s="7" t="s">
         <v>696</v>
       </c>
@@ -7392,7 +7431,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>704</v>
       </c>
@@ -7436,7 +7475,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>705</v>
       </c>
@@ -7480,7 +7519,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>711</v>
       </c>
@@ -7524,7 +7563,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="56" spans="1:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>717</v>
       </c>
@@ -7568,7 +7607,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="57" spans="1:30" ht="102" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>724</v>
       </c>
@@ -7618,7 +7657,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="58" spans="1:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>731</v>
       </c>
@@ -7662,7 +7701,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="59" spans="1:30" ht="85" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" ht="85" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>736</v>
       </c>
@@ -7706,7 +7745,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="60" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>744</v>
       </c>
@@ -7750,7 +7789,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="61" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>748</v>
       </c>
@@ -7788,7 +7827,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="62" spans="1:30" ht="119" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" ht="119" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>766</v>
       </c>
@@ -7840,17 +7879,17 @@
       <c r="Y62" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA62" s="7" t="s">
+      <c r="AC62" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="AC62" s="7">
+      <c r="AG62" s="7">
         <v>1906</v>
       </c>
-      <c r="AD62" s="16" t="s">
+      <c r="AH62" s="16" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="63" spans="1:30" ht="119" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" ht="119" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>775</v>
       </c>
@@ -7902,17 +7941,17 @@
       <c r="Y63" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AA63" s="7" t="s">
+      <c r="AC63" s="7" t="s">
         <v>783</v>
       </c>
-      <c r="AC63" s="7">
+      <c r="AG63" s="7">
         <v>1910</v>
       </c>
-      <c r="AD63" s="7">
+      <c r="AH63" s="7">
         <v>347</v>
       </c>
     </row>
-    <row r="64" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>785</v>
       </c>
@@ -7956,7 +7995,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="65" spans="1:30" ht="119" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>790</v>
       </c>
@@ -8008,17 +8047,17 @@
       <c r="Y65" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AA65" s="7" t="s">
+      <c r="AC65" s="7" t="s">
         <v>796</v>
       </c>
-      <c r="AC65" s="7">
+      <c r="AG65" s="7">
         <v>1923</v>
       </c>
-      <c r="AD65" s="7">
+      <c r="AH65" s="7">
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>799</v>
       </c>
@@ -8062,7 +8101,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>811</v>
       </c>
@@ -8109,7 +8148,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="68" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>810</v>
       </c>
@@ -8158,14 +8197,14 @@
       <c r="X68" s="7" t="s">
         <v>817</v>
       </c>
-      <c r="AC68" s="7">
+      <c r="AG68" s="7">
         <v>1903</v>
       </c>
-      <c r="AD68" s="7" t="s">
+      <c r="AH68" s="7" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="69" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
         <v>866</v>
       </c>
@@ -8209,7 +8248,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:30" ht="68" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" ht="68" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
         <v>867</v>
       </c>
@@ -8253,7 +8292,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="136" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" ht="136" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
         <v>870</v>
       </c>
@@ -8293,17 +8332,17 @@
       <c r="Y71" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AA71" s="7" t="s">
+      <c r="AC71" s="7" t="s">
         <v>858</v>
       </c>
-      <c r="AC71" s="7">
+      <c r="AG71" s="7">
         <v>1894</v>
       </c>
-      <c r="AD71" s="7">
+      <c r="AH71" s="7">
         <v>66</v>
       </c>
     </row>
-    <row r="72" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
         <v>868</v>
       </c>
@@ -8347,7 +8386,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="73" spans="1:30" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
         <v>869</v>
       </c>
@@ -8391,8 +8430,73 @@
         <v>856</v>
       </c>
     </row>
+    <row r="74" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A74" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>920</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>923</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="L74" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M74" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="V74" s="10" t="s">
+        <v>924</v>
+      </c>
+      <c r="X74" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="Y74" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z74" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA74" s="7" t="s">
+        <v>926</v>
+      </c>
+      <c r="AB74" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="AC74" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="AD74" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="AE74" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="AF74" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="AG74" s="7">
+        <v>1877</v>
+      </c>
+      <c r="AH74" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:AM36">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:AQ36">
     <sortCondition ref="F2:F36"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update mods for new obj
</commit_message>
<xml_diff>
--- a/transcriptions/OMV-MODS-worksheet.xlsx
+++ b/transcriptions/OMV-MODS-worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/onemorevoice/transcriptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF7865E-87AF-A04D-8BE3-A3DB1FD6BC8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BB6929-F6C8-9A48-B3E0-A3B2BD35D35A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="460" windowWidth="24980" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Artifacts" sheetId="1" r:id="rId2"/>
     <sheet name="dev" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1017">
   <si>
     <t>liv_000017</t>
   </si>
@@ -2837,6 +2837,261 @@
   </si>
   <si>
     <t>James Kay</t>
+  </si>
+  <si>
+    <t>liv_021071</t>
+  </si>
+  <si>
+    <t>liv_021072</t>
+  </si>
+  <si>
+    <t>liv_021073</t>
+  </si>
+  <si>
+    <t>liv_021074</t>
+  </si>
+  <si>
+    <t>liv_021075</t>
+  </si>
+  <si>
+    <t>liv_021076</t>
+  </si>
+  <si>
+    <t>liv_021077</t>
+  </si>
+  <si>
+    <t>liv_021078</t>
+  </si>
+  <si>
+    <t>Edith Eaton seated in quarter profile, facing forward and holding a book.</t>
+  </si>
+  <si>
+    <t>Emperor Menelik II on the throne in coronation garb</t>
+  </si>
+  <si>
+    <t>Moshoeshoe seated, holding a cane, and dressed in formal attire including a top hat and overcoat.</t>
+  </si>
+  <si>
+    <t>Moshoeshoe seat and in formal attire, surrounded by five individuals, some seated, some standing.</t>
+  </si>
+  <si>
+    <t>Ranavalona I in quarter profile, standing and dressed in full regnal attire.</t>
+  </si>
+  <si>
+    <t>Tippo Tib seated and surrounded by four individuals, all of whom are standing.</t>
+  </si>
+  <si>
+    <t>Tippo Tip in half-body portrait, standing and facing forward.</t>
+  </si>
+  <si>
+    <t>Tippu Tip and Eugene Wolf seated and facing one another in half profile.</t>
+  </si>
+  <si>
+    <t>Buéna-N'zigué and Tippo-Tip seated side by side and facing forward.</t>
+  </si>
+  <si>
+    <t>liv_021079</t>
+  </si>
+  <si>
+    <t>Image from the private collection of Diana Birchall, great-niece of the author. Creative Commons Attribution-NonCommercial-ShareAlike 4.0 International License (CC BY-NC-SA 4.0)</t>
+  </si>
+  <si>
+    <t>Image courtesy of Michael Graham-Stewart. Published by permission.</t>
+  </si>
+  <si>
+    <t>Public domain, South Africa</t>
+  </si>
+  <si>
+    <t>https://cwrc.ca/islandora/object/cwrc%3A33fa949d-b6d2-474b-b35f-e3d12f2f57ce</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:Emperor_Menelik_II.png</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:King_Moshoeshoe_of_the_Sotho_-_Lesotho_-_from_the_Natal_Archives.jpg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:King_Moshoeshoe_of_the_Basotho_with_his_ministers.jpg</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/File:Ranavalona_I.jpg</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/voicefromcongoco00wardrich/page/62/mode/2up</t>
+  </si>
+  <si>
+    <t>https://collections.rmg.co.uk/collections/objects/261977.html</t>
+  </si>
+  <si>
+    <t>https://archive.org/details/vingtannesdev01delc/page/300/mode/2up</t>
+  </si>
+  <si>
+    <t>http://collections.smvk.se/carlotta-em/web/object/3678987</t>
+  </si>
+  <si>
+    <t>Ramanankirahina, Philippe-Auguste, 1860-1915</t>
+  </si>
+  <si>
+    <t>Ward, Herbert, 1863-1919</t>
+  </si>
+  <si>
+    <t>Dias, E.C., 1845-1883</t>
+  </si>
+  <si>
+    <t>Allgurén, Sven Edvard, 1847-1897</t>
+  </si>
+  <si>
+    <t>Delcommune, Alexandre, 1855-1922</t>
+  </si>
+  <si>
+    <t>oil paintings (visual works)</t>
+  </si>
+  <si>
+    <t>Edith Eaton</t>
+  </si>
+  <si>
+    <t>Emperor Menelik II</t>
+  </si>
+  <si>
+    <t>Ranavalona I</t>
+  </si>
+  <si>
+    <t>Tippo Tib</t>
+  </si>
+  <si>
+    <t>Tippo Tip</t>
+  </si>
+  <si>
+    <t>Tippu Tip and Eugene Wolf</t>
+  </si>
+  <si>
+    <t>Ethiopia Photographed: Historic Photographs of the Country and its People Taken Between 1867 and 1935</t>
+  </si>
+  <si>
+    <t>A Voice from the Congo, Comprising Stories, Anecdotes, and Descriptive Notes</t>
+  </si>
+  <si>
+    <t>Vingt Années de Vie Africaine: Récits de Voyages, d'Aventures et d'Exploration au Congo Belge, 1874-1893</t>
+  </si>
+  <si>
+    <t>[late nineteenth/early twentieth century]</t>
+  </si>
+  <si>
+    <t>[nineteenth century]</t>
+  </si>
+  <si>
+    <t>facing 62</t>
+  </si>
+  <si>
+    <t>facing 300</t>
+  </si>
+  <si>
+    <t>Prankhurst, Richard</t>
+  </si>
+  <si>
+    <t>Kegan Paul International</t>
+  </si>
+  <si>
+    <t>William Heinemann</t>
+  </si>
+  <si>
+    <t>Vve Ferdinand Larcier</t>
+  </si>
+  <si>
+    <t>Zanzibar</t>
+  </si>
+  <si>
+    <t>Bruxelles</t>
+  </si>
+  <si>
+    <t>Royal Museums Greenwich</t>
+  </si>
+  <si>
+    <t>cwrc:33fa949d-b6d2-474b-b35f-e3d12f2f57ce</t>
+  </si>
+  <si>
+    <t>Special Collections, Historical Photographs, Michael Graham-Stewart Collection, ZBA2600</t>
+  </si>
+  <si>
+    <t>1922; 1889</t>
+  </si>
+  <si>
+    <t>The Canadian Writing Research Collaboratory (CWRC) / Le Collaboratoire Scientifique des Écrits du Canada (CSÉC)</t>
+  </si>
+  <si>
+    <t>c.1890</t>
+  </si>
+  <si>
+    <t>Edith Eaton, [late nineteenth/early twentieth century]</t>
+  </si>
+  <si>
+    <t>Ranavalona I, 1905</t>
+  </si>
+  <si>
+    <t>Tippo Tip, c.1890</t>
+  </si>
+  <si>
+    <t>Tippu Tip and Eugene Wolf, 1894</t>
+  </si>
+  <si>
+    <t>Tippo Tib, [late nineteenth/early twentieth century]</t>
+  </si>
+  <si>
+    <t>Emperor Menelik II, [late nineteenth/early twentieth century]</t>
+  </si>
+  <si>
+    <t>“King Moshoeshoe or Moshesh of the Basotho People of Lesotho”</t>
+  </si>
+  <si>
+    <t>“King Moshoeshoe or Moshesh of the Basotho People of Lesotho”, [nineteenth century]</t>
+  </si>
+  <si>
+    <t>“King Moshoeshoe of the Basotho with His Ministers,” [nineteenth century]</t>
+  </si>
+  <si>
+    <t>“King Moshoeshoe of the Basotho with His Ministers”</t>
+  </si>
+  <si>
+    <t>“Tippo-Tip and et son Copain Buéna-N'zigué”</t>
+  </si>
+  <si>
+    <t>“Tippo-Tip and et son Copain Buéna-N'zigué,” 1889</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Pietermaritzburg Archives Repository</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Pietermaritzburg</t>
+  </si>
+  <si>
+    <t>Bensusan Museum of Photography</t>
+  </si>
+  <si>
+    <t>Johannesburg</t>
+  </si>
+  <si>
+    <t>Antananarivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andafiavaratra Palace </t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Etnografiska Museet</t>
+  </si>
+  <si>
+    <t>Stockholm</t>
+  </si>
+  <si>
+    <t>Sweeden</t>
   </si>
 </sst>
 </file>
@@ -2945,7 +3200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2993,6 +3248,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5260,11 +5518,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ74"/>
+  <dimension ref="A1:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS74" sqref="AS74"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U77" sqref="U77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5371,10 +5629,22 @@
       <c r="Z1" s="6" t="s">
         <v>196</v>
       </c>
+      <c r="AA1" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB1" s="6" t="s">
+        <v>196</v>
+      </c>
       <c r="AC1" s="6" t="s">
         <v>197</v>
       </c>
       <c r="AD1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>197</v>
       </c>
       <c r="AG1" s="6" t="s">
@@ -8493,6 +8763,428 @@
       </c>
       <c r="AH74" s="7" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
+        <v>953</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>950</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>940</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O75" s="7" t="s">
+        <v>1005</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="S75" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="T75" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="X75" s="17"/>
+      <c r="AB75" s="1"/>
+      <c r="AH75" s="1"/>
+    </row>
+    <row r="76" spans="1:34" ht="136" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>954</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>941</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>933</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="I76" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L76" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M76" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="V76" s="10" t="s">
+        <v>981</v>
+      </c>
+      <c r="X76" s="17" t="s">
+        <v>974</v>
+      </c>
+      <c r="Y76" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z76" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="AB76" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="AG76" s="1">
+        <v>1996</v>
+      </c>
+      <c r="AH76" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>955</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>952</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>942</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I77" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L77" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="O77" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P77" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="R77" s="1"/>
+      <c r="S77" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="T77" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="X77" s="17"/>
+      <c r="AB77" s="1"/>
+      <c r="AH77" s="1"/>
+    </row>
+    <row r="78" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
+        <v>956</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>943</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I78" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="L78" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O78" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P78" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R78" s="1"/>
+      <c r="S78" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="T78" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="X78" s="17"/>
+      <c r="AB78" s="1"/>
+      <c r="AH78" s="1"/>
+    </row>
+    <row r="79" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A79" s="17" t="s">
+        <v>957</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>944</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="I79" s="17" t="s">
+        <v>962</v>
+      </c>
+      <c r="L79" s="17" t="s">
+        <v>967</v>
+      </c>
+      <c r="O79" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="P79" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="R79" s="1"/>
+      <c r="S79" s="1">
+        <v>1905</v>
+      </c>
+      <c r="T79" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="X79" s="17"/>
+      <c r="AB79" s="1"/>
+      <c r="AH79" s="1"/>
+    </row>
+    <row r="80" spans="1:34" ht="102" x14ac:dyDescent="0.2">
+      <c r="A80" s="17" t="s">
+        <v>958</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>945</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>963</v>
+      </c>
+      <c r="L80" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M80" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="V80" s="17" t="s">
+        <v>963</v>
+      </c>
+      <c r="X80" s="17" t="s">
+        <v>975</v>
+      </c>
+      <c r="Y80" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB80" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="AG80" s="1">
+        <v>1910</v>
+      </c>
+      <c r="AH80" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="81" spans="1:34" ht="68" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
+        <v>959</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>951</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>946</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="I81" s="17" t="s">
+        <v>964</v>
+      </c>
+      <c r="L81" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O81" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="P81" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="S81" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="T81" s="17" t="s">
+        <v>703</v>
+      </c>
+      <c r="X81" s="17"/>
+      <c r="AB81" s="1"/>
+      <c r="AH81" s="1"/>
+    </row>
+    <row r="82" spans="1:34" ht="51" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>961</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>947</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>939</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>965</v>
+      </c>
+      <c r="L82" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="O82" s="7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="P82" s="7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="R82" s="1">
+        <v>909.01310000000001</v>
+      </c>
+      <c r="S82" s="1">
+        <v>1894</v>
+      </c>
+      <c r="T82" s="17" t="s">
+        <v>985</v>
+      </c>
+      <c r="X82" s="17"/>
+      <c r="AB82" s="1"/>
+      <c r="AH82" s="1"/>
+    </row>
+    <row r="83" spans="1:34" ht="136" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
+        <v>960</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>706</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>948</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I83" s="17" t="s">
+        <v>966</v>
+      </c>
+      <c r="L83" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M83" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q83" s="1"/>
+      <c r="V83" s="17" t="s">
+        <v>966</v>
+      </c>
+      <c r="X83" s="17" t="s">
+        <v>976</v>
+      </c>
+      <c r="Y83" s="17" t="s">
+        <v>986</v>
+      </c>
+      <c r="AB83" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="AG83" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="AH83" s="1" t="s">
+        <v>980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>